<commit_message>
Generalized the queries for injecting real data.
</commit_message>
<xml_diff>
--- a/b11_1/fields/insert.xlsx
+++ b/b11_1/fields/insert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yann/Prog/Python/LBA/b11_1/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394BC1F0-033B-6944-A6CC-4BFF8E99967E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9B6C1A-608E-9243-B3F1-05048CA58938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1420" yWindow="5000" windowWidth="46780" windowHeight="18000" activeTab="1" xr2:uid="{41FF1C03-8D98-44C8-8EDC-6562CA448D86}"/>
   </bookViews>
@@ -1258,7 +1258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1F6E88-797B-42CA-9EC0-C2555AB4031B}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="H23" sqref="H23:K23"/>
     </sheetView>
   </sheetViews>
@@ -3645,7 +3645,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB86915-FE40-8640-8F00-428279462302}">
-  <dimension ref="A1:D161"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
@@ -5090,7 +5090,7 @@
         <v>auspraegung_id</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>267</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" t="str">
         <f>_xlfn.CONCAT("'", Sheet1!H2, "',")</f>
         <v>'t',</v>
@@ -5122,7 +5122,7 @@
         <v>'t',</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" t="str">
         <f>_xlfn.CONCAT(Sheet1!H3, ",")</f>
         <v>1,</v>
@@ -5140,7 +5140,7 @@
         <v>4,</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" t="str">
         <f>_xlfn.CONCAT("'", Sheet1!H4, "',")</f>
         <v>'Kurztext DE XYZ',</v>
@@ -5158,7 +5158,7 @@
         <v>'asdfasdfasdfasdf',</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" t="str">
         <f>_xlfn.CONCAT("'", Sheet1!H5, "',")</f>
         <v>'Kurztext FR',</v>
@@ -5176,7 +5176,7 @@
         <v>'1tqgqdbq',</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86" t="str">
         <f>_xlfn.CONCAT("'", Sheet1!H6, "',")</f>
         <v>'Kurztext EN',</v>
@@ -5194,7 +5194,7 @@
         <v>'asahasr5t',</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87" t="str">
         <f>_xlfn.CONCAT("'", Sheet1!H7, "',")</f>
         <v>'Grunddatentext DE - 1. Zeile',</v>
@@ -5212,7 +5212,7 @@
         <v>'Grunddatentext DE - 1. Zeile 4',</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88" t="str">
         <f>_xlfn.CONCAT("'", Sheet1!H8, "',")</f>
         <v>'Grunddatentext DE - 2. Zeile',</v>
@@ -5230,7 +5230,7 @@
         <v>'Grunddatentext DE - 2. Zeile 4',</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89" t="str">
         <f>_xlfn.CONCAT("'", Sheet1!H9, "',")</f>
         <v>'Grunddatentext FR - 1. Zeile',</v>
@@ -5248,7 +5248,7 @@
         <v>'Grunddatentext FR - 1. Zeile 4',</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90" t="str">
         <f>_xlfn.CONCAT("'", Sheet1!H10, "',")</f>
         <v>'Grunddatentext FR - 2. Zeile',</v>
@@ -5266,7 +5266,7 @@
         <v>'Grunddatentext FR - 2. Zeile 4',</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91" t="str">
         <f>_xlfn.CONCAT("'", Sheet1!H11, "',")</f>
         <v>'Grunddatentext EN - 1. Zeile',</v>
@@ -5284,7 +5284,7 @@
         <v>'Grunddatentext EN - 1. Zeile 4',</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92" t="str">
         <f>_xlfn.CONCAT("'", Sheet1!H12, "',")</f>
         <v>'Grunddatentext EN - 2. Zeile',</v>
@@ -5302,1228 +5302,1500 @@
         <v>'Grunddatentext EN - 2. Zeile 4',</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H13, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H13), Sheet1!H13, IF(Sheet1!H13="Null", "Null", _xlfn.CONCAT("'", Sheet1!H13, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="B93" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I13, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I13), Sheet1!I13, IF(Sheet1!I13="Null", "Null", _xlfn.CONCAT("'", Sheet1!I13, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="C93" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J13, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J13), Sheet1!J13, IF(Sheet1!J13="Null", "Null", _xlfn.CONCAT("'", Sheet1!J13, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="D93" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K13, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K13), Sheet1!K13, IF(Sheet1!K13="Null", "Null", _xlfn.CONCAT("'", Sheet1!K13, "'"))), ",")</f>
         <v>4,</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F93">
+        <f>IF(ISNUMBER(Sheet1!H13), Sheet1!H13, IF(Sheet1!H13="Null", "Null", _xlfn.CONCAT("'", Sheet1!H13, "'")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H14, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H14), Sheet1!H14, IF(Sheet1!H14="Null", "Null", _xlfn.CONCAT("'", Sheet1!H14, "'"))), ",")</f>
         <v>12,</v>
       </c>
       <c r="B94" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I14, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I14), Sheet1!I14, IF(Sheet1!I14="Null", "Null", _xlfn.CONCAT("'", Sheet1!I14, "'"))), ",")</f>
         <v>22,</v>
       </c>
       <c r="C94" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J14, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J14), Sheet1!J14, IF(Sheet1!J14="Null", "Null", _xlfn.CONCAT("'", Sheet1!J14, "'"))), ",")</f>
         <v>32,</v>
       </c>
       <c r="D94" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K14, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K14), Sheet1!K14, IF(Sheet1!K14="Null", "Null", _xlfn.CONCAT("'", Sheet1!K14, "'"))), ",")</f>
         <v>42,</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F94">
+        <f>IF(ISNUMBER(Sheet1!H14), Sheet1!H14, IF(Sheet1!H14="Null", "Null", _xlfn.CONCAT("'", Sheet1!H14, "'")))</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A95" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H15, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H15), Sheet1!H15, IF(Sheet1!H15="Null", "Null", _xlfn.CONCAT("'", Sheet1!H15, "'"))), ",")</f>
         <v>23,</v>
       </c>
       <c r="B95" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I15, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I15), Sheet1!I15, IF(Sheet1!I15="Null", "Null", _xlfn.CONCAT("'", Sheet1!I15, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C95" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J15, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J15), Sheet1!J15, IF(Sheet1!J15="Null", "Null", _xlfn.CONCAT("'", Sheet1!J15, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D95" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K15, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K15), Sheet1!K15, IF(Sheet1!K15="Null", "Null", _xlfn.CONCAT("'", Sheet1!K15, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F95">
+        <f>IF(ISNUMBER(Sheet1!H15), Sheet1!H15, IF(Sheet1!H15="Null", "Null", _xlfn.CONCAT("'", Sheet1!H15, "'")))</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A96" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H16, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H16), Sheet1!H16, IF(Sheet1!H16="Null", "Null", _xlfn.CONCAT("'", Sheet1!H16, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="B96" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I16, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I16), Sheet1!I16, IF(Sheet1!I16="Null", "Null", _xlfn.CONCAT("'", Sheet1!I16, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C96" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J16, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J16), Sheet1!J16, IF(Sheet1!J16="Null", "Null", _xlfn.CONCAT("'", Sheet1!J16, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D96" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K16, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K16), Sheet1!K16, IF(Sheet1!K16="Null", "Null", _xlfn.CONCAT("'", Sheet1!K16, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F96" t="str">
+        <f>IF(ISNUMBER(Sheet1!H16), Sheet1!H16, IF(Sheet1!H16="Null", "Null", _xlfn.CONCAT("'", Sheet1!H16, "'")))</f>
+        <v>Null</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A97" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H17, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H17), Sheet1!H17, IF(Sheet1!H17="Null", "Null", _xlfn.CONCAT("'", Sheet1!H17, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="B97" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I17, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I17), Sheet1!I17, IF(Sheet1!I17="Null", "Null", _xlfn.CONCAT("'", Sheet1!I17, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C97" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J17, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J17), Sheet1!J17, IF(Sheet1!J17="Null", "Null", _xlfn.CONCAT("'", Sheet1!J17, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D97" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K17, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K17), Sheet1!K17, IF(Sheet1!K17="Null", "Null", _xlfn.CONCAT("'", Sheet1!K17, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F97" t="str">
+        <f>IF(ISNUMBER(Sheet1!H17), Sheet1!H17, IF(Sheet1!H17="Null", "Null", _xlfn.CONCAT("'", Sheet1!H17, "'")))</f>
+        <v>Null</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A98" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H18, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H18), Sheet1!H18, IF(Sheet1!H18="Null", "Null", _xlfn.CONCAT("'", Sheet1!H18, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="B98" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I18, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I18), Sheet1!I18, IF(Sheet1!I18="Null", "Null", _xlfn.CONCAT("'", Sheet1!I18, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C98" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J18, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J18), Sheet1!J18, IF(Sheet1!J18="Null", "Null", _xlfn.CONCAT("'", Sheet1!J18, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D98" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K18, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K18), Sheet1!K18, IF(Sheet1!K18="Null", "Null", _xlfn.CONCAT("'", Sheet1!K18, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F98" t="str">
+        <f>IF(ISNUMBER(Sheet1!H18), Sheet1!H18, IF(Sheet1!H18="Null", "Null", _xlfn.CONCAT("'", Sheet1!H18, "'")))</f>
+        <v>Null</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H19, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H19), Sheet1!H19, IF(Sheet1!H19="Null", "Null", _xlfn.CONCAT("'", Sheet1!H19, "'"))), ",")</f>
         <v>'yann011111111111111',</v>
       </c>
       <c r="B99" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I19, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I19), Sheet1!I19, IF(Sheet1!I19="Null", "Null", _xlfn.CONCAT("'", Sheet1!I19, "'"))), ",")</f>
         <v>'yann022222222222222',</v>
       </c>
       <c r="C99" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J19, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J19), Sheet1!J19, IF(Sheet1!J19="Null", "Null", _xlfn.CONCAT("'", Sheet1!J19, "'"))), ",")</f>
         <v>'yann033333333333333',</v>
       </c>
       <c r="D99" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K19, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K19), Sheet1!K19, IF(Sheet1!K19="Null", "Null", _xlfn.CONCAT("'", Sheet1!K19, "'"))), ",")</f>
         <v>'yann044444444444444',</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F99" t="str">
+        <f>IF(ISNUMBER(Sheet1!H19), Sheet1!H19, IF(Sheet1!H19="Null", "Null", _xlfn.CONCAT("'", Sheet1!H19, "'")))</f>
+        <v>'yann011111111111111'</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A100" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H20, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H20), Sheet1!H20, IF(Sheet1!H20="Null", "Null", _xlfn.CONCAT("'", Sheet1!H20, "'"))), ",")</f>
         <v>'aa',</v>
       </c>
       <c r="B100" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I20, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I20), Sheet1!I20, IF(Sheet1!I20="Null", "Null", _xlfn.CONCAT("'", Sheet1!I20, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C100" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J20, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J20), Sheet1!J20, IF(Sheet1!J20="Null", "Null", _xlfn.CONCAT("'", Sheet1!J20, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D100" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K20, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K20), Sheet1!K20, IF(Sheet1!K20="Null", "Null", _xlfn.CONCAT("'", Sheet1!K20, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F100" t="str">
+        <f>IF(ISNUMBER(Sheet1!H20), Sheet1!H20, IF(Sheet1!H20="Null", "Null", _xlfn.CONCAT("'", Sheet1!H20, "'")))</f>
+        <v>'aa'</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A101" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H21, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H21), Sheet1!H21, IF(Sheet1!H21="Null", "Null", _xlfn.CONCAT("'", Sheet1!H21, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="B101" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I21, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I21), Sheet1!I21, IF(Sheet1!I21="Null", "Null", _xlfn.CONCAT("'", Sheet1!I21, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="C101" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J21, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J21), Sheet1!J21, IF(Sheet1!J21="Null", "Null", _xlfn.CONCAT("'", Sheet1!J21, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="D101" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K21, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K21), Sheet1!K21, IF(Sheet1!K21="Null", "Null", _xlfn.CONCAT("'", Sheet1!K21, "'"))), ",")</f>
         <v>2,</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F101">
+        <f>IF(ISNUMBER(Sheet1!H21), Sheet1!H21, IF(Sheet1!H21="Null", "Null", _xlfn.CONCAT("'", Sheet1!H21, "'")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A102" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H22, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H22), Sheet1!H22, IF(Sheet1!H22="Null", "Null", _xlfn.CONCAT("'", Sheet1!H22, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="B102" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I22, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I22), Sheet1!I22, IF(Sheet1!I22="Null", "Null", _xlfn.CONCAT("'", Sheet1!I22, "'"))), ",")</f>
         <v>'f',</v>
       </c>
       <c r="C102" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J22, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J22), Sheet1!J22, IF(Sheet1!J22="Null", "Null", _xlfn.CONCAT("'", Sheet1!J22, "'"))), ",")</f>
         <v>'f',</v>
       </c>
       <c r="D102" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K22, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K22), Sheet1!K22, IF(Sheet1!K22="Null", "Null", _xlfn.CONCAT("'", Sheet1!K22, "'"))), ",")</f>
         <v>'f',</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F102" t="str">
+        <f>IF(ISNUMBER(Sheet1!H22), Sheet1!H22, IF(Sheet1!H22="Null", "Null", _xlfn.CONCAT("'", Sheet1!H22, "'")))</f>
+        <v>'t'</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A103" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H23, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H23), Sheet1!H23, IF(Sheet1!H23="Null", "Null", _xlfn.CONCAT("'", Sheet1!H23, "'"))), ",")</f>
         <v>'f',</v>
       </c>
       <c r="B103" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I23, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I23), Sheet1!I23, IF(Sheet1!I23="Null", "Null", _xlfn.CONCAT("'", Sheet1!I23, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="C103" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J23, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J23), Sheet1!J23, IF(Sheet1!J23="Null", "Null", _xlfn.CONCAT("'", Sheet1!J23, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="D103" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K23, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K23), Sheet1!K23, IF(Sheet1!K23="Null", "Null", _xlfn.CONCAT("'", Sheet1!K23, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F103" t="str">
+        <f>IF(ISNUMBER(Sheet1!H23), Sheet1!H23, IF(Sheet1!H23="Null", "Null", _xlfn.CONCAT("'", Sheet1!H23, "'")))</f>
+        <v>'f'</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A104" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H24, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H24), Sheet1!H24, IF(Sheet1!H24="Null", "Null", _xlfn.CONCAT("'", Sheet1!H24, "'"))), ",")</f>
         <v>10,</v>
       </c>
       <c r="B104" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I24, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I24), Sheet1!I24, IF(Sheet1!I24="Null", "Null", _xlfn.CONCAT("'", Sheet1!I24, "'"))), ",")</f>
         <v>10,</v>
       </c>
       <c r="C104" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J24, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J24), Sheet1!J24, IF(Sheet1!J24="Null", "Null", _xlfn.CONCAT("'", Sheet1!J24, "'"))), ",")</f>
         <v>10,</v>
       </c>
       <c r="D104" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K24, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K24), Sheet1!K24, IF(Sheet1!K24="Null", "Null", _xlfn.CONCAT("'", Sheet1!K24, "'"))), ",")</f>
         <v>10,</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F104">
+        <f>IF(ISNUMBER(Sheet1!H24), Sheet1!H24, IF(Sheet1!H24="Null", "Null", _xlfn.CONCAT("'", Sheet1!H24, "'")))</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A105" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H25, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H25), Sheet1!H25, IF(Sheet1!H25="Null", "Null", _xlfn.CONCAT("'", Sheet1!H25, "'"))), ",")</f>
         <v>11,</v>
       </c>
       <c r="B105" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I25, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I25), Sheet1!I25, IF(Sheet1!I25="Null", "Null", _xlfn.CONCAT("'", Sheet1!I25, "'"))), ",")</f>
         <v>22,</v>
       </c>
       <c r="C105" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J25, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J25), Sheet1!J25, IF(Sheet1!J25="Null", "Null", _xlfn.CONCAT("'", Sheet1!J25, "'"))), ",")</f>
         <v>33,</v>
       </c>
       <c r="D105" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K25, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K25), Sheet1!K25, IF(Sheet1!K25="Null", "Null", _xlfn.CONCAT("'", Sheet1!K25, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F105">
+        <f>IF(ISNUMBER(Sheet1!H25), Sheet1!H25, IF(Sheet1!H25="Null", "Null", _xlfn.CONCAT("'", Sheet1!H25, "'")))</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A106" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H26, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H26), Sheet1!H26, IF(Sheet1!H26="Null", "Null", _xlfn.CONCAT("'", Sheet1!H26, "'"))), ",")</f>
         <v>111,</v>
       </c>
       <c r="B106" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I26, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I26), Sheet1!I26, IF(Sheet1!I26="Null", "Null", _xlfn.CONCAT("'", Sheet1!I26, "'"))), ",")</f>
         <v>222,</v>
       </c>
       <c r="C106" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J26, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J26), Sheet1!J26, IF(Sheet1!J26="Null", "Null", _xlfn.CONCAT("'", Sheet1!J26, "'"))), ",")</f>
         <v>333,</v>
       </c>
       <c r="D106" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K26, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K26), Sheet1!K26, IF(Sheet1!K26="Null", "Null", _xlfn.CONCAT("'", Sheet1!K26, "'"))), ",")</f>
         <v>444,</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F106">
+        <f>IF(ISNUMBER(Sheet1!H26), Sheet1!H26, IF(Sheet1!H26="Null", "Null", _xlfn.CONCAT("'", Sheet1!H26, "'")))</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A107" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H27, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H27), Sheet1!H27, IF(Sheet1!H27="Null", "Null", _xlfn.CONCAT("'", Sheet1!H27, "'"))), ",")</f>
         <v>55,</v>
       </c>
       <c r="B107" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I27, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I27), Sheet1!I27, IF(Sheet1!I27="Null", "Null", _xlfn.CONCAT("'", Sheet1!I27, "'"))), ",")</f>
         <v>66,</v>
       </c>
       <c r="C107" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J27, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J27), Sheet1!J27, IF(Sheet1!J27="Null", "Null", _xlfn.CONCAT("'", Sheet1!J27, "'"))), ",")</f>
         <v>77,</v>
       </c>
       <c r="D107" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K27, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K27), Sheet1!K27, IF(Sheet1!K27="Null", "Null", _xlfn.CONCAT("'", Sheet1!K27, "'"))), ",")</f>
         <v>88,</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F107">
+        <f>IF(ISNUMBER(Sheet1!H27), Sheet1!H27, IF(Sheet1!H27="Null", "Null", _xlfn.CONCAT("'", Sheet1!H27, "'")))</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A108" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H28, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H28), Sheet1!H28, IF(Sheet1!H28="Null", "Null", _xlfn.CONCAT("'", Sheet1!H28, "'"))), ",")</f>
         <v>44,</v>
       </c>
       <c r="B108" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I28, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I28), Sheet1!I28, IF(Sheet1!I28="Null", "Null", _xlfn.CONCAT("'", Sheet1!I28, "'"))), ",")</f>
         <v>987,</v>
       </c>
       <c r="C108" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J28, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J28), Sheet1!J28, IF(Sheet1!J28="Null", "Null", _xlfn.CONCAT("'", Sheet1!J28, "'"))), ",")</f>
         <v>12,</v>
       </c>
       <c r="D108" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K28, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K28), Sheet1!K28, IF(Sheet1!K28="Null", "Null", _xlfn.CONCAT("'", Sheet1!K28, "'"))), ",")</f>
         <v>15,</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F108">
+        <f>IF(ISNUMBER(Sheet1!H28), Sheet1!H28, IF(Sheet1!H28="Null", "Null", _xlfn.CONCAT("'", Sheet1!H28, "'")))</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A109" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H29, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H29), Sheet1!H29, IF(Sheet1!H29="Null", "Null", _xlfn.CONCAT("'", Sheet1!H29, "'"))), ",")</f>
         <v>33,</v>
       </c>
       <c r="B109" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I29, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I29), Sheet1!I29, IF(Sheet1!I29="Null", "Null", _xlfn.CONCAT("'", Sheet1!I29, "'"))), ",")</f>
         <v>232,</v>
       </c>
       <c r="C109" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J29, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J29), Sheet1!J29, IF(Sheet1!J29="Null", "Null", _xlfn.CONCAT("'", Sheet1!J29, "'"))), ",")</f>
         <v>253,</v>
       </c>
       <c r="D109" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K29, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K29), Sheet1!K29, IF(Sheet1!K29="Null", "Null", _xlfn.CONCAT("'", Sheet1!K29, "'"))), ",")</f>
         <v>75,</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F109">
+        <f>IF(ISNUMBER(Sheet1!H29), Sheet1!H29, IF(Sheet1!H29="Null", "Null", _xlfn.CONCAT("'", Sheet1!H29, "'")))</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A110" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H30, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H30), Sheet1!H30, IF(Sheet1!H30="Null", "Null", _xlfn.CONCAT("'", Sheet1!H30, "'"))), ",")</f>
         <v>22,</v>
       </c>
       <c r="B110" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I30, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I30), Sheet1!I30, IF(Sheet1!I30="Null", "Null", _xlfn.CONCAT("'", Sheet1!I30, "'"))), ",")</f>
         <v>253,</v>
       </c>
       <c r="C110" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J30, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J30), Sheet1!J30, IF(Sheet1!J30="Null", "Null", _xlfn.CONCAT("'", Sheet1!J30, "'"))), ",")</f>
         <v>1000,</v>
       </c>
       <c r="D110" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K30, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K30), Sheet1!K30, IF(Sheet1!K30="Null", "Null", _xlfn.CONCAT("'", Sheet1!K30, "'"))), ",")</f>
         <v>65,</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F110">
+        <f>IF(ISNUMBER(Sheet1!H30), Sheet1!H30, IF(Sheet1!H30="Null", "Null", _xlfn.CONCAT("'", Sheet1!H30, "'")))</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A111" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H31, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H31), Sheet1!H31, IF(Sheet1!H31="Null", "Null", _xlfn.CONCAT("'", Sheet1!H31, "'"))), ",")</f>
         <v>50,</v>
       </c>
       <c r="B111" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I31, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I31), Sheet1!I31, IF(Sheet1!I31="Null", "Null", _xlfn.CONCAT("'", Sheet1!I31, "'"))), ",")</f>
         <v>23,</v>
       </c>
       <c r="C111" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J31, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J31), Sheet1!J31, IF(Sheet1!J31="Null", "Null", _xlfn.CONCAT("'", Sheet1!J31, "'"))), ",")</f>
         <v>465,</v>
       </c>
       <c r="D111" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K31, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K31), Sheet1!K31, IF(Sheet1!K31="Null", "Null", _xlfn.CONCAT("'", Sheet1!K31, "'"))), ",")</f>
         <v>50,</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F111">
+        <f>IF(ISNUMBER(Sheet1!H31), Sheet1!H31, IF(Sheet1!H31="Null", "Null", _xlfn.CONCAT("'", Sheet1!H31, "'")))</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A112" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H32, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H32), Sheet1!H32, IF(Sheet1!H32="Null", "Null", _xlfn.CONCAT("'", Sheet1!H32, "'"))), ",")</f>
         <v>100,</v>
       </c>
       <c r="B112" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I32, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I32), Sheet1!I32, IF(Sheet1!I32="Null", "Null", _xlfn.CONCAT("'", Sheet1!I32, "'"))), ",")</f>
         <v>55,</v>
       </c>
       <c r="C112" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J32, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J32), Sheet1!J32, IF(Sheet1!J32="Null", "Null", _xlfn.CONCAT("'", Sheet1!J32, "'"))), ",")</f>
         <v>313,</v>
       </c>
       <c r="D112" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K32, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K32), Sheet1!K32, IF(Sheet1!K32="Null", "Null", _xlfn.CONCAT("'", Sheet1!K32, "'"))), ",")</f>
         <v>987,</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F112">
+        <f>IF(ISNUMBER(Sheet1!H32), Sheet1!H32, IF(Sheet1!H32="Null", "Null", _xlfn.CONCAT("'", Sheet1!H32, "'")))</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A113" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H33, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H33), Sheet1!H33, IF(Sheet1!H33="Null", "Null", _xlfn.CONCAT("'", Sheet1!H33, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="B113" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I33, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I33), Sheet1!I33, IF(Sheet1!I33="Null", "Null", _xlfn.CONCAT("'", Sheet1!I33, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C113" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J33, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J33), Sheet1!J33, IF(Sheet1!J33="Null", "Null", _xlfn.CONCAT("'", Sheet1!J33, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D113" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K33, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K33), Sheet1!K33, IF(Sheet1!K33="Null", "Null", _xlfn.CONCAT("'", Sheet1!K33, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F113" t="str">
+        <f>IF(ISNUMBER(Sheet1!H33), Sheet1!H33, IF(Sheet1!H33="Null", "Null", _xlfn.CONCAT("'", Sheet1!H33, "'")))</f>
+        <v>'t'</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A114" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H34, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H34), Sheet1!H34, IF(Sheet1!H34="Null", "Null", _xlfn.CONCAT("'", Sheet1!H34, "'"))), ",")</f>
         <v>'D9182',</v>
       </c>
       <c r="B114" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I34, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I34), Sheet1!I34, IF(Sheet1!I34="Null", "Null", _xlfn.CONCAT("'", Sheet1!I34, "'"))), ",")</f>
         <v>'KCX07',</v>
       </c>
       <c r="C114" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J34, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J34), Sheet1!J34, IF(Sheet1!J34="Null", "Null", _xlfn.CONCAT("'", Sheet1!J34, "'"))), ",")</f>
         <v>'DD901',</v>
       </c>
       <c r="D114" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K34, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K34), Sheet1!K34, IF(Sheet1!K34="Null", "Null", _xlfn.CONCAT("'", Sheet1!K34, "'"))), ",")</f>
         <v>'1NQ67',</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F114" t="str">
+        <f>IF(ISNUMBER(Sheet1!H34), Sheet1!H34, IF(Sheet1!H34="Null", "Null", _xlfn.CONCAT("'", Sheet1!H34, "'")))</f>
+        <v>'D9182'</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A115" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H35, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H35), Sheet1!H35, IF(Sheet1!H35="Null", "Null", _xlfn.CONCAT("'", Sheet1!H35, "'"))), ",")</f>
         <v>'MOWAG',</v>
       </c>
       <c r="B115" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I35, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I35), Sheet1!I35, IF(Sheet1!I35="Null", "Null", _xlfn.CONCAT("'", Sheet1!I35, "'"))), ",")</f>
         <v>'asdfas',</v>
       </c>
       <c r="C115" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J35, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J35), Sheet1!J35, IF(Sheet1!J35="Null", "Null", _xlfn.CONCAT("'", Sheet1!J35, "'"))), ",")</f>
         <v>'Apple',</v>
       </c>
       <c r="D115" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K35, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K35), Sheet1!K35, IF(Sheet1!K35="Null", "Null", _xlfn.CONCAT("'", Sheet1!K35, "'"))), ",")</f>
         <v>'Samsung',</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F115" t="str">
+        <f>IF(ISNUMBER(Sheet1!H35), Sheet1!H35, IF(Sheet1!H35="Null", "Null", _xlfn.CONCAT("'", Sheet1!H35, "'")))</f>
+        <v>'MOWAG'</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A116" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H36, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H36), Sheet1!H36, IF(Sheet1!H36="Null", "Null", _xlfn.CONCAT("'", Sheet1!H36, "'"))), ",")</f>
         <v>'Bernstrasse 1',</v>
       </c>
       <c r="B116" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I36, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I36), Sheet1!I36, IF(Sheet1!I36="Null", "Null", _xlfn.CONCAT("'", Sheet1!I36, "'"))), ",")</f>
         <v>'Rte du Lac 12',</v>
       </c>
       <c r="C116" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J36, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J36), Sheet1!J36, IF(Sheet1!J36="Null", "Null", _xlfn.CONCAT("'", Sheet1!J36, "'"))), ",")</f>
         <v>'One Apple Park Way',</v>
       </c>
       <c r="D116" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K36, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K36), Sheet1!K36, IF(Sheet1!K36="Null", "Null", _xlfn.CONCAT("'", Sheet1!K36, "'"))), ",")</f>
         <v>'Against Apple Way',</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F116" t="str">
+        <f>IF(ISNUMBER(Sheet1!H36), Sheet1!H36, IF(Sheet1!H36="Null", "Null", _xlfn.CONCAT("'", Sheet1!H36, "'")))</f>
+        <v>'Bernstrasse 1'</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A117" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H37, "',")</f>
-        <v>'2000',</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H37), Sheet1!H37, IF(Sheet1!H37="Null", "Null", _xlfn.CONCAT("'", Sheet1!H37, "'"))), ",")</f>
+        <v>2000,</v>
       </c>
       <c r="B117" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I37, "',")</f>
-        <v>'1215',</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I37), Sheet1!I37, IF(Sheet1!I37="Null", "Null", _xlfn.CONCAT("'", Sheet1!I37, "'"))), ",")</f>
+        <v>1215,</v>
       </c>
       <c r="C117" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J37, "',")</f>
-        <v>'95014',</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J37), Sheet1!J37, IF(Sheet1!J37="Null", "Null", _xlfn.CONCAT("'", Sheet1!J37, "'"))), ",")</f>
+        <v>95014,</v>
       </c>
       <c r="D117" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K37, "',")</f>
-        <v>'1',</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K37), Sheet1!K37, IF(Sheet1!K37="Null", "Null", _xlfn.CONCAT("'", Sheet1!K37, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+      <c r="F117">
+        <f>IF(ISNUMBER(Sheet1!H37), Sheet1!H37, IF(Sheet1!H37="Null", "Null", _xlfn.CONCAT("'", Sheet1!H37, "'")))</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A118" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H38, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H38), Sheet1!H38, IF(Sheet1!H38="Null", "Null", _xlfn.CONCAT("'", Sheet1!H38, "'"))), ",")</f>
         <v>'Neuchâtel',</v>
       </c>
       <c r="B118" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I38, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I38), Sheet1!I38, IF(Sheet1!I38="Null", "Null", _xlfn.CONCAT("'", Sheet1!I38, "'"))), ",")</f>
         <v>'Genère',</v>
       </c>
       <c r="C118" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J38, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J38), Sheet1!J38, IF(Sheet1!J38="Null", "Null", _xlfn.CONCAT("'", Sheet1!J38, "'"))), ",")</f>
         <v>'Cupertino',</v>
       </c>
       <c r="D118" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K38, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K38), Sheet1!K38, IF(Sheet1!K38="Null", "Null", _xlfn.CONCAT("'", Sheet1!K38, "'"))), ",")</f>
         <v>'Seoul',</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F118" t="str">
+        <f>IF(ISNUMBER(Sheet1!H38), Sheet1!H38, IF(Sheet1!H38="Null", "Null", _xlfn.CONCAT("'", Sheet1!H38, "'")))</f>
+        <v>'Neuchâtel'</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A119" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H39, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H39), Sheet1!H39, IF(Sheet1!H39="Null", "Null", _xlfn.CONCAT("'", Sheet1!H39, "'"))), ",")</f>
         <v>'1.1',</v>
       </c>
       <c r="B119" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I39, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I39), Sheet1!I39, IF(Sheet1!I39="Null", "Null", _xlfn.CONCAT("'", Sheet1!I39, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C119" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J39, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J39), Sheet1!J39, IF(Sheet1!J39="Null", "Null", _xlfn.CONCAT("'", Sheet1!J39, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D119" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K39, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K39), Sheet1!K39, IF(Sheet1!K39="Null", "Null", _xlfn.CONCAT("'", Sheet1!K39, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F119" t="str">
+        <f>IF(ISNUMBER(Sheet1!H39), Sheet1!H39, IF(Sheet1!H39="Null", "Null", _xlfn.CONCAT("'", Sheet1!H39, "'")))</f>
+        <v>'1.1'</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A120" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H40, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H40), Sheet1!H40, IF(Sheet1!H40="Null", "Null", _xlfn.CONCAT("'", Sheet1!H40, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="B120" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I40, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I40), Sheet1!I40, IF(Sheet1!I40="Null", "Null", _xlfn.CONCAT("'", Sheet1!I40, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C120" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J40, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J40), Sheet1!J40, IF(Sheet1!J40="Null", "Null", _xlfn.CONCAT("'", Sheet1!J40, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D120" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K40, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K40), Sheet1!K40, IF(Sheet1!K40="Null", "Null", _xlfn.CONCAT("'", Sheet1!K40, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F120" t="str">
+        <f>IF(ISNUMBER(Sheet1!H40), Sheet1!H40, IF(Sheet1!H40="Null", "Null", _xlfn.CONCAT("'", Sheet1!H40, "'")))</f>
+        <v>Null</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A121" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H41, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H41), Sheet1!H41, IF(Sheet1!H41="Null", "Null", _xlfn.CONCAT("'", Sheet1!H41, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="B121" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I41, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I41), Sheet1!I41, IF(Sheet1!I41="Null", "Null", _xlfn.CONCAT("'", Sheet1!I41, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="C121" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J41, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J41), Sheet1!J41, IF(Sheet1!J41="Null", "Null", _xlfn.CONCAT("'", Sheet1!J41, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="D121" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K41, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K41), Sheet1!K41, IF(Sheet1!K41="Null", "Null", _xlfn.CONCAT("'", Sheet1!K41, "'"))), ",")</f>
         <v>1,</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F121">
+        <f>IF(ISNUMBER(Sheet1!H41), Sheet1!H41, IF(Sheet1!H41="Null", "Null", _xlfn.CONCAT("'", Sheet1!H41, "'")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A122" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H42, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H42), Sheet1!H42, IF(Sheet1!H42="Null", "Null", _xlfn.CONCAT("'", Sheet1!H42, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="B122" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I42, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I42), Sheet1!I42, IF(Sheet1!I42="Null", "Null", _xlfn.CONCAT("'", Sheet1!I42, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="C122" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J42, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J42), Sheet1!J42, IF(Sheet1!J42="Null", "Null", _xlfn.CONCAT("'", Sheet1!J42, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="D122" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K42, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K42), Sheet1!K42, IF(Sheet1!K42="Null", "Null", _xlfn.CONCAT("'", Sheet1!K42, "'"))), ",")</f>
         <v>3,</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F122">
+        <f>IF(ISNUMBER(Sheet1!H42), Sheet1!H42, IF(Sheet1!H42="Null", "Null", _xlfn.CONCAT("'", Sheet1!H42, "'")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A123" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H43, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H43), Sheet1!H43, IF(Sheet1!H43="Null", "Null", _xlfn.CONCAT("'", Sheet1!H43, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="B123" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I43, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I43), Sheet1!I43, IF(Sheet1!I43="Null", "Null", _xlfn.CONCAT("'", Sheet1!I43, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="C123" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J43, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J43), Sheet1!J43, IF(Sheet1!J43="Null", "Null", _xlfn.CONCAT("'", Sheet1!J43, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="D123" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K43, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K43), Sheet1!K43, IF(Sheet1!K43="Null", "Null", _xlfn.CONCAT("'", Sheet1!K43, "'"))), ",")</f>
         <v>2,</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F123">
+        <f>IF(ISNUMBER(Sheet1!H43), Sheet1!H43, IF(Sheet1!H43="Null", "Null", _xlfn.CONCAT("'", Sheet1!H43, "'")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A124" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H44, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H44), Sheet1!H44, IF(Sheet1!H44="Null", "Null", _xlfn.CONCAT("'", Sheet1!H44, "'"))), ",")</f>
         <v>'0022',</v>
       </c>
       <c r="B124" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I44, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I44), Sheet1!I44, IF(Sheet1!I44="Null", "Null", _xlfn.CONCAT("'", Sheet1!I44, "'"))), ",")</f>
         <v>'0045',</v>
       </c>
       <c r="C124" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J44, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J44), Sheet1!J44, IF(Sheet1!J44="Null", "Null", _xlfn.CONCAT("'", Sheet1!J44, "'"))), ",")</f>
         <v>'0001',</v>
       </c>
       <c r="D124" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K44, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K44), Sheet1!K44, IF(Sheet1!K44="Null", "Null", _xlfn.CONCAT("'", Sheet1!K44, "'"))), ",")</f>
         <v>'0496',</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F124" t="str">
+        <f>IF(ISNUMBER(Sheet1!H44), Sheet1!H44, IF(Sheet1!H44="Null", "Null", _xlfn.CONCAT("'", Sheet1!H44, "'")))</f>
+        <v>'0022'</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A125" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H45, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H45), Sheet1!H45, IF(Sheet1!H45="Null", "Null", _xlfn.CONCAT("'", Sheet1!H45, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="B125" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I45, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I45), Sheet1!I45, IF(Sheet1!I45="Null", "Null", _xlfn.CONCAT("'", Sheet1!I45, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C125" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J45, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J45), Sheet1!J45, IF(Sheet1!J45="Null", "Null", _xlfn.CONCAT("'", Sheet1!J45, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D125" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K45, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K45), Sheet1!K45, IF(Sheet1!K45="Null", "Null", _xlfn.CONCAT("'", Sheet1!K45, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F125" t="str">
+        <f>IF(ISNUMBER(Sheet1!H45), Sheet1!H45, IF(Sheet1!H45="Null", "Null", _xlfn.CONCAT("'", Sheet1!H45, "'")))</f>
+        <v>Null</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A126" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H46, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H46), Sheet1!H46, IF(Sheet1!H46="Null", "Null", _xlfn.CONCAT("'", Sheet1!H46, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="B126" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I46, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I46), Sheet1!I46, IF(Sheet1!I46="Null", "Null", _xlfn.CONCAT("'", Sheet1!I46, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="C126" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J46, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J46), Sheet1!J46, IF(Sheet1!J46="Null", "Null", _xlfn.CONCAT("'", Sheet1!J46, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="D126" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K46, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K46), Sheet1!K46, IF(Sheet1!K46="Null", "Null", _xlfn.CONCAT("'", Sheet1!K46, "'"))), ",")</f>
         <v>1,</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F126">
+        <f>IF(ISNUMBER(Sheet1!H46), Sheet1!H46, IF(Sheet1!H46="Null", "Null", _xlfn.CONCAT("'", Sheet1!H46, "'")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A127" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H47, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H47), Sheet1!H47, IF(Sheet1!H47="Null", "Null", _xlfn.CONCAT("'", Sheet1!H47, "'"))), ",")</f>
         <v>'1000051294',</v>
       </c>
       <c r="B127" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I47, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I47), Sheet1!I47, IF(Sheet1!I47="Null", "Null", _xlfn.CONCAT("'", Sheet1!I47, "'"))), ",")</f>
         <v>'1000058908',</v>
       </c>
       <c r="C127" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J47, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J47), Sheet1!J47, IF(Sheet1!J47="Null", "Null", _xlfn.CONCAT("'", Sheet1!J47, "'"))), ",")</f>
         <v>'1000057308',</v>
       </c>
       <c r="D127" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K47, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K47), Sheet1!K47, IF(Sheet1!K47="Null", "Null", _xlfn.CONCAT("'", Sheet1!K47, "'"))), ",")</f>
         <v>'1000053644',</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F127" t="str">
+        <f>IF(ISNUMBER(Sheet1!H47), Sheet1!H47, IF(Sheet1!H47="Null", "Null", _xlfn.CONCAT("'", Sheet1!H47, "'")))</f>
+        <v>'1000051294'</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A128" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H48, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H48), Sheet1!H48, IF(Sheet1!H48="Null", "Null", _xlfn.CONCAT("'", Sheet1!H48, "'"))), ",")</f>
         <v>'ZX0000040',</v>
       </c>
       <c r="B128" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I48, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I48), Sheet1!I48, IF(Sheet1!I48="Null", "Null", _xlfn.CONCAT("'", Sheet1!I48, "'"))), ",")</f>
         <v>'ZX0000040',</v>
       </c>
       <c r="C128" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J48, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J48), Sheet1!J48, IF(Sheet1!J48="Null", "Null", _xlfn.CONCAT("'", Sheet1!J48, "'"))), ",")</f>
         <v>'ZX0000040',</v>
       </c>
       <c r="D128" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K48, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K48), Sheet1!K48, IF(Sheet1!K48="Null", "Null", _xlfn.CONCAT("'", Sheet1!K48, "'"))), ",")</f>
         <v>'ZX0000040',</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F128" t="str">
+        <f>IF(ISNUMBER(Sheet1!H48), Sheet1!H48, IF(Sheet1!H48="Null", "Null", _xlfn.CONCAT("'", Sheet1!H48, "'")))</f>
+        <v>'ZX0000040'</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A129" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H49, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H49), Sheet1!H49, IF(Sheet1!H49="Null", "Null", _xlfn.CONCAT("'", Sheet1!H49, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="B129" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I49, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I49), Sheet1!I49, IF(Sheet1!I49="Null", "Null", _xlfn.CONCAT("'", Sheet1!I49, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="C129" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J49, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J49), Sheet1!J49, IF(Sheet1!J49="Null", "Null", _xlfn.CONCAT("'", Sheet1!J49, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="D129" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K49, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K49), Sheet1!K49, IF(Sheet1!K49="Null", "Null", _xlfn.CONCAT("'", Sheet1!K49, "'"))), ",")</f>
         <v>1,</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F129">
+        <f>IF(ISNUMBER(Sheet1!H49), Sheet1!H49, IF(Sheet1!H49="Null", "Null", _xlfn.CONCAT("'", Sheet1!H49, "'")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A130" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H50, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H50), Sheet1!H50, IF(Sheet1!H50="Null", "Null", _xlfn.CONCAT("'", Sheet1!H50, "'"))), ",")</f>
         <v>'abcde',</v>
       </c>
       <c r="B130" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I50, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I50), Sheet1!I50, IF(Sheet1!I50="Null", "Null", _xlfn.CONCAT("'", Sheet1!I50, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C130" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J50, "',")</f>
-        <v>'54321',</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J50), Sheet1!J50, IF(Sheet1!J50="Null", "Null", _xlfn.CONCAT("'", Sheet1!J50, "'"))), ",")</f>
+        <v>54321,</v>
       </c>
       <c r="D130" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K50, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K50), Sheet1!K50, IF(Sheet1!K50="Null", "Null", _xlfn.CONCAT("'", Sheet1!K50, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F130" t="str">
+        <f>IF(ISNUMBER(Sheet1!H50), Sheet1!H50, IF(Sheet1!H50="Null", "Null", _xlfn.CONCAT("'", Sheet1!H50, "'")))</f>
+        <v>'abcde'</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A131" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H51, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H51), Sheet1!H51, IF(Sheet1!H51="Null", "Null", _xlfn.CONCAT("'", Sheet1!H51, "'"))), ",")</f>
         <v>'.1',</v>
       </c>
       <c r="B131" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I51, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I51), Sheet1!I51, IF(Sheet1!I51="Null", "Null", _xlfn.CONCAT("'", Sheet1!I51, "'"))), ",")</f>
         <v>'0000',</v>
       </c>
       <c r="C131" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J51, "',")</f>
-        <v>'1.01',</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J51), Sheet1!J51, IF(Sheet1!J51="Null", "Null", _xlfn.CONCAT("'", Sheet1!J51, "'"))), ",")</f>
+        <v>1.01,</v>
       </c>
       <c r="D131" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K51, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K51), Sheet1!K51, IF(Sheet1!K51="Null", "Null", _xlfn.CONCAT("'", Sheet1!K51, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F131" t="str">
+        <f>IF(ISNUMBER(Sheet1!H51), Sheet1!H51, IF(Sheet1!H51="Null", "Null", _xlfn.CONCAT("'", Sheet1!H51, "'")))</f>
+        <v>'.1'</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A132" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H52, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H52), Sheet1!H52, IF(Sheet1!H52="Null", "Null", _xlfn.CONCAT("'", Sheet1!H52, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="B132" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I52, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I52), Sheet1!I52, IF(Sheet1!I52="Null", "Null", _xlfn.CONCAT("'", Sheet1!I52, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C132" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J52, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J52), Sheet1!J52, IF(Sheet1!J52="Null", "Null", _xlfn.CONCAT("'", Sheet1!J52, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="D132" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K52, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K52), Sheet1!K52, IF(Sheet1!K52="Null", "Null", _xlfn.CONCAT("'", Sheet1!K52, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F132" t="str">
+        <f>IF(ISNUMBER(Sheet1!H52), Sheet1!H52, IF(Sheet1!H52="Null", "Null", _xlfn.CONCAT("'", Sheet1!H52, "'")))</f>
+        <v>'t'</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A133" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H53, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H53), Sheet1!H53, IF(Sheet1!H53="Null", "Null", _xlfn.CONCAT("'", Sheet1!H53, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="B133" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I53, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I53), Sheet1!I53, IF(Sheet1!I53="Null", "Null", _xlfn.CONCAT("'", Sheet1!I53, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C133" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J53, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J53), Sheet1!J53, IF(Sheet1!J53="Null", "Null", _xlfn.CONCAT("'", Sheet1!J53, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D133" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K53, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K53), Sheet1!K53, IF(Sheet1!K53="Null", "Null", _xlfn.CONCAT("'", Sheet1!K53, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F133" t="str">
+        <f>IF(ISNUMBER(Sheet1!H53), Sheet1!H53, IF(Sheet1!H53="Null", "Null", _xlfn.CONCAT("'", Sheet1!H53, "'")))</f>
+        <v>Null</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A134" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H54, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H54), Sheet1!H54, IF(Sheet1!H54="Null", "Null", _xlfn.CONCAT("'", Sheet1!H54, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="B134" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I54, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I54), Sheet1!I54, IF(Sheet1!I54="Null", "Null", _xlfn.CONCAT("'", Sheet1!I54, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="C134" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J54, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J54), Sheet1!J54, IF(Sheet1!J54="Null", "Null", _xlfn.CONCAT("'", Sheet1!J54, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D134" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K54, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K54), Sheet1!K54, IF(Sheet1!K54="Null", "Null", _xlfn.CONCAT("'", Sheet1!K54, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F134" t="str">
+        <f>IF(ISNUMBER(Sheet1!H54), Sheet1!H54, IF(Sheet1!H54="Null", "Null", _xlfn.CONCAT("'", Sheet1!H54, "'")))</f>
+        <v>'t'</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A135" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H55, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H55), Sheet1!H55, IF(Sheet1!H55="Null", "Null", _xlfn.CONCAT("'", Sheet1!H55, "'"))), ",")</f>
         <v>'f',</v>
       </c>
       <c r="B135" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I55, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I55), Sheet1!I55, IF(Sheet1!I55="Null", "Null", _xlfn.CONCAT("'", Sheet1!I55, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="C135" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J55, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J55), Sheet1!J55, IF(Sheet1!J55="Null", "Null", _xlfn.CONCAT("'", Sheet1!J55, "'"))), ",")</f>
         <v>'f',</v>
       </c>
       <c r="D135" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K55, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K55), Sheet1!K55, IF(Sheet1!K55="Null", "Null", _xlfn.CONCAT("'", Sheet1!K55, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F135" t="str">
+        <f>IF(ISNUMBER(Sheet1!H55), Sheet1!H55, IF(Sheet1!H55="Null", "Null", _xlfn.CONCAT("'", Sheet1!H55, "'")))</f>
+        <v>'f'</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A136" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H56, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H56), Sheet1!H56, IF(Sheet1!H56="Null", "Null", _xlfn.CONCAT("'", Sheet1!H56, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="B136" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I56, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I56), Sheet1!I56, IF(Sheet1!I56="Null", "Null", _xlfn.CONCAT("'", Sheet1!I56, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="C136" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J56, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J56), Sheet1!J56, IF(Sheet1!J56="Null", "Null", _xlfn.CONCAT("'", Sheet1!J56, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="D136" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K56, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K56), Sheet1!K56, IF(Sheet1!K56="Null", "Null", _xlfn.CONCAT("'", Sheet1!K56, "'"))), ",")</f>
         <v>1,</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F136">
+        <f>IF(ISNUMBER(Sheet1!H56), Sheet1!H56, IF(Sheet1!H56="Null", "Null", _xlfn.CONCAT("'", Sheet1!H56, "'")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A137" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H57, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H57), Sheet1!H57, IF(Sheet1!H57="Null", "Null", _xlfn.CONCAT("'", Sheet1!H57, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="B137" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I57, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I57), Sheet1!I57, IF(Sheet1!I57="Null", "Null", _xlfn.CONCAT("'", Sheet1!I57, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="C137" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J57, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J57), Sheet1!J57, IF(Sheet1!J57="Null", "Null", _xlfn.CONCAT("'", Sheet1!J57, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="D137" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K57, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K57), Sheet1!K57, IF(Sheet1!K57="Null", "Null", _xlfn.CONCAT("'", Sheet1!K57, "'"))), ",")</f>
         <v>4,</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F137">
+        <f>IF(ISNUMBER(Sheet1!H57), Sheet1!H57, IF(Sheet1!H57="Null", "Null", _xlfn.CONCAT("'", Sheet1!H57, "'")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A138" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H58, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H58), Sheet1!H58, IF(Sheet1!H58="Null", "Null", _xlfn.CONCAT("'", Sheet1!H58, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="B138" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I58, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I58), Sheet1!I58, IF(Sheet1!I58="Null", "Null", _xlfn.CONCAT("'", Sheet1!I58, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C138" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J58, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J58), Sheet1!J58, IF(Sheet1!J58="Null", "Null", _xlfn.CONCAT("'", Sheet1!J58, "'"))), ",")</f>
         <v>4,</v>
       </c>
       <c r="D138" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K58, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K58), Sheet1!K58, IF(Sheet1!K58="Null", "Null", _xlfn.CONCAT("'", Sheet1!K58, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F138" t="str">
+        <f>IF(ISNUMBER(Sheet1!H58), Sheet1!H58, IF(Sheet1!H58="Null", "Null", _xlfn.CONCAT("'", Sheet1!H58, "'")))</f>
+        <v>Null</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A139" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H59, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H59), Sheet1!H59, IF(Sheet1!H59="Null", "Null", _xlfn.CONCAT("'", Sheet1!H59, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="B139" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I59, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I59), Sheet1!I59, IF(Sheet1!I59="Null", "Null", _xlfn.CONCAT("'", Sheet1!I59, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C139" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J59, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J59), Sheet1!J59, IF(Sheet1!J59="Null", "Null", _xlfn.CONCAT("'", Sheet1!J59, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D139" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K59, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K59), Sheet1!K59, IF(Sheet1!K59="Null", "Null", _xlfn.CONCAT("'", Sheet1!K59, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F139" t="str">
+        <f>IF(ISNUMBER(Sheet1!H59), Sheet1!H59, IF(Sheet1!H59="Null", "Null", _xlfn.CONCAT("'", Sheet1!H59, "'")))</f>
+        <v>Null</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A140" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H60, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H60), Sheet1!H60, IF(Sheet1!H60="Null", "Null", _xlfn.CONCAT("'", Sheet1!H60, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="B140" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I60, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I60), Sheet1!I60, IF(Sheet1!I60="Null", "Null", _xlfn.CONCAT("'", Sheet1!I60, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="C140" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J60, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J60), Sheet1!J60, IF(Sheet1!J60="Null", "Null", _xlfn.CONCAT("'", Sheet1!J60, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="D140" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K60, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K60), Sheet1!K60, IF(Sheet1!K60="Null", "Null", _xlfn.CONCAT("'", Sheet1!K60, "'"))), ",")</f>
         <v>3,</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F140">
+        <f>IF(ISNUMBER(Sheet1!H60), Sheet1!H60, IF(Sheet1!H60="Null", "Null", _xlfn.CONCAT("'", Sheet1!H60, "'")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A141" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H61, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H61), Sheet1!H61, IF(Sheet1!H61="Null", "Null", _xlfn.CONCAT("'", Sheet1!H61, "'"))), ",")</f>
         <v>35,</v>
       </c>
       <c r="B141" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I61, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I61), Sheet1!I61, IF(Sheet1!I61="Null", "Null", _xlfn.CONCAT("'", Sheet1!I61, "'"))), ",")</f>
         <v>35,</v>
       </c>
       <c r="C141" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J61, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J61), Sheet1!J61, IF(Sheet1!J61="Null", "Null", _xlfn.CONCAT("'", Sheet1!J61, "'"))), ",")</f>
         <v>35,</v>
       </c>
       <c r="D141" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K61, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K61), Sheet1!K61, IF(Sheet1!K61="Null", "Null", _xlfn.CONCAT("'", Sheet1!K61, "'"))), ",")</f>
         <v>35,</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F141">
+        <f>IF(ISNUMBER(Sheet1!H61), Sheet1!H61, IF(Sheet1!H61="Null", "Null", _xlfn.CONCAT("'", Sheet1!H61, "'")))</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A142" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H62, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H62), Sheet1!H62, IF(Sheet1!H62="Null", "Null", _xlfn.CONCAT("'", Sheet1!H62, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="B142" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I62, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I62), Sheet1!I62, IF(Sheet1!I62="Null", "Null", _xlfn.CONCAT("'", Sheet1!I62, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C142" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J62, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J62), Sheet1!J62, IF(Sheet1!J62="Null", "Null", _xlfn.CONCAT("'", Sheet1!J62, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D142" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K62, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K62), Sheet1!K62, IF(Sheet1!K62="Null", "Null", _xlfn.CONCAT("'", Sheet1!K62, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F142" t="str">
+        <f>IF(ISNUMBER(Sheet1!H62), Sheet1!H62, IF(Sheet1!H62="Null", "Null", _xlfn.CONCAT("'", Sheet1!H62, "'")))</f>
+        <v>Null</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A143" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H63, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H63), Sheet1!H63, IF(Sheet1!H63="Null", "Null", _xlfn.CONCAT("'", Sheet1!H63, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="B143" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I63, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I63), Sheet1!I63, IF(Sheet1!I63="Null", "Null", _xlfn.CONCAT("'", Sheet1!I63, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="C143" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J63, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J63), Sheet1!J63, IF(Sheet1!J63="Null", "Null", _xlfn.CONCAT("'", Sheet1!J63, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="D143" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K63, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K63), Sheet1!K63, IF(Sheet1!K63="Null", "Null", _xlfn.CONCAT("'", Sheet1!K63, "'"))), ",")</f>
         <v>1,</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F143">
+        <f>IF(ISNUMBER(Sheet1!H63), Sheet1!H63, IF(Sheet1!H63="Null", "Null", _xlfn.CONCAT("'", Sheet1!H63, "'")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A144" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H64, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H64), Sheet1!H64, IF(Sheet1!H64="Null", "Null", _xlfn.CONCAT("'", Sheet1!H64, "'"))), ",")</f>
         <v>'09211600-7',</v>
       </c>
       <c r="B144" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I64, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I64), Sheet1!I64, IF(Sheet1!I64="Null", "Null", _xlfn.CONCAT("'", Sheet1!I64, "'"))), ",")</f>
         <v>'09221000-4',</v>
       </c>
       <c r="C144" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J64, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J64), Sheet1!J64, IF(Sheet1!J64="Null", "Null", _xlfn.CONCAT("'", Sheet1!J64, "'"))), ",")</f>
         <v>'09221400-8',</v>
       </c>
       <c r="D144" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K64, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K64), Sheet1!K64, IF(Sheet1!K64="Null", "Null", _xlfn.CONCAT("'", Sheet1!K64, "'"))), ",")</f>
         <v>'09230000-0',</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F144" t="str">
+        <f>IF(ISNUMBER(Sheet1!H64), Sheet1!H64, IF(Sheet1!H64="Null", "Null", _xlfn.CONCAT("'", Sheet1!H64, "'")))</f>
+        <v>'09211600-7'</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A145" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H65, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H65), Sheet1!H65, IF(Sheet1!H65="Null", "Null", _xlfn.CONCAT("'", Sheet1!H65, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="B145" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I65, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I65), Sheet1!I65, IF(Sheet1!I65="Null", "Null", _xlfn.CONCAT("'", Sheet1!I65, "'"))), ",")</f>
         <v>4,</v>
       </c>
       <c r="C145" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J65, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J65), Sheet1!J65, IF(Sheet1!J65="Null", "Null", _xlfn.CONCAT("'", Sheet1!J65, "'"))), ",")</f>
         <v>4,</v>
       </c>
       <c r="D145" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K65, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K65), Sheet1!K65, IF(Sheet1!K65="Null", "Null", _xlfn.CONCAT("'", Sheet1!K65, "'"))), ",")</f>
         <v>3,</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F145">
+        <f>IF(ISNUMBER(Sheet1!H65), Sheet1!H65, IF(Sheet1!H65="Null", "Null", _xlfn.CONCAT("'", Sheet1!H65, "'")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A146" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H66, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H66), Sheet1!H66, IF(Sheet1!H66="Null", "Null", _xlfn.CONCAT("'", Sheet1!H66, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="B146" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I66, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I66), Sheet1!I66, IF(Sheet1!I66="Null", "Null", _xlfn.CONCAT("'", Sheet1!I66, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="C146" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J66, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J66), Sheet1!J66, IF(Sheet1!J66="Null", "Null", _xlfn.CONCAT("'", Sheet1!J66, "'"))), ",")</f>
         <v>4,</v>
       </c>
       <c r="D146" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K66, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K66), Sheet1!K66, IF(Sheet1!K66="Null", "Null", _xlfn.CONCAT("'", Sheet1!K66, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F146" t="str">
+        <f>IF(ISNUMBER(Sheet1!H66), Sheet1!H66, IF(Sheet1!H66="Null", "Null", _xlfn.CONCAT("'", Sheet1!H66, "'")))</f>
+        <v>Null</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A147" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H67, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H67), Sheet1!H67, IF(Sheet1!H67="Null", "Null", _xlfn.CONCAT("'", Sheet1!H67, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="B147" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I67, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I67), Sheet1!I67, IF(Sheet1!I67="Null", "Null", _xlfn.CONCAT("'", Sheet1!I67, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C147" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J67, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J67), Sheet1!J67, IF(Sheet1!J67="Null", "Null", _xlfn.CONCAT("'", Sheet1!J67, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="D147" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K67, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K67), Sheet1!K67, IF(Sheet1!K67="Null", "Null", _xlfn.CONCAT("'", Sheet1!K67, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F147" t="str">
+        <f>IF(ISNUMBER(Sheet1!H67), Sheet1!H67, IF(Sheet1!H67="Null", "Null", _xlfn.CONCAT("'", Sheet1!H67, "'")))</f>
+        <v>'t'</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A148" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H68, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H68), Sheet1!H68, IF(Sheet1!H68="Null", "Null", _xlfn.CONCAT("'", Sheet1!H68, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="B148" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I68, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I68), Sheet1!I68, IF(Sheet1!I68="Null", "Null", _xlfn.CONCAT("'", Sheet1!I68, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C148" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J68, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J68), Sheet1!J68, IF(Sheet1!J68="Null", "Null", _xlfn.CONCAT("'", Sheet1!J68, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="D148" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K68, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K68), Sheet1!K68, IF(Sheet1!K68="Null", "Null", _xlfn.CONCAT("'", Sheet1!K68, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F148">
+        <f>IF(ISNUMBER(Sheet1!H68), Sheet1!H68, IF(Sheet1!H68="Null", "Null", _xlfn.CONCAT("'", Sheet1!H68, "'")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A149" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H69, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H69), Sheet1!H69, IF(Sheet1!H69="Null", "Null", _xlfn.CONCAT("'", Sheet1!H69, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="B149" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I69, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I69), Sheet1!I69, IF(Sheet1!I69="Null", "Null", _xlfn.CONCAT("'", Sheet1!I69, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C149" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J69, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J69), Sheet1!J69, IF(Sheet1!J69="Null", "Null", _xlfn.CONCAT("'", Sheet1!J69, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="D149" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K69, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K69), Sheet1!K69, IF(Sheet1!K69="Null", "Null", _xlfn.CONCAT("'", Sheet1!K69, "'"))), ",")</f>
         <v>1,</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F149">
+        <f>IF(ISNUMBER(Sheet1!H69), Sheet1!H69, IF(Sheet1!H69="Null", "Null", _xlfn.CONCAT("'", Sheet1!H69, "'")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A150" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H70, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H70), Sheet1!H70, IF(Sheet1!H70="Null", "Null", _xlfn.CONCAT("'", Sheet1!H70, "'"))), ",")</f>
         <v>14,</v>
       </c>
       <c r="B150" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I70, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I70), Sheet1!I70, IF(Sheet1!I70="Null", "Null", _xlfn.CONCAT("'", Sheet1!I70, "'"))), ",")</f>
         <v>14,</v>
       </c>
       <c r="C150" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J70, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J70), Sheet1!J70, IF(Sheet1!J70="Null", "Null", _xlfn.CONCAT("'", Sheet1!J70, "'"))), ",")</f>
         <v>14,</v>
       </c>
       <c r="D150" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K70, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K70), Sheet1!K70, IF(Sheet1!K70="Null", "Null", _xlfn.CONCAT("'", Sheet1!K70, "'"))), ",")</f>
         <v>14,</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F150">
+        <f>IF(ISNUMBER(Sheet1!H70), Sheet1!H70, IF(Sheet1!H70="Null", "Null", _xlfn.CONCAT("'", Sheet1!H70, "'")))</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A151" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H71, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H71), Sheet1!H71, IF(Sheet1!H71="Null", "Null", _xlfn.CONCAT("'", Sheet1!H71, "'"))), ",")</f>
         <v>'SYSTEMM',</v>
       </c>
       <c r="B151" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I71, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I71), Sheet1!I71, IF(Sheet1!I71="Null", "Null", _xlfn.CONCAT("'", Sheet1!I71, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C151" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J71, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J71), Sheet1!J71, IF(Sheet1!J71="Null", "Null", _xlfn.CONCAT("'", Sheet1!J71, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D151" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K71, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K71), Sheet1!K71, IF(Sheet1!K71="Null", "Null", _xlfn.CONCAT("'", Sheet1!K71, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F151" t="str">
+        <f>IF(ISNUMBER(Sheet1!H71), Sheet1!H71, IF(Sheet1!H71="Null", "Null", _xlfn.CONCAT("'", Sheet1!H71, "'")))</f>
+        <v>'SYSTEMM'</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A152" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H72, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H72), Sheet1!H72, IF(Sheet1!H72="Null", "Null", _xlfn.CONCAT("'", Sheet1!H72, "'"))), ",")</f>
         <v>'55G',</v>
       </c>
       <c r="B152" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I72, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I72), Sheet1!I72, IF(Sheet1!I72="Null", "Null", _xlfn.CONCAT("'", Sheet1!I72, "'"))), ",")</f>
         <v>'55G',</v>
       </c>
       <c r="C152" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J72, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J72), Sheet1!J72, IF(Sheet1!J72="Null", "Null", _xlfn.CONCAT("'", Sheet1!J72, "'"))), ",")</f>
         <v>'55G',</v>
       </c>
       <c r="D152" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K72, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K72), Sheet1!K72, IF(Sheet1!K72="Null", "Null", _xlfn.CONCAT("'", Sheet1!K72, "'"))), ",")</f>
         <v>'55G',</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F152" t="str">
+        <f>IF(ISNUMBER(Sheet1!H72), Sheet1!H72, IF(Sheet1!H72="Null", "Null", _xlfn.CONCAT("'", Sheet1!H72, "'")))</f>
+        <v>'55G'</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A153" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H73, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H73), Sheet1!H73, IF(Sheet1!H73="Null", "Null", _xlfn.CONCAT("'", Sheet1!H73, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="B153" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I73, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I73), Sheet1!I73, IF(Sheet1!I73="Null", "Null", _xlfn.CONCAT("'", Sheet1!I73, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C153" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J73, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J73), Sheet1!J73, IF(Sheet1!J73="Null", "Null", _xlfn.CONCAT("'", Sheet1!J73, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="D153" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K73, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K73), Sheet1!K73, IF(Sheet1!K73="Null", "Null", _xlfn.CONCAT("'", Sheet1!K73, "'"))), ",")</f>
         <v>'f',</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="F153" t="str">
+        <f>IF(ISNUMBER(Sheet1!H73), Sheet1!H73, IF(Sheet1!H73="Null", "Null", _xlfn.CONCAT("'", Sheet1!H73, "'")))</f>
+        <v>'t'</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A154" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H74, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H74), Sheet1!H74, IF(Sheet1!H74="Null", "Null", _xlfn.CONCAT("'", Sheet1!H74, "'"))), ",")</f>
         <v>'NEXTHIGHER',</v>
       </c>
       <c r="B154" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I74, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I74), Sheet1!I74, IF(Sheet1!I74="Null", "Null", _xlfn.CONCAT("'", Sheet1!I74, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C154" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J74, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J74), Sheet1!J74, IF(Sheet1!J74="Null", "Null", _xlfn.CONCAT("'", Sheet1!J74, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D154" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K74, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K74), Sheet1!K74, IF(Sheet1!K74="Null", "Null", _xlfn.CONCAT("'", Sheet1!K74, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F154" t="str">
+        <f>IF(ISNUMBER(Sheet1!H74), Sheet1!H74, IF(Sheet1!H74="Null", "Null", _xlfn.CONCAT("'", Sheet1!H74, "'")))</f>
+        <v>'NEXTHIGHER'</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A155" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H75, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H75), Sheet1!H75, IF(Sheet1!H75="Null", "Null", _xlfn.CONCAT("'", Sheet1!H75, "'"))), ",")</f>
         <v>'NESCHUB',</v>
       </c>
       <c r="B155" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I75, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I75), Sheet1!I75, IF(Sheet1!I75="Null", "Null", _xlfn.CONCAT("'", Sheet1!I75, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C155" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J75, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J75), Sheet1!J75, IF(Sheet1!J75="Null", "Null", _xlfn.CONCAT("'", Sheet1!J75, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D155" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K75, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K75), Sheet1!K75, IF(Sheet1!K75="Null", "Null", _xlfn.CONCAT("'", Sheet1!K75, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F155" t="str">
+        <f>IF(ISNUMBER(Sheet1!H75), Sheet1!H75, IF(Sheet1!H75="Null", "Null", _xlfn.CONCAT("'", Sheet1!H75, "'")))</f>
+        <v>'NESCHUB'</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A156" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H76, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H76), Sheet1!H76, IF(Sheet1!H76="Null", "Null", _xlfn.CONCAT("'", Sheet1!H76, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="B156" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I76, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I76), Sheet1!I76, IF(Sheet1!I76="Null", "Null", _xlfn.CONCAT("'", Sheet1!I76, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C156" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J76, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J76), Sheet1!J76, IF(Sheet1!J76="Null", "Null", _xlfn.CONCAT("'", Sheet1!J76, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="D156" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K76, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K76), Sheet1!K76, IF(Sheet1!K76="Null", "Null", _xlfn.CONCAT("'", Sheet1!K76, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F156" t="str">
+        <f>IF(ISNUMBER(Sheet1!H76), Sheet1!H76, IF(Sheet1!H76="Null", "Null", _xlfn.CONCAT("'", Sheet1!H76, "'")))</f>
+        <v>'t'</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A157" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H77, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H77), Sheet1!H77, IF(Sheet1!H77="Null", "Null", _xlfn.CONCAT("'", Sheet1!H77, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="B157" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I77, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I77), Sheet1!I77, IF(Sheet1!I77="Null", "Null", _xlfn.CONCAT("'", Sheet1!I77, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C157" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J77, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J77), Sheet1!J77, IF(Sheet1!J77="Null", "Null", _xlfn.CONCAT("'", Sheet1!J77, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D157" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K77, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K77), Sheet1!K77, IF(Sheet1!K77="Null", "Null", _xlfn.CONCAT("'", Sheet1!K77, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F157" t="str">
+        <f>IF(ISNUMBER(Sheet1!H77), Sheet1!H77, IF(Sheet1!H77="Null", "Null", _xlfn.CONCAT("'", Sheet1!H77, "'")))</f>
+        <v>'t'</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A158" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H78, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H78), Sheet1!H78, IF(Sheet1!H78="Null", "Null", _xlfn.CONCAT("'", Sheet1!H78, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="B158" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I78, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I78), Sheet1!I78, IF(Sheet1!I78="Null", "Null", _xlfn.CONCAT("'", Sheet1!I78, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="C158" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J78, ",")</f>
-        <v>null,</v>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J78), Sheet1!J78, IF(Sheet1!J78="Null", "Null", _xlfn.CONCAT("'", Sheet1!J78, "'"))), ",")</f>
+        <v>Null,</v>
       </c>
       <c r="D158" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K78, ",")</f>
-        <v>null,</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K78), Sheet1!K78, IF(Sheet1!K78="Null", "Null", _xlfn.CONCAT("'", Sheet1!K78, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="F158" t="str">
+        <f>IF(ISNUMBER(Sheet1!H78), Sheet1!H78, IF(Sheet1!H78="Null", "Null", _xlfn.CONCAT("'", Sheet1!H78, "'")))</f>
+        <v>'t'</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A159" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H79, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H79), Sheet1!H79, IF(Sheet1!H79="Null", "Null", _xlfn.CONCAT("'", Sheet1!H79, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="B159" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I79, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I79), Sheet1!I79, IF(Sheet1!I79="Null", "Null", _xlfn.CONCAT("'", Sheet1!I79, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="C159" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J79, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J79), Sheet1!J79, IF(Sheet1!J79="Null", "Null", _xlfn.CONCAT("'", Sheet1!J79, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="D159" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K79, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K79), Sheet1!K79, IF(Sheet1!K79="Null", "Null", _xlfn.CONCAT("'", Sheet1!K79, "'"))), ",")</f>
         <v>4,</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A160">
-        <f>Sheet1!H80</f>
+      <c r="F159">
+        <f>IF(ISNUMBER(Sheet1!H79), Sheet1!H79, IF(Sheet1!H79="Null", "Null", _xlfn.CONCAT("'", Sheet1!H79, "'")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A160" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H80), Sheet1!H80, IF(Sheet1!H80="Null", "Null", _xlfn.CONCAT("'", Sheet1!H80, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="B160" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I80), Sheet1!I80, IF(Sheet1!I80="Null", "Null", _xlfn.CONCAT("'", Sheet1!I80, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="C160" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J80), Sheet1!J80, IF(Sheet1!J80="Null", "Null", _xlfn.CONCAT("'", Sheet1!J80, "'"))), ",")</f>
+        <v>4,</v>
+      </c>
+      <c r="D160" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K80), Sheet1!K80, IF(Sheet1!K80="Null", "Null", _xlfn.CONCAT("'", Sheet1!K80, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="F160">
+        <f>IF(ISNUMBER(Sheet1!H80), Sheet1!H80, IF(Sheet1!H80="Null", "Null", _xlfn.CONCAT("'", Sheet1!H80, "'")))</f>
         <v>3</v>
-      </c>
-      <c r="B160">
-        <f>Sheet1!I80</f>
-        <v>2</v>
-      </c>
-      <c r="C160">
-        <f>Sheet1!J80</f>
-        <v>4</v>
-      </c>
-      <c r="D160">
-        <f>Sheet1!K80</f>
-        <v>2</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Fixed the queries for injecting real data.
</commit_message>
<xml_diff>
--- a/b11_1/fields/insert.xlsx
+++ b/b11_1/fields/insert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yann/Prog/Python/LBA/b11_1/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9B6C1A-608E-9243-B3F1-05048CA58938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA054F5B-81EA-7940-90B9-DB15437D4E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="5000" windowWidth="46780" windowHeight="18000" activeTab="1" xr2:uid="{41FF1C03-8D98-44C8-8EDC-6562CA448D86}"/>
+    <workbookView xWindow="1400" yWindow="5000" windowWidth="46780" windowHeight="18000" activeTab="1" xr2:uid="{41FF1C03-8D98-44C8-8EDC-6562CA448D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1258,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1F6E88-797B-42CA-9EC0-C2555AB4031B}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23:K23"/>
+    <sheetView topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24:K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1968,18 +1968,6 @@
       <c r="B24" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="H24">
-        <v>10</v>
-      </c>
-      <c r="I24">
-        <v>10</v>
-      </c>
-      <c r="J24">
-        <v>10</v>
-      </c>
-      <c r="K24">
-        <v>10</v>
-      </c>
     </row>
     <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -3645,9 +3633,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB86915-FE40-8640-8F00-428279462302}">
-  <dimension ref="A1:F161"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5090,7 +5080,7 @@
         <v>auspraegung_id</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>267</v>
       </c>
@@ -5104,1698 +5094,1426 @@
         <v>267</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A82" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H2, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H2), Sheet1!H2, IF(OR(Sheet1!H2="Null", Sheet1!H2=""), "Null", _xlfn.CONCAT("'", Sheet1!H2, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="B82" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I2, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I2), Sheet1!I2, IF(OR(Sheet1!I2="Null", Sheet1!I2=""), "Null", _xlfn.CONCAT("'", Sheet1!I2, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="C82" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J2, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J2), Sheet1!J2, IF(OR(Sheet1!J2="Null", Sheet1!J2=""), "Null", _xlfn.CONCAT("'", Sheet1!J2, "'"))), ",")</f>
         <v>'t',</v>
       </c>
       <c r="D82" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K2, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K2), Sheet1!K2, IF(OR(Sheet1!K2="Null", Sheet1!K2=""), "Null", _xlfn.CONCAT("'", Sheet1!K2, "'"))), ",")</f>
         <v>'t',</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A83" t="str">
-        <f>_xlfn.CONCAT(Sheet1!H3, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H3), Sheet1!H3, IF(OR(Sheet1!H3="Null", Sheet1!H3=""), "Null", _xlfn.CONCAT("'", Sheet1!H3, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="B83" t="str">
-        <f>_xlfn.CONCAT(Sheet1!I3, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I3), Sheet1!I3, IF(OR(Sheet1!I3="Null", Sheet1!I3=""), "Null", _xlfn.CONCAT("'", Sheet1!I3, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="C83" t="str">
-        <f>_xlfn.CONCAT(Sheet1!J3, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J3), Sheet1!J3, IF(OR(Sheet1!J3="Null", Sheet1!J3=""), "Null", _xlfn.CONCAT("'", Sheet1!J3, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="D83" t="str">
-        <f>_xlfn.CONCAT(Sheet1!K3, ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K3), Sheet1!K3, IF(OR(Sheet1!K3="Null", Sheet1!K3=""), "Null", _xlfn.CONCAT("'", Sheet1!K3, "'"))), ",")</f>
         <v>4,</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A84" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H4, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H4), Sheet1!H4, IF(OR(Sheet1!H4="Null", Sheet1!H4=""), "Null", _xlfn.CONCAT("'", Sheet1!H4, "'"))), ",")</f>
         <v>'Kurztext DE XYZ',</v>
       </c>
       <c r="B84" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I4, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I4), Sheet1!I4, IF(OR(Sheet1!I4="Null", Sheet1!I4=""), "Null", _xlfn.CONCAT("'", Sheet1!I4, "'"))), ",")</f>
         <v>'Kurztext DE 2',</v>
       </c>
       <c r="C84" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J4, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J4), Sheet1!J4, IF(OR(Sheet1!J4="Null", Sheet1!J4=""), "Null", _xlfn.CONCAT("'", Sheet1!J4, "'"))), ",")</f>
         <v>'Kurztext DE 3',</v>
       </c>
       <c r="D84" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K4, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K4), Sheet1!K4, IF(OR(Sheet1!K4="Null", Sheet1!K4=""), "Null", _xlfn.CONCAT("'", Sheet1!K4, "'"))), ",")</f>
         <v>'asdfasdfasdfasdf',</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A85" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H5, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H5), Sheet1!H5, IF(OR(Sheet1!H5="Null", Sheet1!H5=""), "Null", _xlfn.CONCAT("'", Sheet1!H5, "'"))), ",")</f>
         <v>'Kurztext FR',</v>
       </c>
       <c r="B85" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I5, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I5), Sheet1!I5, IF(OR(Sheet1!I5="Null", Sheet1!I5=""), "Null", _xlfn.CONCAT("'", Sheet1!I5, "'"))), ",")</f>
         <v>'asdfasF',</v>
       </c>
       <c r="C85" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J5, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J5), Sheet1!J5, IF(OR(Sheet1!J5="Null", Sheet1!J5=""), "Null", _xlfn.CONCAT("'", Sheet1!J5, "'"))), ",")</f>
         <v>'rrhqhqF',</v>
       </c>
       <c r="D85" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K5, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K5), Sheet1!K5, IF(OR(Sheet1!K5="Null", Sheet1!K5=""), "Null", _xlfn.CONCAT("'", Sheet1!K5, "'"))), ",")</f>
         <v>'1tqgqdbq',</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A86" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H6, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H6), Sheet1!H6, IF(OR(Sheet1!H6="Null", Sheet1!H6=""), "Null", _xlfn.CONCAT("'", Sheet1!H6, "'"))), ",")</f>
         <v>'Kurztext EN',</v>
       </c>
       <c r="B86" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I6, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I6), Sheet1!I6, IF(OR(Sheet1!I6="Null", Sheet1!I6=""), "Null", _xlfn.CONCAT("'", Sheet1!I6, "'"))), ",")</f>
         <v>'asdfasE',</v>
       </c>
       <c r="C86" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J6, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J6), Sheet1!J6, IF(OR(Sheet1!J6="Null", Sheet1!J6=""), "Null", _xlfn.CONCAT("'", Sheet1!J6, "'"))), ",")</f>
         <v>'rrhqhqE',</v>
       </c>
       <c r="D86" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K6, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K6), Sheet1!K6, IF(OR(Sheet1!K6="Null", Sheet1!K6=""), "Null", _xlfn.CONCAT("'", Sheet1!K6, "'"))), ",")</f>
         <v>'asahasr5t',</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A87" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H7, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H7), Sheet1!H7, IF(OR(Sheet1!H7="Null", Sheet1!H7=""), "Null", _xlfn.CONCAT("'", Sheet1!H7, "'"))), ",")</f>
         <v>'Grunddatentext DE - 1. Zeile',</v>
       </c>
       <c r="B87" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I7, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I7), Sheet1!I7, IF(OR(Sheet1!I7="Null", Sheet1!I7=""), "Null", _xlfn.CONCAT("'", Sheet1!I7, "'"))), ",")</f>
         <v>'Grunddatentext DE - 1. Zeile 2',</v>
       </c>
       <c r="C87" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J7, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J7), Sheet1!J7, IF(OR(Sheet1!J7="Null", Sheet1!J7=""), "Null", _xlfn.CONCAT("'", Sheet1!J7, "'"))), ",")</f>
         <v>'Grunddatentext DE - 1. Zeile 3',</v>
       </c>
       <c r="D87" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K7, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K7), Sheet1!K7, IF(OR(Sheet1!K7="Null", Sheet1!K7=""), "Null", _xlfn.CONCAT("'", Sheet1!K7, "'"))), ",")</f>
         <v>'Grunddatentext DE - 1. Zeile 4',</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A88" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H8, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H8), Sheet1!H8, IF(OR(Sheet1!H8="Null", Sheet1!H8=""), "Null", _xlfn.CONCAT("'", Sheet1!H8, "'"))), ",")</f>
         <v>'Grunddatentext DE - 2. Zeile',</v>
       </c>
       <c r="B88" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I8, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I8), Sheet1!I8, IF(OR(Sheet1!I8="Null", Sheet1!I8=""), "Null", _xlfn.CONCAT("'", Sheet1!I8, "'"))), ",")</f>
         <v>'Grunddatentext DE - 2. Zeile 2',</v>
       </c>
       <c r="C88" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J8, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J8), Sheet1!J8, IF(OR(Sheet1!J8="Null", Sheet1!J8=""), "Null", _xlfn.CONCAT("'", Sheet1!J8, "'"))), ",")</f>
         <v>'Grunddatentext DE - 2. Zeile 3',</v>
       </c>
       <c r="D88" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K8, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K8), Sheet1!K8, IF(OR(Sheet1!K8="Null", Sheet1!K8=""), "Null", _xlfn.CONCAT("'", Sheet1!K8, "'"))), ",")</f>
         <v>'Grunddatentext DE - 2. Zeile 4',</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H9, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H9), Sheet1!H9, IF(OR(Sheet1!H9="Null", Sheet1!H9=""), "Null", _xlfn.CONCAT("'", Sheet1!H9, "'"))), ",")</f>
         <v>'Grunddatentext FR - 1. Zeile',</v>
       </c>
       <c r="B89" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I9, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I9), Sheet1!I9, IF(OR(Sheet1!I9="Null", Sheet1!I9=""), "Null", _xlfn.CONCAT("'", Sheet1!I9, "'"))), ",")</f>
         <v>'Grunddatentext FR - 1. Zeile 2',</v>
       </c>
       <c r="C89" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J9, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J9), Sheet1!J9, IF(OR(Sheet1!J9="Null", Sheet1!J9=""), "Null", _xlfn.CONCAT("'", Sheet1!J9, "'"))), ",")</f>
         <v>'Grunddatentext FR - 1. Zeile 3',</v>
       </c>
       <c r="D89" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K9, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K9), Sheet1!K9, IF(OR(Sheet1!K9="Null", Sheet1!K9=""), "Null", _xlfn.CONCAT("'", Sheet1!K9, "'"))), ",")</f>
         <v>'Grunddatentext FR - 1. Zeile 4',</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A90" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H10, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H10), Sheet1!H10, IF(OR(Sheet1!H10="Null", Sheet1!H10=""), "Null", _xlfn.CONCAT("'", Sheet1!H10, "'"))), ",")</f>
         <v>'Grunddatentext FR - 2. Zeile',</v>
       </c>
       <c r="B90" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I10, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I10), Sheet1!I10, IF(OR(Sheet1!I10="Null", Sheet1!I10=""), "Null", _xlfn.CONCAT("'", Sheet1!I10, "'"))), ",")</f>
         <v>'Grunddatentext FR - 2. Zeile 2',</v>
       </c>
       <c r="C90" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J10, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J10), Sheet1!J10, IF(OR(Sheet1!J10="Null", Sheet1!J10=""), "Null", _xlfn.CONCAT("'", Sheet1!J10, "'"))), ",")</f>
         <v>'Grunddatentext FR - 2. Zeile 3',</v>
       </c>
       <c r="D90" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K10, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K10), Sheet1!K10, IF(OR(Sheet1!K10="Null", Sheet1!K10=""), "Null", _xlfn.CONCAT("'", Sheet1!K10, "'"))), ",")</f>
         <v>'Grunddatentext FR - 2. Zeile 4',</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A91" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H11, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H11), Sheet1!H11, IF(OR(Sheet1!H11="Null", Sheet1!H11=""), "Null", _xlfn.CONCAT("'", Sheet1!H11, "'"))), ",")</f>
         <v>'Grunddatentext EN - 1. Zeile',</v>
       </c>
       <c r="B91" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I11, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I11), Sheet1!I11, IF(OR(Sheet1!I11="Null", Sheet1!I11=""), "Null", _xlfn.CONCAT("'", Sheet1!I11, "'"))), ",")</f>
         <v>'Grunddatentext EN - 1. Zeile 2',</v>
       </c>
       <c r="C91" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J11, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J11), Sheet1!J11, IF(OR(Sheet1!J11="Null", Sheet1!J11=""), "Null", _xlfn.CONCAT("'", Sheet1!J11, "'"))), ",")</f>
         <v>'Grunddatentext EN - 1. Zeile 3',</v>
       </c>
       <c r="D91" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K11, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K11), Sheet1!K11, IF(OR(Sheet1!K11="Null", Sheet1!K11=""), "Null", _xlfn.CONCAT("'", Sheet1!K11, "'"))), ",")</f>
         <v>'Grunddatentext EN - 1. Zeile 4',</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A92" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!H12, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H12), Sheet1!H12, IF(OR(Sheet1!H12="Null", Sheet1!H12=""), "Null", _xlfn.CONCAT("'", Sheet1!H12, "'"))), ",")</f>
         <v>'Grunddatentext EN - 2. Zeile',</v>
       </c>
       <c r="B92" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!I12, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I12), Sheet1!I12, IF(OR(Sheet1!I12="Null", Sheet1!I12=""), "Null", _xlfn.CONCAT("'", Sheet1!I12, "'"))), ",")</f>
         <v>'Grunddatentext EN - 2. Zeile 2',</v>
       </c>
       <c r="C92" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!J12, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J12), Sheet1!J12, IF(OR(Sheet1!J12="Null", Sheet1!J12=""), "Null", _xlfn.CONCAT("'", Sheet1!J12, "'"))), ",")</f>
         <v>'Grunddatentext EN - 2. Zeile 3',</v>
       </c>
       <c r="D92" t="str">
-        <f>_xlfn.CONCAT("'", Sheet1!K12, "',")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K12), Sheet1!K12, IF(OR(Sheet1!K12="Null", Sheet1!K12=""), "Null", _xlfn.CONCAT("'", Sheet1!K12, "'"))), ",")</f>
         <v>'Grunddatentext EN - 2. Zeile 4',</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A93" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H13), Sheet1!H13, IF(Sheet1!H13="Null", "Null", _xlfn.CONCAT("'", Sheet1!H13, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H13), Sheet1!H13, IF(OR(Sheet1!H13="Null", Sheet1!H13=""), "Null", _xlfn.CONCAT("'", Sheet1!H13, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="B93" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I13), Sheet1!I13, IF(Sheet1!I13="Null", "Null", _xlfn.CONCAT("'", Sheet1!I13, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I13), Sheet1!I13, IF(OR(Sheet1!I13="Null", Sheet1!I13=""), "Null", _xlfn.CONCAT("'", Sheet1!I13, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="C93" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J13), Sheet1!J13, IF(Sheet1!J13="Null", "Null", _xlfn.CONCAT("'", Sheet1!J13, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J13), Sheet1!J13, IF(OR(Sheet1!J13="Null", Sheet1!J13=""), "Null", _xlfn.CONCAT("'", Sheet1!J13, "'"))), ",")</f>
         <v>3,</v>
       </c>
       <c r="D93" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K13), Sheet1!K13, IF(Sheet1!K13="Null", "Null", _xlfn.CONCAT("'", Sheet1!K13, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K13), Sheet1!K13, IF(OR(Sheet1!K13="Null", Sheet1!K13=""), "Null", _xlfn.CONCAT("'", Sheet1!K13, "'"))), ",")</f>
         <v>4,</v>
       </c>
-      <c r="F93">
-        <f>IF(ISNUMBER(Sheet1!H13), Sheet1!H13, IF(Sheet1!H13="Null", "Null", _xlfn.CONCAT("'", Sheet1!H13, "'")))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A94" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H14), Sheet1!H14, IF(Sheet1!H14="Null", "Null", _xlfn.CONCAT("'", Sheet1!H14, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H14), Sheet1!H14, IF(OR(Sheet1!H14="Null", Sheet1!H14=""), "Null", _xlfn.CONCAT("'", Sheet1!H14, "'"))), ",")</f>
         <v>12,</v>
       </c>
       <c r="B94" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I14), Sheet1!I14, IF(Sheet1!I14="Null", "Null", _xlfn.CONCAT("'", Sheet1!I14, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I14), Sheet1!I14, IF(OR(Sheet1!I14="Null", Sheet1!I14=""), "Null", _xlfn.CONCAT("'", Sheet1!I14, "'"))), ",")</f>
         <v>22,</v>
       </c>
       <c r="C94" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J14), Sheet1!J14, IF(Sheet1!J14="Null", "Null", _xlfn.CONCAT("'", Sheet1!J14, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J14), Sheet1!J14, IF(OR(Sheet1!J14="Null", Sheet1!J14=""), "Null", _xlfn.CONCAT("'", Sheet1!J14, "'"))), ",")</f>
         <v>32,</v>
       </c>
       <c r="D94" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K14), Sheet1!K14, IF(Sheet1!K14="Null", "Null", _xlfn.CONCAT("'", Sheet1!K14, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K14), Sheet1!K14, IF(OR(Sheet1!K14="Null", Sheet1!K14=""), "Null", _xlfn.CONCAT("'", Sheet1!K14, "'"))), ",")</f>
         <v>42,</v>
       </c>
-      <c r="F94">
-        <f>IF(ISNUMBER(Sheet1!H14), Sheet1!H14, IF(Sheet1!H14="Null", "Null", _xlfn.CONCAT("'", Sheet1!H14, "'")))</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A95" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H15), Sheet1!H15, IF(Sheet1!H15="Null", "Null", _xlfn.CONCAT("'", Sheet1!H15, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H15), Sheet1!H15, IF(OR(Sheet1!H15="Null", Sheet1!H15=""), "Null", _xlfn.CONCAT("'", Sheet1!H15, "'"))), ",")</f>
         <v>23,</v>
       </c>
       <c r="B95" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I15), Sheet1!I15, IF(Sheet1!I15="Null", "Null", _xlfn.CONCAT("'", Sheet1!I15, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I15), Sheet1!I15, IF(OR(Sheet1!I15="Null", Sheet1!I15=""), "Null", _xlfn.CONCAT("'", Sheet1!I15, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="C95" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J15), Sheet1!J15, IF(Sheet1!J15="Null", "Null", _xlfn.CONCAT("'", Sheet1!J15, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J15), Sheet1!J15, IF(OR(Sheet1!J15="Null", Sheet1!J15=""), "Null", _xlfn.CONCAT("'", Sheet1!J15, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="D95" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K15), Sheet1!K15, IF(Sheet1!K15="Null", "Null", _xlfn.CONCAT("'", Sheet1!K15, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F95">
-        <f>IF(ISNUMBER(Sheet1!H15), Sheet1!H15, IF(Sheet1!H15="Null", "Null", _xlfn.CONCAT("'", Sheet1!H15, "'")))</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K15), Sheet1!K15, IF(OR(Sheet1!K15="Null", Sheet1!K15=""), "Null", _xlfn.CONCAT("'", Sheet1!K15, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A96" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H16), Sheet1!H16, IF(Sheet1!H16="Null", "Null", _xlfn.CONCAT("'", Sheet1!H16, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H16), Sheet1!H16, IF(OR(Sheet1!H16="Null", Sheet1!H16=""), "Null", _xlfn.CONCAT("'", Sheet1!H16, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="B96" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I16), Sheet1!I16, IF(Sheet1!I16="Null", "Null", _xlfn.CONCAT("'", Sheet1!I16, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I16), Sheet1!I16, IF(OR(Sheet1!I16="Null", Sheet1!I16=""), "Null", _xlfn.CONCAT("'", Sheet1!I16, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="C96" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J16), Sheet1!J16, IF(Sheet1!J16="Null", "Null", _xlfn.CONCAT("'", Sheet1!J16, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J16), Sheet1!J16, IF(OR(Sheet1!J16="Null", Sheet1!J16=""), "Null", _xlfn.CONCAT("'", Sheet1!J16, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="D96" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K16), Sheet1!K16, IF(Sheet1!K16="Null", "Null", _xlfn.CONCAT("'", Sheet1!K16, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F96" t="str">
-        <f>IF(ISNUMBER(Sheet1!H16), Sheet1!H16, IF(Sheet1!H16="Null", "Null", _xlfn.CONCAT("'", Sheet1!H16, "'")))</f>
-        <v>Null</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K16), Sheet1!K16, IF(OR(Sheet1!K16="Null", Sheet1!K16=""), "Null", _xlfn.CONCAT("'", Sheet1!K16, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H17), Sheet1!H17, IF(Sheet1!H17="Null", "Null", _xlfn.CONCAT("'", Sheet1!H17, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H17), Sheet1!H17, IF(OR(Sheet1!H17="Null", Sheet1!H17=""), "Null", _xlfn.CONCAT("'", Sheet1!H17, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="B97" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I17), Sheet1!I17, IF(Sheet1!I17="Null", "Null", _xlfn.CONCAT("'", Sheet1!I17, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I17), Sheet1!I17, IF(OR(Sheet1!I17="Null", Sheet1!I17=""), "Null", _xlfn.CONCAT("'", Sheet1!I17, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="C97" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J17), Sheet1!J17, IF(Sheet1!J17="Null", "Null", _xlfn.CONCAT("'", Sheet1!J17, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J17), Sheet1!J17, IF(OR(Sheet1!J17="Null", Sheet1!J17=""), "Null", _xlfn.CONCAT("'", Sheet1!J17, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="D97" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K17), Sheet1!K17, IF(Sheet1!K17="Null", "Null", _xlfn.CONCAT("'", Sheet1!K17, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F97" t="str">
-        <f>IF(ISNUMBER(Sheet1!H17), Sheet1!H17, IF(Sheet1!H17="Null", "Null", _xlfn.CONCAT("'", Sheet1!H17, "'")))</f>
-        <v>Null</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K17), Sheet1!K17, IF(OR(Sheet1!K17="Null", Sheet1!K17=""), "Null", _xlfn.CONCAT("'", Sheet1!K17, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H18), Sheet1!H18, IF(Sheet1!H18="Null", "Null", _xlfn.CONCAT("'", Sheet1!H18, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H18), Sheet1!H18, IF(OR(Sheet1!H18="Null", Sheet1!H18=""), "Null", _xlfn.CONCAT("'", Sheet1!H18, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="B98" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I18), Sheet1!I18, IF(Sheet1!I18="Null", "Null", _xlfn.CONCAT("'", Sheet1!I18, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I18), Sheet1!I18, IF(OR(Sheet1!I18="Null", Sheet1!I18=""), "Null", _xlfn.CONCAT("'", Sheet1!I18, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="C98" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J18), Sheet1!J18, IF(Sheet1!J18="Null", "Null", _xlfn.CONCAT("'", Sheet1!J18, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J18), Sheet1!J18, IF(OR(Sheet1!J18="Null", Sheet1!J18=""), "Null", _xlfn.CONCAT("'", Sheet1!J18, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="D98" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K18), Sheet1!K18, IF(Sheet1!K18="Null", "Null", _xlfn.CONCAT("'", Sheet1!K18, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F98" t="str">
-        <f>IF(ISNUMBER(Sheet1!H18), Sheet1!H18, IF(Sheet1!H18="Null", "Null", _xlfn.CONCAT("'", Sheet1!H18, "'")))</f>
-        <v>Null</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K18), Sheet1!K18, IF(OR(Sheet1!K18="Null", Sheet1!K18=""), "Null", _xlfn.CONCAT("'", Sheet1!K18, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H19), Sheet1!H19, IF(Sheet1!H19="Null", "Null", _xlfn.CONCAT("'", Sheet1!H19, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H19), Sheet1!H19, IF(OR(Sheet1!H19="Null", Sheet1!H19=""), "Null", _xlfn.CONCAT("'", Sheet1!H19, "'"))), ",")</f>
         <v>'yann011111111111111',</v>
       </c>
       <c r="B99" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I19), Sheet1!I19, IF(Sheet1!I19="Null", "Null", _xlfn.CONCAT("'", Sheet1!I19, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I19), Sheet1!I19, IF(OR(Sheet1!I19="Null", Sheet1!I19=""), "Null", _xlfn.CONCAT("'", Sheet1!I19, "'"))), ",")</f>
         <v>'yann022222222222222',</v>
       </c>
       <c r="C99" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J19), Sheet1!J19, IF(Sheet1!J19="Null", "Null", _xlfn.CONCAT("'", Sheet1!J19, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J19), Sheet1!J19, IF(OR(Sheet1!J19="Null", Sheet1!J19=""), "Null", _xlfn.CONCAT("'", Sheet1!J19, "'"))), ",")</f>
         <v>'yann033333333333333',</v>
       </c>
       <c r="D99" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K19), Sheet1!K19, IF(Sheet1!K19="Null", "Null", _xlfn.CONCAT("'", Sheet1!K19, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K19), Sheet1!K19, IF(OR(Sheet1!K19="Null", Sheet1!K19=""), "Null", _xlfn.CONCAT("'", Sheet1!K19, "'"))), ",")</f>
         <v>'yann044444444444444',</v>
       </c>
-      <c r="F99" t="str">
-        <f>IF(ISNUMBER(Sheet1!H19), Sheet1!H19, IF(Sheet1!H19="Null", "Null", _xlfn.CONCAT("'", Sheet1!H19, "'")))</f>
-        <v>'yann011111111111111'</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A100" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H20), Sheet1!H20, IF(Sheet1!H20="Null", "Null", _xlfn.CONCAT("'", Sheet1!H20, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H20), Sheet1!H20, IF(OR(Sheet1!H20="Null", Sheet1!H20=""), "Null", _xlfn.CONCAT("'", Sheet1!H20, "'"))), ",")</f>
         <v>'aa',</v>
       </c>
       <c r="B100" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I20), Sheet1!I20, IF(Sheet1!I20="Null", "Null", _xlfn.CONCAT("'", Sheet1!I20, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I20), Sheet1!I20, IF(OR(Sheet1!I20="Null", Sheet1!I20=""), "Null", _xlfn.CONCAT("'", Sheet1!I20, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="C100" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J20), Sheet1!J20, IF(Sheet1!J20="Null", "Null", _xlfn.CONCAT("'", Sheet1!J20, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J20), Sheet1!J20, IF(OR(Sheet1!J20="Null", Sheet1!J20=""), "Null", _xlfn.CONCAT("'", Sheet1!J20, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="D100" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K20), Sheet1!K20, IF(Sheet1!K20="Null", "Null", _xlfn.CONCAT("'", Sheet1!K20, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F100" t="str">
-        <f>IF(ISNUMBER(Sheet1!H20), Sheet1!H20, IF(Sheet1!H20="Null", "Null", _xlfn.CONCAT("'", Sheet1!H20, "'")))</f>
-        <v>'aa'</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K20), Sheet1!K20, IF(OR(Sheet1!K20="Null", Sheet1!K20=""), "Null", _xlfn.CONCAT("'", Sheet1!K20, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A101" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H21), Sheet1!H21, IF(Sheet1!H21="Null", "Null", _xlfn.CONCAT("'", Sheet1!H21, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H21), Sheet1!H21, IF(OR(Sheet1!H21="Null", Sheet1!H21=""), "Null", _xlfn.CONCAT("'", Sheet1!H21, "'"))), ",")</f>
         <v>2,</v>
       </c>
       <c r="B101" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I21), Sheet1!I21, IF(Sheet1!I21="Null", "Null", _xlfn.CONCAT("'", Sheet1!I21, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I21), Sheet1!I21, IF(OR(Sheet1!I21="Null", Sheet1!I21=""), "Null", _xlfn.CONCAT("'", Sheet1!I21, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="C101" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J21), Sheet1!J21, IF(Sheet1!J21="Null", "Null", _xlfn.CONCAT("'", Sheet1!J21, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J21), Sheet1!J21, IF(OR(Sheet1!J21="Null", Sheet1!J21=""), "Null", _xlfn.CONCAT("'", Sheet1!J21, "'"))), ",")</f>
         <v>1,</v>
       </c>
       <c r="D101" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K21), Sheet1!K21, IF(Sheet1!K21="Null", "Null", _xlfn.CONCAT("'", Sheet1!K21, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K21), Sheet1!K21, IF(OR(Sheet1!K21="Null", Sheet1!K21=""), "Null", _xlfn.CONCAT("'", Sheet1!K21, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="F101">
-        <f>IF(ISNUMBER(Sheet1!H21), Sheet1!H21, IF(Sheet1!H21="Null", "Null", _xlfn.CONCAT("'", Sheet1!H21, "'")))</f>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A102" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H22), Sheet1!H22, IF(OR(Sheet1!H22="Null", Sheet1!H22=""), "Null", _xlfn.CONCAT("'", Sheet1!H22, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="B102" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I22), Sheet1!I22, IF(OR(Sheet1!I22="Null", Sheet1!I22=""), "Null", _xlfn.CONCAT("'", Sheet1!I22, "'"))), ",")</f>
+        <v>'f',</v>
+      </c>
+      <c r="C102" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J22), Sheet1!J22, IF(OR(Sheet1!J22="Null", Sheet1!J22=""), "Null", _xlfn.CONCAT("'", Sheet1!J22, "'"))), ",")</f>
+        <v>'f',</v>
+      </c>
+      <c r="D102" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K22), Sheet1!K22, IF(OR(Sheet1!K22="Null", Sheet1!K22=""), "Null", _xlfn.CONCAT("'", Sheet1!K22, "'"))), ",")</f>
+        <v>'f',</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A103" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H23), Sheet1!H23, IF(OR(Sheet1!H23="Null", Sheet1!H23=""), "Null", _xlfn.CONCAT("'", Sheet1!H23, "'"))), ",")</f>
+        <v>'f',</v>
+      </c>
+      <c r="B103" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I23), Sheet1!I23, IF(OR(Sheet1!I23="Null", Sheet1!I23=""), "Null", _xlfn.CONCAT("'", Sheet1!I23, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="C103" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J23), Sheet1!J23, IF(OR(Sheet1!J23="Null", Sheet1!J23=""), "Null", _xlfn.CONCAT("'", Sheet1!J23, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="D103" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K23), Sheet1!K23, IF(OR(Sheet1!K23="Null", Sheet1!K23=""), "Null", _xlfn.CONCAT("'", Sheet1!K23, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A104" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H24), Sheet1!H24, IF(OR(Sheet1!H24="Null", Sheet1!H24=""), "Null", _xlfn.CONCAT("'", Sheet1!H24, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B104" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I24), Sheet1!I24, IF(OR(Sheet1!I24="Null", Sheet1!I24=""), "Null", _xlfn.CONCAT("'", Sheet1!I24, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C104" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J24), Sheet1!J24, IF(OR(Sheet1!J24="Null", Sheet1!J24=""), "Null", _xlfn.CONCAT("'", Sheet1!J24, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D104" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K24), Sheet1!K24, IF(OR(Sheet1!K24="Null", Sheet1!K24=""), "Null", _xlfn.CONCAT("'", Sheet1!K24, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A105" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H25), Sheet1!H25, IF(OR(Sheet1!H25="Null", Sheet1!H25=""), "Null", _xlfn.CONCAT("'", Sheet1!H25, "'"))), ",")</f>
+        <v>11,</v>
+      </c>
+      <c r="B105" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I25), Sheet1!I25, IF(OR(Sheet1!I25="Null", Sheet1!I25=""), "Null", _xlfn.CONCAT("'", Sheet1!I25, "'"))), ",")</f>
+        <v>22,</v>
+      </c>
+      <c r="C105" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J25), Sheet1!J25, IF(OR(Sheet1!J25="Null", Sheet1!J25=""), "Null", _xlfn.CONCAT("'", Sheet1!J25, "'"))), ",")</f>
+        <v>33,</v>
+      </c>
+      <c r="D105" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K25), Sheet1!K25, IF(OR(Sheet1!K25="Null", Sheet1!K25=""), "Null", _xlfn.CONCAT("'", Sheet1!K25, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A106" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H26), Sheet1!H26, IF(OR(Sheet1!H26="Null", Sheet1!H26=""), "Null", _xlfn.CONCAT("'", Sheet1!H26, "'"))), ",")</f>
+        <v>111,</v>
+      </c>
+      <c r="B106" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I26), Sheet1!I26, IF(OR(Sheet1!I26="Null", Sheet1!I26=""), "Null", _xlfn.CONCAT("'", Sheet1!I26, "'"))), ",")</f>
+        <v>222,</v>
+      </c>
+      <c r="C106" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J26), Sheet1!J26, IF(OR(Sheet1!J26="Null", Sheet1!J26=""), "Null", _xlfn.CONCAT("'", Sheet1!J26, "'"))), ",")</f>
+        <v>333,</v>
+      </c>
+      <c r="D106" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K26), Sheet1!K26, IF(OR(Sheet1!K26="Null", Sheet1!K26=""), "Null", _xlfn.CONCAT("'", Sheet1!K26, "'"))), ",")</f>
+        <v>444,</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A107" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H27), Sheet1!H27, IF(OR(Sheet1!H27="Null", Sheet1!H27=""), "Null", _xlfn.CONCAT("'", Sheet1!H27, "'"))), ",")</f>
+        <v>55,</v>
+      </c>
+      <c r="B107" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I27), Sheet1!I27, IF(OR(Sheet1!I27="Null", Sheet1!I27=""), "Null", _xlfn.CONCAT("'", Sheet1!I27, "'"))), ",")</f>
+        <v>66,</v>
+      </c>
+      <c r="C107" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J27), Sheet1!J27, IF(OR(Sheet1!J27="Null", Sheet1!J27=""), "Null", _xlfn.CONCAT("'", Sheet1!J27, "'"))), ",")</f>
+        <v>77,</v>
+      </c>
+      <c r="D107" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K27), Sheet1!K27, IF(OR(Sheet1!K27="Null", Sheet1!K27=""), "Null", _xlfn.CONCAT("'", Sheet1!K27, "'"))), ",")</f>
+        <v>88,</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A108" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H28), Sheet1!H28, IF(OR(Sheet1!H28="Null", Sheet1!H28=""), "Null", _xlfn.CONCAT("'", Sheet1!H28, "'"))), ",")</f>
+        <v>44,</v>
+      </c>
+      <c r="B108" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I28), Sheet1!I28, IF(OR(Sheet1!I28="Null", Sheet1!I28=""), "Null", _xlfn.CONCAT("'", Sheet1!I28, "'"))), ",")</f>
+        <v>987,</v>
+      </c>
+      <c r="C108" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J28), Sheet1!J28, IF(OR(Sheet1!J28="Null", Sheet1!J28=""), "Null", _xlfn.CONCAT("'", Sheet1!J28, "'"))), ",")</f>
+        <v>12,</v>
+      </c>
+      <c r="D108" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K28), Sheet1!K28, IF(OR(Sheet1!K28="Null", Sheet1!K28=""), "Null", _xlfn.CONCAT("'", Sheet1!K28, "'"))), ",")</f>
+        <v>15,</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A109" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H29), Sheet1!H29, IF(OR(Sheet1!H29="Null", Sheet1!H29=""), "Null", _xlfn.CONCAT("'", Sheet1!H29, "'"))), ",")</f>
+        <v>33,</v>
+      </c>
+      <c r="B109" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I29), Sheet1!I29, IF(OR(Sheet1!I29="Null", Sheet1!I29=""), "Null", _xlfn.CONCAT("'", Sheet1!I29, "'"))), ",")</f>
+        <v>232,</v>
+      </c>
+      <c r="C109" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J29), Sheet1!J29, IF(OR(Sheet1!J29="Null", Sheet1!J29=""), "Null", _xlfn.CONCAT("'", Sheet1!J29, "'"))), ",")</f>
+        <v>253,</v>
+      </c>
+      <c r="D109" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K29), Sheet1!K29, IF(OR(Sheet1!K29="Null", Sheet1!K29=""), "Null", _xlfn.CONCAT("'", Sheet1!K29, "'"))), ",")</f>
+        <v>75,</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A110" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H30), Sheet1!H30, IF(OR(Sheet1!H30="Null", Sheet1!H30=""), "Null", _xlfn.CONCAT("'", Sheet1!H30, "'"))), ",")</f>
+        <v>22,</v>
+      </c>
+      <c r="B110" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I30), Sheet1!I30, IF(OR(Sheet1!I30="Null", Sheet1!I30=""), "Null", _xlfn.CONCAT("'", Sheet1!I30, "'"))), ",")</f>
+        <v>253,</v>
+      </c>
+      <c r="C110" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J30), Sheet1!J30, IF(OR(Sheet1!J30="Null", Sheet1!J30=""), "Null", _xlfn.CONCAT("'", Sheet1!J30, "'"))), ",")</f>
+        <v>1000,</v>
+      </c>
+      <c r="D110" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K30), Sheet1!K30, IF(OR(Sheet1!K30="Null", Sheet1!K30=""), "Null", _xlfn.CONCAT("'", Sheet1!K30, "'"))), ",")</f>
+        <v>65,</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A111" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H31), Sheet1!H31, IF(OR(Sheet1!H31="Null", Sheet1!H31=""), "Null", _xlfn.CONCAT("'", Sheet1!H31, "'"))), ",")</f>
+        <v>50,</v>
+      </c>
+      <c r="B111" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I31), Sheet1!I31, IF(OR(Sheet1!I31="Null", Sheet1!I31=""), "Null", _xlfn.CONCAT("'", Sheet1!I31, "'"))), ",")</f>
+        <v>23,</v>
+      </c>
+      <c r="C111" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J31), Sheet1!J31, IF(OR(Sheet1!J31="Null", Sheet1!J31=""), "Null", _xlfn.CONCAT("'", Sheet1!J31, "'"))), ",")</f>
+        <v>465,</v>
+      </c>
+      <c r="D111" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K31), Sheet1!K31, IF(OR(Sheet1!K31="Null", Sheet1!K31=""), "Null", _xlfn.CONCAT("'", Sheet1!K31, "'"))), ",")</f>
+        <v>50,</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A112" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H32), Sheet1!H32, IF(OR(Sheet1!H32="Null", Sheet1!H32=""), "Null", _xlfn.CONCAT("'", Sheet1!H32, "'"))), ",")</f>
+        <v>100,</v>
+      </c>
+      <c r="B112" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I32), Sheet1!I32, IF(OR(Sheet1!I32="Null", Sheet1!I32=""), "Null", _xlfn.CONCAT("'", Sheet1!I32, "'"))), ",")</f>
+        <v>55,</v>
+      </c>
+      <c r="C112" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J32), Sheet1!J32, IF(OR(Sheet1!J32="Null", Sheet1!J32=""), "Null", _xlfn.CONCAT("'", Sheet1!J32, "'"))), ",")</f>
+        <v>313,</v>
+      </c>
+      <c r="D112" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K32), Sheet1!K32, IF(OR(Sheet1!K32="Null", Sheet1!K32=""), "Null", _xlfn.CONCAT("'", Sheet1!K32, "'"))), ",")</f>
+        <v>987,</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A113" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H33), Sheet1!H33, IF(OR(Sheet1!H33="Null", Sheet1!H33=""), "Null", _xlfn.CONCAT("'", Sheet1!H33, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="B113" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I33), Sheet1!I33, IF(OR(Sheet1!I33="Null", Sheet1!I33=""), "Null", _xlfn.CONCAT("'", Sheet1!I33, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C113" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J33), Sheet1!J33, IF(OR(Sheet1!J33="Null", Sheet1!J33=""), "Null", _xlfn.CONCAT("'", Sheet1!J33, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D113" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K33), Sheet1!K33, IF(OR(Sheet1!K33="Null", Sheet1!K33=""), "Null", _xlfn.CONCAT("'", Sheet1!K33, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A114" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H34), Sheet1!H34, IF(OR(Sheet1!H34="Null", Sheet1!H34=""), "Null", _xlfn.CONCAT("'", Sheet1!H34, "'"))), ",")</f>
+        <v>'D9182',</v>
+      </c>
+      <c r="B114" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I34), Sheet1!I34, IF(OR(Sheet1!I34="Null", Sheet1!I34=""), "Null", _xlfn.CONCAT("'", Sheet1!I34, "'"))), ",")</f>
+        <v>'KCX07',</v>
+      </c>
+      <c r="C114" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J34), Sheet1!J34, IF(OR(Sheet1!J34="Null", Sheet1!J34=""), "Null", _xlfn.CONCAT("'", Sheet1!J34, "'"))), ",")</f>
+        <v>'DD901',</v>
+      </c>
+      <c r="D114" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K34), Sheet1!K34, IF(OR(Sheet1!K34="Null", Sheet1!K34=""), "Null", _xlfn.CONCAT("'", Sheet1!K34, "'"))), ",")</f>
+        <v>'1NQ67',</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A115" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H35), Sheet1!H35, IF(OR(Sheet1!H35="Null", Sheet1!H35=""), "Null", _xlfn.CONCAT("'", Sheet1!H35, "'"))), ",")</f>
+        <v>'MOWAG',</v>
+      </c>
+      <c r="B115" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I35), Sheet1!I35, IF(OR(Sheet1!I35="Null", Sheet1!I35=""), "Null", _xlfn.CONCAT("'", Sheet1!I35, "'"))), ",")</f>
+        <v>'asdfas',</v>
+      </c>
+      <c r="C115" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J35), Sheet1!J35, IF(OR(Sheet1!J35="Null", Sheet1!J35=""), "Null", _xlfn.CONCAT("'", Sheet1!J35, "'"))), ",")</f>
+        <v>'Apple',</v>
+      </c>
+      <c r="D115" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K35), Sheet1!K35, IF(OR(Sheet1!K35="Null", Sheet1!K35=""), "Null", _xlfn.CONCAT("'", Sheet1!K35, "'"))), ",")</f>
+        <v>'Samsung',</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A116" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H36), Sheet1!H36, IF(OR(Sheet1!H36="Null", Sheet1!H36=""), "Null", _xlfn.CONCAT("'", Sheet1!H36, "'"))), ",")</f>
+        <v>'Bernstrasse 1',</v>
+      </c>
+      <c r="B116" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I36), Sheet1!I36, IF(OR(Sheet1!I36="Null", Sheet1!I36=""), "Null", _xlfn.CONCAT("'", Sheet1!I36, "'"))), ",")</f>
+        <v>'Rte du Lac 12',</v>
+      </c>
+      <c r="C116" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J36), Sheet1!J36, IF(OR(Sheet1!J36="Null", Sheet1!J36=""), "Null", _xlfn.CONCAT("'", Sheet1!J36, "'"))), ",")</f>
+        <v>'One Apple Park Way',</v>
+      </c>
+      <c r="D116" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K36), Sheet1!K36, IF(OR(Sheet1!K36="Null", Sheet1!K36=""), "Null", _xlfn.CONCAT("'", Sheet1!K36, "'"))), ",")</f>
+        <v>'Against Apple Way',</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A117" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H37), Sheet1!H37, IF(OR(Sheet1!H37="Null", Sheet1!H37=""), "Null", _xlfn.CONCAT("'", Sheet1!H37, "'"))), ",")</f>
+        <v>2000,</v>
+      </c>
+      <c r="B117" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I37), Sheet1!I37, IF(OR(Sheet1!I37="Null", Sheet1!I37=""), "Null", _xlfn.CONCAT("'", Sheet1!I37, "'"))), ",")</f>
+        <v>1215,</v>
+      </c>
+      <c r="C117" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J37), Sheet1!J37, IF(OR(Sheet1!J37="Null", Sheet1!J37=""), "Null", _xlfn.CONCAT("'", Sheet1!J37, "'"))), ",")</f>
+        <v>95014,</v>
+      </c>
+      <c r="D117" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K37), Sheet1!K37, IF(OR(Sheet1!K37="Null", Sheet1!K37=""), "Null", _xlfn.CONCAT("'", Sheet1!K37, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A118" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H38), Sheet1!H38, IF(OR(Sheet1!H38="Null", Sheet1!H38=""), "Null", _xlfn.CONCAT("'", Sheet1!H38, "'"))), ",")</f>
+        <v>'Neuchâtel',</v>
+      </c>
+      <c r="B118" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I38), Sheet1!I38, IF(OR(Sheet1!I38="Null", Sheet1!I38=""), "Null", _xlfn.CONCAT("'", Sheet1!I38, "'"))), ",")</f>
+        <v>'Genère',</v>
+      </c>
+      <c r="C118" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J38), Sheet1!J38, IF(OR(Sheet1!J38="Null", Sheet1!J38=""), "Null", _xlfn.CONCAT("'", Sheet1!J38, "'"))), ",")</f>
+        <v>'Cupertino',</v>
+      </c>
+      <c r="D118" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K38), Sheet1!K38, IF(OR(Sheet1!K38="Null", Sheet1!K38=""), "Null", _xlfn.CONCAT("'", Sheet1!K38, "'"))), ",")</f>
+        <v>'Seoul',</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A119" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H39), Sheet1!H39, IF(OR(Sheet1!H39="Null", Sheet1!H39=""), "Null", _xlfn.CONCAT("'", Sheet1!H39, "'"))), ",")</f>
+        <v>'1.1',</v>
+      </c>
+      <c r="B119" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I39), Sheet1!I39, IF(OR(Sheet1!I39="Null", Sheet1!I39=""), "Null", _xlfn.CONCAT("'", Sheet1!I39, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C119" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J39), Sheet1!J39, IF(OR(Sheet1!J39="Null", Sheet1!J39=""), "Null", _xlfn.CONCAT("'", Sheet1!J39, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D119" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K39), Sheet1!K39, IF(OR(Sheet1!K39="Null", Sheet1!K39=""), "Null", _xlfn.CONCAT("'", Sheet1!K39, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A120" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H40), Sheet1!H40, IF(OR(Sheet1!H40="Null", Sheet1!H40=""), "Null", _xlfn.CONCAT("'", Sheet1!H40, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B120" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I40), Sheet1!I40, IF(OR(Sheet1!I40="Null", Sheet1!I40=""), "Null", _xlfn.CONCAT("'", Sheet1!I40, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C120" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J40), Sheet1!J40, IF(OR(Sheet1!J40="Null", Sheet1!J40=""), "Null", _xlfn.CONCAT("'", Sheet1!J40, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D120" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K40), Sheet1!K40, IF(OR(Sheet1!K40="Null", Sheet1!K40=""), "Null", _xlfn.CONCAT("'", Sheet1!K40, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A121" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H41), Sheet1!H41, IF(OR(Sheet1!H41="Null", Sheet1!H41=""), "Null", _xlfn.CONCAT("'", Sheet1!H41, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+      <c r="B121" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I41), Sheet1!I41, IF(OR(Sheet1!I41="Null", Sheet1!I41=""), "Null", _xlfn.CONCAT("'", Sheet1!I41, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+      <c r="C121" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J41), Sheet1!J41, IF(OR(Sheet1!J41="Null", Sheet1!J41=""), "Null", _xlfn.CONCAT("'", Sheet1!J41, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="D121" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K41), Sheet1!K41, IF(OR(Sheet1!K41="Null", Sheet1!K41=""), "Null", _xlfn.CONCAT("'", Sheet1!K41, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A122" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H42), Sheet1!H42, IF(OR(Sheet1!H42="Null", Sheet1!H42=""), "Null", _xlfn.CONCAT("'", Sheet1!H42, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="B122" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I42), Sheet1!I42, IF(OR(Sheet1!I42="Null", Sheet1!I42=""), "Null", _xlfn.CONCAT("'", Sheet1!I42, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="C122" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J42), Sheet1!J42, IF(OR(Sheet1!J42="Null", Sheet1!J42=""), "Null", _xlfn.CONCAT("'", Sheet1!J42, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="D122" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K42), Sheet1!K42, IF(OR(Sheet1!K42="Null", Sheet1!K42=""), "Null", _xlfn.CONCAT("'", Sheet1!K42, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A123" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H43), Sheet1!H43, IF(OR(Sheet1!H43="Null", Sheet1!H43=""), "Null", _xlfn.CONCAT("'", Sheet1!H43, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="B123" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I43), Sheet1!I43, IF(OR(Sheet1!I43="Null", Sheet1!I43=""), "Null", _xlfn.CONCAT("'", Sheet1!I43, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="C123" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J43), Sheet1!J43, IF(OR(Sheet1!J43="Null", Sheet1!J43=""), "Null", _xlfn.CONCAT("'", Sheet1!J43, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="D123" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K43), Sheet1!K43, IF(OR(Sheet1!K43="Null", Sheet1!K43=""), "Null", _xlfn.CONCAT("'", Sheet1!K43, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A124" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H44), Sheet1!H44, IF(OR(Sheet1!H44="Null", Sheet1!H44=""), "Null", _xlfn.CONCAT("'", Sheet1!H44, "'"))), ",")</f>
+        <v>'0022',</v>
+      </c>
+      <c r="B124" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I44), Sheet1!I44, IF(OR(Sheet1!I44="Null", Sheet1!I44=""), "Null", _xlfn.CONCAT("'", Sheet1!I44, "'"))), ",")</f>
+        <v>'0045',</v>
+      </c>
+      <c r="C124" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J44), Sheet1!J44, IF(OR(Sheet1!J44="Null", Sheet1!J44=""), "Null", _xlfn.CONCAT("'", Sheet1!J44, "'"))), ",")</f>
+        <v>'0001',</v>
+      </c>
+      <c r="D124" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K44), Sheet1!K44, IF(OR(Sheet1!K44="Null", Sheet1!K44=""), "Null", _xlfn.CONCAT("'", Sheet1!K44, "'"))), ",")</f>
+        <v>'0496',</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A125" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H45), Sheet1!H45, IF(OR(Sheet1!H45="Null", Sheet1!H45=""), "Null", _xlfn.CONCAT("'", Sheet1!H45, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B125" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I45), Sheet1!I45, IF(OR(Sheet1!I45="Null", Sheet1!I45=""), "Null", _xlfn.CONCAT("'", Sheet1!I45, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C125" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J45), Sheet1!J45, IF(OR(Sheet1!J45="Null", Sheet1!J45=""), "Null", _xlfn.CONCAT("'", Sheet1!J45, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D125" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K45), Sheet1!K45, IF(OR(Sheet1!K45="Null", Sheet1!K45=""), "Null", _xlfn.CONCAT("'", Sheet1!K45, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A126" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H46), Sheet1!H46, IF(OR(Sheet1!H46="Null", Sheet1!H46=""), "Null", _xlfn.CONCAT("'", Sheet1!H46, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="B126" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I46), Sheet1!I46, IF(OR(Sheet1!I46="Null", Sheet1!I46=""), "Null", _xlfn.CONCAT("'", Sheet1!I46, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="C126" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J46), Sheet1!J46, IF(OR(Sheet1!J46="Null", Sheet1!J46=""), "Null", _xlfn.CONCAT("'", Sheet1!J46, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="D126" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K46), Sheet1!K46, IF(OR(Sheet1!K46="Null", Sheet1!K46=""), "Null", _xlfn.CONCAT("'", Sheet1!K46, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A127" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H47), Sheet1!H47, IF(OR(Sheet1!H47="Null", Sheet1!H47=""), "Null", _xlfn.CONCAT("'", Sheet1!H47, "'"))), ",")</f>
+        <v>'1000051294',</v>
+      </c>
+      <c r="B127" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I47), Sheet1!I47, IF(OR(Sheet1!I47="Null", Sheet1!I47=""), "Null", _xlfn.CONCAT("'", Sheet1!I47, "'"))), ",")</f>
+        <v>'1000058908',</v>
+      </c>
+      <c r="C127" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J47), Sheet1!J47, IF(OR(Sheet1!J47="Null", Sheet1!J47=""), "Null", _xlfn.CONCAT("'", Sheet1!J47, "'"))), ",")</f>
+        <v>'1000057308',</v>
+      </c>
+      <c r="D127" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K47), Sheet1!K47, IF(OR(Sheet1!K47="Null", Sheet1!K47=""), "Null", _xlfn.CONCAT("'", Sheet1!K47, "'"))), ",")</f>
+        <v>'1000053644',</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A128" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H48), Sheet1!H48, IF(OR(Sheet1!H48="Null", Sheet1!H48=""), "Null", _xlfn.CONCAT("'", Sheet1!H48, "'"))), ",")</f>
+        <v>'ZX0000040',</v>
+      </c>
+      <c r="B128" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I48), Sheet1!I48, IF(OR(Sheet1!I48="Null", Sheet1!I48=""), "Null", _xlfn.CONCAT("'", Sheet1!I48, "'"))), ",")</f>
+        <v>'ZX0000040',</v>
+      </c>
+      <c r="C128" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J48), Sheet1!J48, IF(OR(Sheet1!J48="Null", Sheet1!J48=""), "Null", _xlfn.CONCAT("'", Sheet1!J48, "'"))), ",")</f>
+        <v>'ZX0000040',</v>
+      </c>
+      <c r="D128" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K48), Sheet1!K48, IF(OR(Sheet1!K48="Null", Sheet1!K48=""), "Null", _xlfn.CONCAT("'", Sheet1!K48, "'"))), ",")</f>
+        <v>'ZX0000040',</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A129" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H49), Sheet1!H49, IF(OR(Sheet1!H49="Null", Sheet1!H49=""), "Null", _xlfn.CONCAT("'", Sheet1!H49, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+      <c r="B129" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I49), Sheet1!I49, IF(OR(Sheet1!I49="Null", Sheet1!I49=""), "Null", _xlfn.CONCAT("'", Sheet1!I49, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="C129" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J49), Sheet1!J49, IF(OR(Sheet1!J49="Null", Sheet1!J49=""), "Null", _xlfn.CONCAT("'", Sheet1!J49, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="D129" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K49), Sheet1!K49, IF(OR(Sheet1!K49="Null", Sheet1!K49=""), "Null", _xlfn.CONCAT("'", Sheet1!K49, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A130" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H50), Sheet1!H50, IF(OR(Sheet1!H50="Null", Sheet1!H50=""), "Null", _xlfn.CONCAT("'", Sheet1!H50, "'"))), ",")</f>
+        <v>'abcde',</v>
+      </c>
+      <c r="B130" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I50), Sheet1!I50, IF(OR(Sheet1!I50="Null", Sheet1!I50=""), "Null", _xlfn.CONCAT("'", Sheet1!I50, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C130" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J50), Sheet1!J50, IF(OR(Sheet1!J50="Null", Sheet1!J50=""), "Null", _xlfn.CONCAT("'", Sheet1!J50, "'"))), ",")</f>
+        <v>54321,</v>
+      </c>
+      <c r="D130" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K50), Sheet1!K50, IF(OR(Sheet1!K50="Null", Sheet1!K50=""), "Null", _xlfn.CONCAT("'", Sheet1!K50, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A131" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H51), Sheet1!H51, IF(OR(Sheet1!H51="Null", Sheet1!H51=""), "Null", _xlfn.CONCAT("'", Sheet1!H51, "'"))), ",")</f>
+        <v>'.1',</v>
+      </c>
+      <c r="B131" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I51), Sheet1!I51, IF(OR(Sheet1!I51="Null", Sheet1!I51=""), "Null", _xlfn.CONCAT("'", Sheet1!I51, "'"))), ",")</f>
+        <v>'0000',</v>
+      </c>
+      <c r="C131" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J51), Sheet1!J51, IF(OR(Sheet1!J51="Null", Sheet1!J51=""), "Null", _xlfn.CONCAT("'", Sheet1!J51, "'"))), ",")</f>
+        <v>1.01,</v>
+      </c>
+      <c r="D131" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K51), Sheet1!K51, IF(OR(Sheet1!K51="Null", Sheet1!K51=""), "Null", _xlfn.CONCAT("'", Sheet1!K51, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A132" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H52), Sheet1!H52, IF(OR(Sheet1!H52="Null", Sheet1!H52=""), "Null", _xlfn.CONCAT("'", Sheet1!H52, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="B132" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I52), Sheet1!I52, IF(OR(Sheet1!I52="Null", Sheet1!I52=""), "Null", _xlfn.CONCAT("'", Sheet1!I52, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C132" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J52), Sheet1!J52, IF(OR(Sheet1!J52="Null", Sheet1!J52=""), "Null", _xlfn.CONCAT("'", Sheet1!J52, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="D132" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K52), Sheet1!K52, IF(OR(Sheet1!K52="Null", Sheet1!K52=""), "Null", _xlfn.CONCAT("'", Sheet1!K52, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A133" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H53), Sheet1!H53, IF(OR(Sheet1!H53="Null", Sheet1!H53=""), "Null", _xlfn.CONCAT("'", Sheet1!H53, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B133" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I53), Sheet1!I53, IF(OR(Sheet1!I53="Null", Sheet1!I53=""), "Null", _xlfn.CONCAT("'", Sheet1!I53, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C133" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J53), Sheet1!J53, IF(OR(Sheet1!J53="Null", Sheet1!J53=""), "Null", _xlfn.CONCAT("'", Sheet1!J53, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D133" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K53), Sheet1!K53, IF(OR(Sheet1!K53="Null", Sheet1!K53=""), "Null", _xlfn.CONCAT("'", Sheet1!K53, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A134" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H54), Sheet1!H54, IF(OR(Sheet1!H54="Null", Sheet1!H54=""), "Null", _xlfn.CONCAT("'", Sheet1!H54, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="B134" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I54), Sheet1!I54, IF(OR(Sheet1!I54="Null", Sheet1!I54=""), "Null", _xlfn.CONCAT("'", Sheet1!I54, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="C134" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J54), Sheet1!J54, IF(OR(Sheet1!J54="Null", Sheet1!J54=""), "Null", _xlfn.CONCAT("'", Sheet1!J54, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D134" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K54), Sheet1!K54, IF(OR(Sheet1!K54="Null", Sheet1!K54=""), "Null", _xlfn.CONCAT("'", Sheet1!K54, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A135" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H55), Sheet1!H55, IF(OR(Sheet1!H55="Null", Sheet1!H55=""), "Null", _xlfn.CONCAT("'", Sheet1!H55, "'"))), ",")</f>
+        <v>'f',</v>
+      </c>
+      <c r="B135" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I55), Sheet1!I55, IF(OR(Sheet1!I55="Null", Sheet1!I55=""), "Null", _xlfn.CONCAT("'", Sheet1!I55, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="C135" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J55), Sheet1!J55, IF(OR(Sheet1!J55="Null", Sheet1!J55=""), "Null", _xlfn.CONCAT("'", Sheet1!J55, "'"))), ",")</f>
+        <v>'f',</v>
+      </c>
+      <c r="D135" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K55), Sheet1!K55, IF(OR(Sheet1!K55="Null", Sheet1!K55=""), "Null", _xlfn.CONCAT("'", Sheet1!K55, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A136" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H56), Sheet1!H56, IF(OR(Sheet1!H56="Null", Sheet1!H56=""), "Null", _xlfn.CONCAT("'", Sheet1!H56, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+      <c r="B136" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I56), Sheet1!I56, IF(OR(Sheet1!I56="Null", Sheet1!I56=""), "Null", _xlfn.CONCAT("'", Sheet1!I56, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+      <c r="C136" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J56), Sheet1!J56, IF(OR(Sheet1!J56="Null", Sheet1!J56=""), "Null", _xlfn.CONCAT("'", Sheet1!J56, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+      <c r="D136" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K56), Sheet1!K56, IF(OR(Sheet1!K56="Null", Sheet1!K56=""), "Null", _xlfn.CONCAT("'", Sheet1!K56, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A137" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H57), Sheet1!H57, IF(OR(Sheet1!H57="Null", Sheet1!H57=""), "Null", _xlfn.CONCAT("'", Sheet1!H57, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="B137" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I57), Sheet1!I57, IF(OR(Sheet1!I57="Null", Sheet1!I57=""), "Null", _xlfn.CONCAT("'", Sheet1!I57, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="C137" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J57), Sheet1!J57, IF(OR(Sheet1!J57="Null", Sheet1!J57=""), "Null", _xlfn.CONCAT("'", Sheet1!J57, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="D137" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K57), Sheet1!K57, IF(OR(Sheet1!K57="Null", Sheet1!K57=""), "Null", _xlfn.CONCAT("'", Sheet1!K57, "'"))), ",")</f>
+        <v>4,</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A138" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H58), Sheet1!H58, IF(OR(Sheet1!H58="Null", Sheet1!H58=""), "Null", _xlfn.CONCAT("'", Sheet1!H58, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B138" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I58), Sheet1!I58, IF(OR(Sheet1!I58="Null", Sheet1!I58=""), "Null", _xlfn.CONCAT("'", Sheet1!I58, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C138" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J58), Sheet1!J58, IF(OR(Sheet1!J58="Null", Sheet1!J58=""), "Null", _xlfn.CONCAT("'", Sheet1!J58, "'"))), ",")</f>
+        <v>4,</v>
+      </c>
+      <c r="D138" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K58), Sheet1!K58, IF(OR(Sheet1!K58="Null", Sheet1!K58=""), "Null", _xlfn.CONCAT("'", Sheet1!K58, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A139" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H59), Sheet1!H59, IF(OR(Sheet1!H59="Null", Sheet1!H59=""), "Null", _xlfn.CONCAT("'", Sheet1!H59, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B139" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I59), Sheet1!I59, IF(OR(Sheet1!I59="Null", Sheet1!I59=""), "Null", _xlfn.CONCAT("'", Sheet1!I59, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C139" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J59), Sheet1!J59, IF(OR(Sheet1!J59="Null", Sheet1!J59=""), "Null", _xlfn.CONCAT("'", Sheet1!J59, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D139" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K59), Sheet1!K59, IF(OR(Sheet1!K59="Null", Sheet1!K59=""), "Null", _xlfn.CONCAT("'", Sheet1!K59, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A140" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H60), Sheet1!H60, IF(OR(Sheet1!H60="Null", Sheet1!H60=""), "Null", _xlfn.CONCAT("'", Sheet1!H60, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="B140" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I60), Sheet1!I60, IF(OR(Sheet1!I60="Null", Sheet1!I60=""), "Null", _xlfn.CONCAT("'", Sheet1!I60, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="C140" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J60), Sheet1!J60, IF(OR(Sheet1!J60="Null", Sheet1!J60=""), "Null", _xlfn.CONCAT("'", Sheet1!J60, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="D140" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K60), Sheet1!K60, IF(OR(Sheet1!K60="Null", Sheet1!K60=""), "Null", _xlfn.CONCAT("'", Sheet1!K60, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A141" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H61), Sheet1!H61, IF(OR(Sheet1!H61="Null", Sheet1!H61=""), "Null", _xlfn.CONCAT("'", Sheet1!H61, "'"))), ",")</f>
+        <v>35,</v>
+      </c>
+      <c r="B141" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I61), Sheet1!I61, IF(OR(Sheet1!I61="Null", Sheet1!I61=""), "Null", _xlfn.CONCAT("'", Sheet1!I61, "'"))), ",")</f>
+        <v>35,</v>
+      </c>
+      <c r="C141" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J61), Sheet1!J61, IF(OR(Sheet1!J61="Null", Sheet1!J61=""), "Null", _xlfn.CONCAT("'", Sheet1!J61, "'"))), ",")</f>
+        <v>35,</v>
+      </c>
+      <c r="D141" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K61), Sheet1!K61, IF(OR(Sheet1!K61="Null", Sheet1!K61=""), "Null", _xlfn.CONCAT("'", Sheet1!K61, "'"))), ",")</f>
+        <v>35,</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A142" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H62), Sheet1!H62, IF(OR(Sheet1!H62="Null", Sheet1!H62=""), "Null", _xlfn.CONCAT("'", Sheet1!H62, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B142" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I62), Sheet1!I62, IF(OR(Sheet1!I62="Null", Sheet1!I62=""), "Null", _xlfn.CONCAT("'", Sheet1!I62, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C142" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J62), Sheet1!J62, IF(OR(Sheet1!J62="Null", Sheet1!J62=""), "Null", _xlfn.CONCAT("'", Sheet1!J62, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D142" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K62), Sheet1!K62, IF(OR(Sheet1!K62="Null", Sheet1!K62=""), "Null", _xlfn.CONCAT("'", Sheet1!K62, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A143" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H63), Sheet1!H63, IF(OR(Sheet1!H63="Null", Sheet1!H63=""), "Null", _xlfn.CONCAT("'", Sheet1!H63, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="B143" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I63), Sheet1!I63, IF(OR(Sheet1!I63="Null", Sheet1!I63=""), "Null", _xlfn.CONCAT("'", Sheet1!I63, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="C143" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J63), Sheet1!J63, IF(OR(Sheet1!J63="Null", Sheet1!J63=""), "Null", _xlfn.CONCAT("'", Sheet1!J63, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+      <c r="D143" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K63), Sheet1!K63, IF(OR(Sheet1!K63="Null", Sheet1!K63=""), "Null", _xlfn.CONCAT("'", Sheet1!K63, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A144" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H64), Sheet1!H64, IF(OR(Sheet1!H64="Null", Sheet1!H64=""), "Null", _xlfn.CONCAT("'", Sheet1!H64, "'"))), ",")</f>
+        <v>'09211600-7',</v>
+      </c>
+      <c r="B144" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I64), Sheet1!I64, IF(OR(Sheet1!I64="Null", Sheet1!I64=""), "Null", _xlfn.CONCAT("'", Sheet1!I64, "'"))), ",")</f>
+        <v>'09221000-4',</v>
+      </c>
+      <c r="C144" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J64), Sheet1!J64, IF(OR(Sheet1!J64="Null", Sheet1!J64=""), "Null", _xlfn.CONCAT("'", Sheet1!J64, "'"))), ",")</f>
+        <v>'09221400-8',</v>
+      </c>
+      <c r="D144" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K64), Sheet1!K64, IF(OR(Sheet1!K64="Null", Sheet1!K64=""), "Null", _xlfn.CONCAT("'", Sheet1!K64, "'"))), ",")</f>
+        <v>'09230000-0',</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A145" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H65), Sheet1!H65, IF(OR(Sheet1!H65="Null", Sheet1!H65=""), "Null", _xlfn.CONCAT("'", Sheet1!H65, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="B145" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I65), Sheet1!I65, IF(OR(Sheet1!I65="Null", Sheet1!I65=""), "Null", _xlfn.CONCAT("'", Sheet1!I65, "'"))), ",")</f>
+        <v>4,</v>
+      </c>
+      <c r="C145" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J65), Sheet1!J65, IF(OR(Sheet1!J65="Null", Sheet1!J65=""), "Null", _xlfn.CONCAT("'", Sheet1!J65, "'"))), ",")</f>
+        <v>4,</v>
+      </c>
+      <c r="D145" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K65), Sheet1!K65, IF(OR(Sheet1!K65="Null", Sheet1!K65=""), "Null", _xlfn.CONCAT("'", Sheet1!K65, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A146" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H66), Sheet1!H66, IF(OR(Sheet1!H66="Null", Sheet1!H66=""), "Null", _xlfn.CONCAT("'", Sheet1!H66, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B146" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I66), Sheet1!I66, IF(OR(Sheet1!I66="Null", Sheet1!I66=""), "Null", _xlfn.CONCAT("'", Sheet1!I66, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="C146" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J66), Sheet1!J66, IF(OR(Sheet1!J66="Null", Sheet1!J66=""), "Null", _xlfn.CONCAT("'", Sheet1!J66, "'"))), ",")</f>
+        <v>4,</v>
+      </c>
+      <c r="D146" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K66), Sheet1!K66, IF(OR(Sheet1!K66="Null", Sheet1!K66=""), "Null", _xlfn.CONCAT("'", Sheet1!K66, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A147" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H67), Sheet1!H67, IF(OR(Sheet1!H67="Null", Sheet1!H67=""), "Null", _xlfn.CONCAT("'", Sheet1!H67, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="B147" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I67), Sheet1!I67, IF(OR(Sheet1!I67="Null", Sheet1!I67=""), "Null", _xlfn.CONCAT("'", Sheet1!I67, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C147" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J67), Sheet1!J67, IF(OR(Sheet1!J67="Null", Sheet1!J67=""), "Null", _xlfn.CONCAT("'", Sheet1!J67, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="D147" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K67), Sheet1!K67, IF(OR(Sheet1!K67="Null", Sheet1!K67=""), "Null", _xlfn.CONCAT("'", Sheet1!K67, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A148" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H68), Sheet1!H68, IF(OR(Sheet1!H68="Null", Sheet1!H68=""), "Null", _xlfn.CONCAT("'", Sheet1!H68, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="B148" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I68), Sheet1!I68, IF(OR(Sheet1!I68="Null", Sheet1!I68=""), "Null", _xlfn.CONCAT("'", Sheet1!I68, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C148" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J68), Sheet1!J68, IF(OR(Sheet1!J68="Null", Sheet1!J68=""), "Null", _xlfn.CONCAT("'", Sheet1!J68, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+      <c r="D148" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K68), Sheet1!K68, IF(OR(Sheet1!K68="Null", Sheet1!K68=""), "Null", _xlfn.CONCAT("'", Sheet1!K68, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A149" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H69), Sheet1!H69, IF(OR(Sheet1!H69="Null", Sheet1!H69=""), "Null", _xlfn.CONCAT("'", Sheet1!H69, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="B149" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I69), Sheet1!I69, IF(OR(Sheet1!I69="Null", Sheet1!I69=""), "Null", _xlfn.CONCAT("'", Sheet1!I69, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C149" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J69), Sheet1!J69, IF(OR(Sheet1!J69="Null", Sheet1!J69=""), "Null", _xlfn.CONCAT("'", Sheet1!J69, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="D149" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K69), Sheet1!K69, IF(OR(Sheet1!K69="Null", Sheet1!K69=""), "Null", _xlfn.CONCAT("'", Sheet1!K69, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A150" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H70), Sheet1!H70, IF(OR(Sheet1!H70="Null", Sheet1!H70=""), "Null", _xlfn.CONCAT("'", Sheet1!H70, "'"))), ",")</f>
+        <v>14,</v>
+      </c>
+      <c r="B150" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I70), Sheet1!I70, IF(OR(Sheet1!I70="Null", Sheet1!I70=""), "Null", _xlfn.CONCAT("'", Sheet1!I70, "'"))), ",")</f>
+        <v>14,</v>
+      </c>
+      <c r="C150" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J70), Sheet1!J70, IF(OR(Sheet1!J70="Null", Sheet1!J70=""), "Null", _xlfn.CONCAT("'", Sheet1!J70, "'"))), ",")</f>
+        <v>14,</v>
+      </c>
+      <c r="D150" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K70), Sheet1!K70, IF(OR(Sheet1!K70="Null", Sheet1!K70=""), "Null", _xlfn.CONCAT("'", Sheet1!K70, "'"))), ",")</f>
+        <v>14,</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A151" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H71), Sheet1!H71, IF(OR(Sheet1!H71="Null", Sheet1!H71=""), "Null", _xlfn.CONCAT("'", Sheet1!H71, "'"))), ",")</f>
+        <v>'SYSTEMM',</v>
+      </c>
+      <c r="B151" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I71), Sheet1!I71, IF(OR(Sheet1!I71="Null", Sheet1!I71=""), "Null", _xlfn.CONCAT("'", Sheet1!I71, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C151" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J71), Sheet1!J71, IF(OR(Sheet1!J71="Null", Sheet1!J71=""), "Null", _xlfn.CONCAT("'", Sheet1!J71, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D151" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K71), Sheet1!K71, IF(OR(Sheet1!K71="Null", Sheet1!K71=""), "Null", _xlfn.CONCAT("'", Sheet1!K71, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A152" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H72), Sheet1!H72, IF(OR(Sheet1!H72="Null", Sheet1!H72=""), "Null", _xlfn.CONCAT("'", Sheet1!H72, "'"))), ",")</f>
+        <v>'55G',</v>
+      </c>
+      <c r="B152" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I72), Sheet1!I72, IF(OR(Sheet1!I72="Null", Sheet1!I72=""), "Null", _xlfn.CONCAT("'", Sheet1!I72, "'"))), ",")</f>
+        <v>'55G',</v>
+      </c>
+      <c r="C152" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J72), Sheet1!J72, IF(OR(Sheet1!J72="Null", Sheet1!J72=""), "Null", _xlfn.CONCAT("'", Sheet1!J72, "'"))), ",")</f>
+        <v>'55G',</v>
+      </c>
+      <c r="D152" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K72), Sheet1!K72, IF(OR(Sheet1!K72="Null", Sheet1!K72=""), "Null", _xlfn.CONCAT("'", Sheet1!K72, "'"))), ",")</f>
+        <v>'55G',</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A153" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H73), Sheet1!H73, IF(OR(Sheet1!H73="Null", Sheet1!H73=""), "Null", _xlfn.CONCAT("'", Sheet1!H73, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="B153" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I73), Sheet1!I73, IF(OR(Sheet1!I73="Null", Sheet1!I73=""), "Null", _xlfn.CONCAT("'", Sheet1!I73, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C153" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J73), Sheet1!J73, IF(OR(Sheet1!J73="Null", Sheet1!J73=""), "Null", _xlfn.CONCAT("'", Sheet1!J73, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="D153" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K73), Sheet1!K73, IF(OR(Sheet1!K73="Null", Sheet1!K73=""), "Null", _xlfn.CONCAT("'", Sheet1!K73, "'"))), ",")</f>
+        <v>'f',</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A154" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H74), Sheet1!H74, IF(OR(Sheet1!H74="Null", Sheet1!H74=""), "Null", _xlfn.CONCAT("'", Sheet1!H74, "'"))), ",")</f>
+        <v>'NEXTHIGHER',</v>
+      </c>
+      <c r="B154" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I74), Sheet1!I74, IF(OR(Sheet1!I74="Null", Sheet1!I74=""), "Null", _xlfn.CONCAT("'", Sheet1!I74, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C154" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J74), Sheet1!J74, IF(OR(Sheet1!J74="Null", Sheet1!J74=""), "Null", _xlfn.CONCAT("'", Sheet1!J74, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D154" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K74), Sheet1!K74, IF(OR(Sheet1!K74="Null", Sheet1!K74=""), "Null", _xlfn.CONCAT("'", Sheet1!K74, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A155" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H75), Sheet1!H75, IF(OR(Sheet1!H75="Null", Sheet1!H75=""), "Null", _xlfn.CONCAT("'", Sheet1!H75, "'"))), ",")</f>
+        <v>'NESCHUB',</v>
+      </c>
+      <c r="B155" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I75), Sheet1!I75, IF(OR(Sheet1!I75="Null", Sheet1!I75=""), "Null", _xlfn.CONCAT("'", Sheet1!I75, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C155" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J75), Sheet1!J75, IF(OR(Sheet1!J75="Null", Sheet1!J75=""), "Null", _xlfn.CONCAT("'", Sheet1!J75, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D155" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K75), Sheet1!K75, IF(OR(Sheet1!K75="Null", Sheet1!K75=""), "Null", _xlfn.CONCAT("'", Sheet1!K75, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A156" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H76), Sheet1!H76, IF(OR(Sheet1!H76="Null", Sheet1!H76=""), "Null", _xlfn.CONCAT("'", Sheet1!H76, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="B156" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I76), Sheet1!I76, IF(OR(Sheet1!I76="Null", Sheet1!I76=""), "Null", _xlfn.CONCAT("'", Sheet1!I76, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C156" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J76), Sheet1!J76, IF(OR(Sheet1!J76="Null", Sheet1!J76=""), "Null", _xlfn.CONCAT("'", Sheet1!J76, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="D156" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K76), Sheet1!K76, IF(OR(Sheet1!K76="Null", Sheet1!K76=""), "Null", _xlfn.CONCAT("'", Sheet1!K76, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A157" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H77), Sheet1!H77, IF(OR(Sheet1!H77="Null", Sheet1!H77=""), "Null", _xlfn.CONCAT("'", Sheet1!H77, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="B157" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I77), Sheet1!I77, IF(OR(Sheet1!I77="Null", Sheet1!I77=""), "Null", _xlfn.CONCAT("'", Sheet1!I77, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C157" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J77), Sheet1!J77, IF(OR(Sheet1!J77="Null", Sheet1!J77=""), "Null", _xlfn.CONCAT("'", Sheet1!J77, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D157" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K77), Sheet1!K77, IF(OR(Sheet1!K77="Null", Sheet1!K77=""), "Null", _xlfn.CONCAT("'", Sheet1!K77, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A158" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H78), Sheet1!H78, IF(OR(Sheet1!H78="Null", Sheet1!H78=""), "Null", _xlfn.CONCAT("'", Sheet1!H78, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="B158" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I78), Sheet1!I78, IF(OR(Sheet1!I78="Null", Sheet1!I78=""), "Null", _xlfn.CONCAT("'", Sheet1!I78, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C158" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J78), Sheet1!J78, IF(OR(Sheet1!J78="Null", Sheet1!J78=""), "Null", _xlfn.CONCAT("'", Sheet1!J78, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D158" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K78), Sheet1!K78, IF(OR(Sheet1!K78="Null", Sheet1!K78=""), "Null", _xlfn.CONCAT("'", Sheet1!K78, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A159" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H79), Sheet1!H79, IF(OR(Sheet1!H79="Null", Sheet1!H79=""), "Null", _xlfn.CONCAT("'", Sheet1!H79, "'"))), ",")</f>
+        <v>2,</v>
+      </c>
+      <c r="B159" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I79), Sheet1!I79, IF(OR(Sheet1!I79="Null", Sheet1!I79=""), "Null", _xlfn.CONCAT("'", Sheet1!I79, "'"))), ",")</f>
+        <v>3,</v>
+      </c>
+      <c r="C159" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J79), Sheet1!J79, IF(OR(Sheet1!J79="Null", Sheet1!J79=""), "Null", _xlfn.CONCAT("'", Sheet1!J79, "'"))), ",")</f>
+        <v>1,</v>
+      </c>
+      <c r="D159" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K79), Sheet1!K79, IF(OR(Sheet1!K79="Null", Sheet1!K79=""), "Null", _xlfn.CONCAT("'", Sheet1!K79, "'"))), ",")</f>
+        <v>4,</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A160">
+        <f>IF(ISNUMBER(Sheet1!H80),Sheet1!H80,IF(OR(Sheet1!H80="Null",Sheet1!H80=""),"Null",_xlfn.CONCAT("'",Sheet1!H80,"'")))</f>
+        <v>3</v>
+      </c>
+      <c r="B160">
+        <f>IF(ISNUMBER(Sheet1!I80),Sheet1!I80,IF(OR(Sheet1!I80="Null",Sheet1!I80=""),"Null",_xlfn.CONCAT("'",Sheet1!I80,"'")))</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A102" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H22), Sheet1!H22, IF(Sheet1!H22="Null", "Null", _xlfn.CONCAT("'", Sheet1!H22, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="B102" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I22), Sheet1!I22, IF(Sheet1!I22="Null", "Null", _xlfn.CONCAT("'", Sheet1!I22, "'"))), ",")</f>
-        <v>'f',</v>
-      </c>
-      <c r="C102" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J22), Sheet1!J22, IF(Sheet1!J22="Null", "Null", _xlfn.CONCAT("'", Sheet1!J22, "'"))), ",")</f>
-        <v>'f',</v>
-      </c>
-      <c r="D102" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K22), Sheet1!K22, IF(Sheet1!K22="Null", "Null", _xlfn.CONCAT("'", Sheet1!K22, "'"))), ",")</f>
-        <v>'f',</v>
-      </c>
-      <c r="F102" t="str">
-        <f>IF(ISNUMBER(Sheet1!H22), Sheet1!H22, IF(Sheet1!H22="Null", "Null", _xlfn.CONCAT("'", Sheet1!H22, "'")))</f>
-        <v>'t'</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A103" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H23), Sheet1!H23, IF(Sheet1!H23="Null", "Null", _xlfn.CONCAT("'", Sheet1!H23, "'"))), ",")</f>
-        <v>'f',</v>
-      </c>
-      <c r="B103" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I23), Sheet1!I23, IF(Sheet1!I23="Null", "Null", _xlfn.CONCAT("'", Sheet1!I23, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="C103" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J23), Sheet1!J23, IF(Sheet1!J23="Null", "Null", _xlfn.CONCAT("'", Sheet1!J23, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="D103" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K23), Sheet1!K23, IF(Sheet1!K23="Null", "Null", _xlfn.CONCAT("'", Sheet1!K23, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="F103" t="str">
-        <f>IF(ISNUMBER(Sheet1!H23), Sheet1!H23, IF(Sheet1!H23="Null", "Null", _xlfn.CONCAT("'", Sheet1!H23, "'")))</f>
-        <v>'f'</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A104" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H24), Sheet1!H24, IF(Sheet1!H24="Null", "Null", _xlfn.CONCAT("'", Sheet1!H24, "'"))), ",")</f>
-        <v>10,</v>
-      </c>
-      <c r="B104" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I24), Sheet1!I24, IF(Sheet1!I24="Null", "Null", _xlfn.CONCAT("'", Sheet1!I24, "'"))), ",")</f>
-        <v>10,</v>
-      </c>
-      <c r="C104" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J24), Sheet1!J24, IF(Sheet1!J24="Null", "Null", _xlfn.CONCAT("'", Sheet1!J24, "'"))), ",")</f>
-        <v>10,</v>
-      </c>
-      <c r="D104" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K24), Sheet1!K24, IF(Sheet1!K24="Null", "Null", _xlfn.CONCAT("'", Sheet1!K24, "'"))), ",")</f>
-        <v>10,</v>
-      </c>
-      <c r="F104">
-        <f>IF(ISNUMBER(Sheet1!H24), Sheet1!H24, IF(Sheet1!H24="Null", "Null", _xlfn.CONCAT("'", Sheet1!H24, "'")))</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A105" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H25), Sheet1!H25, IF(Sheet1!H25="Null", "Null", _xlfn.CONCAT("'", Sheet1!H25, "'"))), ",")</f>
-        <v>11,</v>
-      </c>
-      <c r="B105" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I25), Sheet1!I25, IF(Sheet1!I25="Null", "Null", _xlfn.CONCAT("'", Sheet1!I25, "'"))), ",")</f>
-        <v>22,</v>
-      </c>
-      <c r="C105" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J25), Sheet1!J25, IF(Sheet1!J25="Null", "Null", _xlfn.CONCAT("'", Sheet1!J25, "'"))), ",")</f>
-        <v>33,</v>
-      </c>
-      <c r="D105" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K25), Sheet1!K25, IF(Sheet1!K25="Null", "Null", _xlfn.CONCAT("'", Sheet1!K25, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F105">
-        <f>IF(ISNUMBER(Sheet1!H25), Sheet1!H25, IF(Sheet1!H25="Null", "Null", _xlfn.CONCAT("'", Sheet1!H25, "'")))</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A106" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H26), Sheet1!H26, IF(Sheet1!H26="Null", "Null", _xlfn.CONCAT("'", Sheet1!H26, "'"))), ",")</f>
-        <v>111,</v>
-      </c>
-      <c r="B106" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I26), Sheet1!I26, IF(Sheet1!I26="Null", "Null", _xlfn.CONCAT("'", Sheet1!I26, "'"))), ",")</f>
-        <v>222,</v>
-      </c>
-      <c r="C106" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J26), Sheet1!J26, IF(Sheet1!J26="Null", "Null", _xlfn.CONCAT("'", Sheet1!J26, "'"))), ",")</f>
-        <v>333,</v>
-      </c>
-      <c r="D106" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K26), Sheet1!K26, IF(Sheet1!K26="Null", "Null", _xlfn.CONCAT("'", Sheet1!K26, "'"))), ",")</f>
-        <v>444,</v>
-      </c>
-      <c r="F106">
-        <f>IF(ISNUMBER(Sheet1!H26), Sheet1!H26, IF(Sheet1!H26="Null", "Null", _xlfn.CONCAT("'", Sheet1!H26, "'")))</f>
-        <v>111</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A107" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H27), Sheet1!H27, IF(Sheet1!H27="Null", "Null", _xlfn.CONCAT("'", Sheet1!H27, "'"))), ",")</f>
-        <v>55,</v>
-      </c>
-      <c r="B107" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I27), Sheet1!I27, IF(Sheet1!I27="Null", "Null", _xlfn.CONCAT("'", Sheet1!I27, "'"))), ",")</f>
-        <v>66,</v>
-      </c>
-      <c r="C107" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J27), Sheet1!J27, IF(Sheet1!J27="Null", "Null", _xlfn.CONCAT("'", Sheet1!J27, "'"))), ",")</f>
-        <v>77,</v>
-      </c>
-      <c r="D107" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K27), Sheet1!K27, IF(Sheet1!K27="Null", "Null", _xlfn.CONCAT("'", Sheet1!K27, "'"))), ",")</f>
-        <v>88,</v>
-      </c>
-      <c r="F107">
-        <f>IF(ISNUMBER(Sheet1!H27), Sheet1!H27, IF(Sheet1!H27="Null", "Null", _xlfn.CONCAT("'", Sheet1!H27, "'")))</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A108" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H28), Sheet1!H28, IF(Sheet1!H28="Null", "Null", _xlfn.CONCAT("'", Sheet1!H28, "'"))), ",")</f>
-        <v>44,</v>
-      </c>
-      <c r="B108" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I28), Sheet1!I28, IF(Sheet1!I28="Null", "Null", _xlfn.CONCAT("'", Sheet1!I28, "'"))), ",")</f>
-        <v>987,</v>
-      </c>
-      <c r="C108" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J28), Sheet1!J28, IF(Sheet1!J28="Null", "Null", _xlfn.CONCAT("'", Sheet1!J28, "'"))), ",")</f>
-        <v>12,</v>
-      </c>
-      <c r="D108" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K28), Sheet1!K28, IF(Sheet1!K28="Null", "Null", _xlfn.CONCAT("'", Sheet1!K28, "'"))), ",")</f>
-        <v>15,</v>
-      </c>
-      <c r="F108">
-        <f>IF(ISNUMBER(Sheet1!H28), Sheet1!H28, IF(Sheet1!H28="Null", "Null", _xlfn.CONCAT("'", Sheet1!H28, "'")))</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A109" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H29), Sheet1!H29, IF(Sheet1!H29="Null", "Null", _xlfn.CONCAT("'", Sheet1!H29, "'"))), ",")</f>
-        <v>33,</v>
-      </c>
-      <c r="B109" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I29), Sheet1!I29, IF(Sheet1!I29="Null", "Null", _xlfn.CONCAT("'", Sheet1!I29, "'"))), ",")</f>
-        <v>232,</v>
-      </c>
-      <c r="C109" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J29), Sheet1!J29, IF(Sheet1!J29="Null", "Null", _xlfn.CONCAT("'", Sheet1!J29, "'"))), ",")</f>
-        <v>253,</v>
-      </c>
-      <c r="D109" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K29), Sheet1!K29, IF(Sheet1!K29="Null", "Null", _xlfn.CONCAT("'", Sheet1!K29, "'"))), ",")</f>
-        <v>75,</v>
-      </c>
-      <c r="F109">
-        <f>IF(ISNUMBER(Sheet1!H29), Sheet1!H29, IF(Sheet1!H29="Null", "Null", _xlfn.CONCAT("'", Sheet1!H29, "'")))</f>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A110" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H30), Sheet1!H30, IF(Sheet1!H30="Null", "Null", _xlfn.CONCAT("'", Sheet1!H30, "'"))), ",")</f>
-        <v>22,</v>
-      </c>
-      <c r="B110" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I30), Sheet1!I30, IF(Sheet1!I30="Null", "Null", _xlfn.CONCAT("'", Sheet1!I30, "'"))), ",")</f>
-        <v>253,</v>
-      </c>
-      <c r="C110" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J30), Sheet1!J30, IF(Sheet1!J30="Null", "Null", _xlfn.CONCAT("'", Sheet1!J30, "'"))), ",")</f>
-        <v>1000,</v>
-      </c>
-      <c r="D110" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K30), Sheet1!K30, IF(Sheet1!K30="Null", "Null", _xlfn.CONCAT("'", Sheet1!K30, "'"))), ",")</f>
-        <v>65,</v>
-      </c>
-      <c r="F110">
-        <f>IF(ISNUMBER(Sheet1!H30), Sheet1!H30, IF(Sheet1!H30="Null", "Null", _xlfn.CONCAT("'", Sheet1!H30, "'")))</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A111" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H31), Sheet1!H31, IF(Sheet1!H31="Null", "Null", _xlfn.CONCAT("'", Sheet1!H31, "'"))), ",")</f>
-        <v>50,</v>
-      </c>
-      <c r="B111" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I31), Sheet1!I31, IF(Sheet1!I31="Null", "Null", _xlfn.CONCAT("'", Sheet1!I31, "'"))), ",")</f>
-        <v>23,</v>
-      </c>
-      <c r="C111" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J31), Sheet1!J31, IF(Sheet1!J31="Null", "Null", _xlfn.CONCAT("'", Sheet1!J31, "'"))), ",")</f>
-        <v>465,</v>
-      </c>
-      <c r="D111" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K31), Sheet1!K31, IF(Sheet1!K31="Null", "Null", _xlfn.CONCAT("'", Sheet1!K31, "'"))), ",")</f>
-        <v>50,</v>
-      </c>
-      <c r="F111">
-        <f>IF(ISNUMBER(Sheet1!H31), Sheet1!H31, IF(Sheet1!H31="Null", "Null", _xlfn.CONCAT("'", Sheet1!H31, "'")))</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A112" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H32), Sheet1!H32, IF(Sheet1!H32="Null", "Null", _xlfn.CONCAT("'", Sheet1!H32, "'"))), ",")</f>
-        <v>100,</v>
-      </c>
-      <c r="B112" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I32), Sheet1!I32, IF(Sheet1!I32="Null", "Null", _xlfn.CONCAT("'", Sheet1!I32, "'"))), ",")</f>
-        <v>55,</v>
-      </c>
-      <c r="C112" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J32), Sheet1!J32, IF(Sheet1!J32="Null", "Null", _xlfn.CONCAT("'", Sheet1!J32, "'"))), ",")</f>
-        <v>313,</v>
-      </c>
-      <c r="D112" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K32), Sheet1!K32, IF(Sheet1!K32="Null", "Null", _xlfn.CONCAT("'", Sheet1!K32, "'"))), ",")</f>
-        <v>987,</v>
-      </c>
-      <c r="F112">
-        <f>IF(ISNUMBER(Sheet1!H32), Sheet1!H32, IF(Sheet1!H32="Null", "Null", _xlfn.CONCAT("'", Sheet1!H32, "'")))</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A113" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H33), Sheet1!H33, IF(Sheet1!H33="Null", "Null", _xlfn.CONCAT("'", Sheet1!H33, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="B113" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I33), Sheet1!I33, IF(Sheet1!I33="Null", "Null", _xlfn.CONCAT("'", Sheet1!I33, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C113" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J33), Sheet1!J33, IF(Sheet1!J33="Null", "Null", _xlfn.CONCAT("'", Sheet1!J33, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D113" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K33), Sheet1!K33, IF(Sheet1!K33="Null", "Null", _xlfn.CONCAT("'", Sheet1!K33, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F113" t="str">
-        <f>IF(ISNUMBER(Sheet1!H33), Sheet1!H33, IF(Sheet1!H33="Null", "Null", _xlfn.CONCAT("'", Sheet1!H33, "'")))</f>
-        <v>'t'</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A114" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H34), Sheet1!H34, IF(Sheet1!H34="Null", "Null", _xlfn.CONCAT("'", Sheet1!H34, "'"))), ",")</f>
-        <v>'D9182',</v>
-      </c>
-      <c r="B114" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I34), Sheet1!I34, IF(Sheet1!I34="Null", "Null", _xlfn.CONCAT("'", Sheet1!I34, "'"))), ",")</f>
-        <v>'KCX07',</v>
-      </c>
-      <c r="C114" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J34), Sheet1!J34, IF(Sheet1!J34="Null", "Null", _xlfn.CONCAT("'", Sheet1!J34, "'"))), ",")</f>
-        <v>'DD901',</v>
-      </c>
-      <c r="D114" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K34), Sheet1!K34, IF(Sheet1!K34="Null", "Null", _xlfn.CONCAT("'", Sheet1!K34, "'"))), ",")</f>
-        <v>'1NQ67',</v>
-      </c>
-      <c r="F114" t="str">
-        <f>IF(ISNUMBER(Sheet1!H34), Sheet1!H34, IF(Sheet1!H34="Null", "Null", _xlfn.CONCAT("'", Sheet1!H34, "'")))</f>
-        <v>'D9182'</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A115" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H35), Sheet1!H35, IF(Sheet1!H35="Null", "Null", _xlfn.CONCAT("'", Sheet1!H35, "'"))), ",")</f>
-        <v>'MOWAG',</v>
-      </c>
-      <c r="B115" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I35), Sheet1!I35, IF(Sheet1!I35="Null", "Null", _xlfn.CONCAT("'", Sheet1!I35, "'"))), ",")</f>
-        <v>'asdfas',</v>
-      </c>
-      <c r="C115" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J35), Sheet1!J35, IF(Sheet1!J35="Null", "Null", _xlfn.CONCAT("'", Sheet1!J35, "'"))), ",")</f>
-        <v>'Apple',</v>
-      </c>
-      <c r="D115" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K35), Sheet1!K35, IF(Sheet1!K35="Null", "Null", _xlfn.CONCAT("'", Sheet1!K35, "'"))), ",")</f>
-        <v>'Samsung',</v>
-      </c>
-      <c r="F115" t="str">
-        <f>IF(ISNUMBER(Sheet1!H35), Sheet1!H35, IF(Sheet1!H35="Null", "Null", _xlfn.CONCAT("'", Sheet1!H35, "'")))</f>
-        <v>'MOWAG'</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A116" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H36), Sheet1!H36, IF(Sheet1!H36="Null", "Null", _xlfn.CONCAT("'", Sheet1!H36, "'"))), ",")</f>
-        <v>'Bernstrasse 1',</v>
-      </c>
-      <c r="B116" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I36), Sheet1!I36, IF(Sheet1!I36="Null", "Null", _xlfn.CONCAT("'", Sheet1!I36, "'"))), ",")</f>
-        <v>'Rte du Lac 12',</v>
-      </c>
-      <c r="C116" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J36), Sheet1!J36, IF(Sheet1!J36="Null", "Null", _xlfn.CONCAT("'", Sheet1!J36, "'"))), ",")</f>
-        <v>'One Apple Park Way',</v>
-      </c>
-      <c r="D116" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K36), Sheet1!K36, IF(Sheet1!K36="Null", "Null", _xlfn.CONCAT("'", Sheet1!K36, "'"))), ",")</f>
-        <v>'Against Apple Way',</v>
-      </c>
-      <c r="F116" t="str">
-        <f>IF(ISNUMBER(Sheet1!H36), Sheet1!H36, IF(Sheet1!H36="Null", "Null", _xlfn.CONCAT("'", Sheet1!H36, "'")))</f>
-        <v>'Bernstrasse 1'</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A117" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H37), Sheet1!H37, IF(Sheet1!H37="Null", "Null", _xlfn.CONCAT("'", Sheet1!H37, "'"))), ",")</f>
-        <v>2000,</v>
-      </c>
-      <c r="B117" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I37), Sheet1!I37, IF(Sheet1!I37="Null", "Null", _xlfn.CONCAT("'", Sheet1!I37, "'"))), ",")</f>
-        <v>1215,</v>
-      </c>
-      <c r="C117" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J37), Sheet1!J37, IF(Sheet1!J37="Null", "Null", _xlfn.CONCAT("'", Sheet1!J37, "'"))), ",")</f>
-        <v>95014,</v>
-      </c>
-      <c r="D117" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K37), Sheet1!K37, IF(Sheet1!K37="Null", "Null", _xlfn.CONCAT("'", Sheet1!K37, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="F117">
-        <f>IF(ISNUMBER(Sheet1!H37), Sheet1!H37, IF(Sheet1!H37="Null", "Null", _xlfn.CONCAT("'", Sheet1!H37, "'")))</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A118" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H38), Sheet1!H38, IF(Sheet1!H38="Null", "Null", _xlfn.CONCAT("'", Sheet1!H38, "'"))), ",")</f>
-        <v>'Neuchâtel',</v>
-      </c>
-      <c r="B118" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I38), Sheet1!I38, IF(Sheet1!I38="Null", "Null", _xlfn.CONCAT("'", Sheet1!I38, "'"))), ",")</f>
-        <v>'Genère',</v>
-      </c>
-      <c r="C118" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J38), Sheet1!J38, IF(Sheet1!J38="Null", "Null", _xlfn.CONCAT("'", Sheet1!J38, "'"))), ",")</f>
-        <v>'Cupertino',</v>
-      </c>
-      <c r="D118" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K38), Sheet1!K38, IF(Sheet1!K38="Null", "Null", _xlfn.CONCAT("'", Sheet1!K38, "'"))), ",")</f>
-        <v>'Seoul',</v>
-      </c>
-      <c r="F118" t="str">
-        <f>IF(ISNUMBER(Sheet1!H38), Sheet1!H38, IF(Sheet1!H38="Null", "Null", _xlfn.CONCAT("'", Sheet1!H38, "'")))</f>
-        <v>'Neuchâtel'</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A119" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H39), Sheet1!H39, IF(Sheet1!H39="Null", "Null", _xlfn.CONCAT("'", Sheet1!H39, "'"))), ",")</f>
-        <v>'1.1',</v>
-      </c>
-      <c r="B119" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I39), Sheet1!I39, IF(Sheet1!I39="Null", "Null", _xlfn.CONCAT("'", Sheet1!I39, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C119" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J39), Sheet1!J39, IF(Sheet1!J39="Null", "Null", _xlfn.CONCAT("'", Sheet1!J39, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D119" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K39), Sheet1!K39, IF(Sheet1!K39="Null", "Null", _xlfn.CONCAT("'", Sheet1!K39, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F119" t="str">
-        <f>IF(ISNUMBER(Sheet1!H39), Sheet1!H39, IF(Sheet1!H39="Null", "Null", _xlfn.CONCAT("'", Sheet1!H39, "'")))</f>
-        <v>'1.1'</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A120" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H40), Sheet1!H40, IF(Sheet1!H40="Null", "Null", _xlfn.CONCAT("'", Sheet1!H40, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B120" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I40), Sheet1!I40, IF(Sheet1!I40="Null", "Null", _xlfn.CONCAT("'", Sheet1!I40, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C120" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J40), Sheet1!J40, IF(Sheet1!J40="Null", "Null", _xlfn.CONCAT("'", Sheet1!J40, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D120" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K40), Sheet1!K40, IF(Sheet1!K40="Null", "Null", _xlfn.CONCAT("'", Sheet1!K40, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F120" t="str">
-        <f>IF(ISNUMBER(Sheet1!H40), Sheet1!H40, IF(Sheet1!H40="Null", "Null", _xlfn.CONCAT("'", Sheet1!H40, "'")))</f>
-        <v>Null</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A121" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H41), Sheet1!H41, IF(Sheet1!H41="Null", "Null", _xlfn.CONCAT("'", Sheet1!H41, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="B121" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I41), Sheet1!I41, IF(Sheet1!I41="Null", "Null", _xlfn.CONCAT("'", Sheet1!I41, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="C121" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J41), Sheet1!J41, IF(Sheet1!J41="Null", "Null", _xlfn.CONCAT("'", Sheet1!J41, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="D121" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K41), Sheet1!K41, IF(Sheet1!K41="Null", "Null", _xlfn.CONCAT("'", Sheet1!K41, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="F121">
-        <f>IF(ISNUMBER(Sheet1!H41), Sheet1!H41, IF(Sheet1!H41="Null", "Null", _xlfn.CONCAT("'", Sheet1!H41, "'")))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A122" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H42), Sheet1!H42, IF(Sheet1!H42="Null", "Null", _xlfn.CONCAT("'", Sheet1!H42, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="B122" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I42), Sheet1!I42, IF(Sheet1!I42="Null", "Null", _xlfn.CONCAT("'", Sheet1!I42, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="C122" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J42), Sheet1!J42, IF(Sheet1!J42="Null", "Null", _xlfn.CONCAT("'", Sheet1!J42, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="D122" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K42), Sheet1!K42, IF(Sheet1!K42="Null", "Null", _xlfn.CONCAT("'", Sheet1!K42, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="F122">
-        <f>IF(ISNUMBER(Sheet1!H42), Sheet1!H42, IF(Sheet1!H42="Null", "Null", _xlfn.CONCAT("'", Sheet1!H42, "'")))</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A123" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H43), Sheet1!H43, IF(Sheet1!H43="Null", "Null", _xlfn.CONCAT("'", Sheet1!H43, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="B123" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I43), Sheet1!I43, IF(Sheet1!I43="Null", "Null", _xlfn.CONCAT("'", Sheet1!I43, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="C123" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J43), Sheet1!J43, IF(Sheet1!J43="Null", "Null", _xlfn.CONCAT("'", Sheet1!J43, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="D123" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K43), Sheet1!K43, IF(Sheet1!K43="Null", "Null", _xlfn.CONCAT("'", Sheet1!K43, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="F123">
-        <f>IF(ISNUMBER(Sheet1!H43), Sheet1!H43, IF(Sheet1!H43="Null", "Null", _xlfn.CONCAT("'", Sheet1!H43, "'")))</f>
+      <c r="C160">
+        <f>IF(ISNUMBER(Sheet1!J80),Sheet1!J80,IF(OR(Sheet1!J80="Null",Sheet1!J80=""),"Null",_xlfn.CONCAT("'",Sheet1!J80,"'")))</f>
+        <v>4</v>
+      </c>
+      <c r="D160">
+        <f>IF(ISNUMBER(Sheet1!K80),Sheet1!K80,IF(OR(Sheet1!K80="Null",Sheet1!K80=""),"Null",_xlfn.CONCAT("'",Sheet1!K80,"'")))</f>
         <v>2</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A124" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H44), Sheet1!H44, IF(Sheet1!H44="Null", "Null", _xlfn.CONCAT("'", Sheet1!H44, "'"))), ",")</f>
-        <v>'0022',</v>
-      </c>
-      <c r="B124" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I44), Sheet1!I44, IF(Sheet1!I44="Null", "Null", _xlfn.CONCAT("'", Sheet1!I44, "'"))), ",")</f>
-        <v>'0045',</v>
-      </c>
-      <c r="C124" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J44), Sheet1!J44, IF(Sheet1!J44="Null", "Null", _xlfn.CONCAT("'", Sheet1!J44, "'"))), ",")</f>
-        <v>'0001',</v>
-      </c>
-      <c r="D124" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K44), Sheet1!K44, IF(Sheet1!K44="Null", "Null", _xlfn.CONCAT("'", Sheet1!K44, "'"))), ",")</f>
-        <v>'0496',</v>
-      </c>
-      <c r="F124" t="str">
-        <f>IF(ISNUMBER(Sheet1!H44), Sheet1!H44, IF(Sheet1!H44="Null", "Null", _xlfn.CONCAT("'", Sheet1!H44, "'")))</f>
-        <v>'0022'</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A125" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H45), Sheet1!H45, IF(Sheet1!H45="Null", "Null", _xlfn.CONCAT("'", Sheet1!H45, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B125" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I45), Sheet1!I45, IF(Sheet1!I45="Null", "Null", _xlfn.CONCAT("'", Sheet1!I45, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C125" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J45), Sheet1!J45, IF(Sheet1!J45="Null", "Null", _xlfn.CONCAT("'", Sheet1!J45, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D125" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K45), Sheet1!K45, IF(Sheet1!K45="Null", "Null", _xlfn.CONCAT("'", Sheet1!K45, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F125" t="str">
-        <f>IF(ISNUMBER(Sheet1!H45), Sheet1!H45, IF(Sheet1!H45="Null", "Null", _xlfn.CONCAT("'", Sheet1!H45, "'")))</f>
-        <v>Null</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A126" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H46), Sheet1!H46, IF(Sheet1!H46="Null", "Null", _xlfn.CONCAT("'", Sheet1!H46, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="B126" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I46), Sheet1!I46, IF(Sheet1!I46="Null", "Null", _xlfn.CONCAT("'", Sheet1!I46, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="C126" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J46), Sheet1!J46, IF(Sheet1!J46="Null", "Null", _xlfn.CONCAT("'", Sheet1!J46, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="D126" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K46), Sheet1!K46, IF(Sheet1!K46="Null", "Null", _xlfn.CONCAT("'", Sheet1!K46, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="F126">
-        <f>IF(ISNUMBER(Sheet1!H46), Sheet1!H46, IF(Sheet1!H46="Null", "Null", _xlfn.CONCAT("'", Sheet1!H46, "'")))</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A127" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H47), Sheet1!H47, IF(Sheet1!H47="Null", "Null", _xlfn.CONCAT("'", Sheet1!H47, "'"))), ",")</f>
-        <v>'1000051294',</v>
-      </c>
-      <c r="B127" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I47), Sheet1!I47, IF(Sheet1!I47="Null", "Null", _xlfn.CONCAT("'", Sheet1!I47, "'"))), ",")</f>
-        <v>'1000058908',</v>
-      </c>
-      <c r="C127" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J47), Sheet1!J47, IF(Sheet1!J47="Null", "Null", _xlfn.CONCAT("'", Sheet1!J47, "'"))), ",")</f>
-        <v>'1000057308',</v>
-      </c>
-      <c r="D127" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K47), Sheet1!K47, IF(Sheet1!K47="Null", "Null", _xlfn.CONCAT("'", Sheet1!K47, "'"))), ",")</f>
-        <v>'1000053644',</v>
-      </c>
-      <c r="F127" t="str">
-        <f>IF(ISNUMBER(Sheet1!H47), Sheet1!H47, IF(Sheet1!H47="Null", "Null", _xlfn.CONCAT("'", Sheet1!H47, "'")))</f>
-        <v>'1000051294'</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A128" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H48), Sheet1!H48, IF(Sheet1!H48="Null", "Null", _xlfn.CONCAT("'", Sheet1!H48, "'"))), ",")</f>
-        <v>'ZX0000040',</v>
-      </c>
-      <c r="B128" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I48), Sheet1!I48, IF(Sheet1!I48="Null", "Null", _xlfn.CONCAT("'", Sheet1!I48, "'"))), ",")</f>
-        <v>'ZX0000040',</v>
-      </c>
-      <c r="C128" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J48), Sheet1!J48, IF(Sheet1!J48="Null", "Null", _xlfn.CONCAT("'", Sheet1!J48, "'"))), ",")</f>
-        <v>'ZX0000040',</v>
-      </c>
-      <c r="D128" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K48), Sheet1!K48, IF(Sheet1!K48="Null", "Null", _xlfn.CONCAT("'", Sheet1!K48, "'"))), ",")</f>
-        <v>'ZX0000040',</v>
-      </c>
-      <c r="F128" t="str">
-        <f>IF(ISNUMBER(Sheet1!H48), Sheet1!H48, IF(Sheet1!H48="Null", "Null", _xlfn.CONCAT("'", Sheet1!H48, "'")))</f>
-        <v>'ZX0000040'</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A129" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H49), Sheet1!H49, IF(Sheet1!H49="Null", "Null", _xlfn.CONCAT("'", Sheet1!H49, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="B129" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I49), Sheet1!I49, IF(Sheet1!I49="Null", "Null", _xlfn.CONCAT("'", Sheet1!I49, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="C129" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J49), Sheet1!J49, IF(Sheet1!J49="Null", "Null", _xlfn.CONCAT("'", Sheet1!J49, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="D129" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K49), Sheet1!K49, IF(Sheet1!K49="Null", "Null", _xlfn.CONCAT("'", Sheet1!K49, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="F129">
-        <f>IF(ISNUMBER(Sheet1!H49), Sheet1!H49, IF(Sheet1!H49="Null", "Null", _xlfn.CONCAT("'", Sheet1!H49, "'")))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A130" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H50), Sheet1!H50, IF(Sheet1!H50="Null", "Null", _xlfn.CONCAT("'", Sheet1!H50, "'"))), ",")</f>
-        <v>'abcde',</v>
-      </c>
-      <c r="B130" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I50), Sheet1!I50, IF(Sheet1!I50="Null", "Null", _xlfn.CONCAT("'", Sheet1!I50, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C130" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J50), Sheet1!J50, IF(Sheet1!J50="Null", "Null", _xlfn.CONCAT("'", Sheet1!J50, "'"))), ",")</f>
-        <v>54321,</v>
-      </c>
-      <c r="D130" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K50), Sheet1!K50, IF(Sheet1!K50="Null", "Null", _xlfn.CONCAT("'", Sheet1!K50, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F130" t="str">
-        <f>IF(ISNUMBER(Sheet1!H50), Sheet1!H50, IF(Sheet1!H50="Null", "Null", _xlfn.CONCAT("'", Sheet1!H50, "'")))</f>
-        <v>'abcde'</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A131" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H51), Sheet1!H51, IF(Sheet1!H51="Null", "Null", _xlfn.CONCAT("'", Sheet1!H51, "'"))), ",")</f>
-        <v>'.1',</v>
-      </c>
-      <c r="B131" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I51), Sheet1!I51, IF(Sheet1!I51="Null", "Null", _xlfn.CONCAT("'", Sheet1!I51, "'"))), ",")</f>
-        <v>'0000',</v>
-      </c>
-      <c r="C131" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J51), Sheet1!J51, IF(Sheet1!J51="Null", "Null", _xlfn.CONCAT("'", Sheet1!J51, "'"))), ",")</f>
-        <v>1.01,</v>
-      </c>
-      <c r="D131" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K51), Sheet1!K51, IF(Sheet1!K51="Null", "Null", _xlfn.CONCAT("'", Sheet1!K51, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F131" t="str">
-        <f>IF(ISNUMBER(Sheet1!H51), Sheet1!H51, IF(Sheet1!H51="Null", "Null", _xlfn.CONCAT("'", Sheet1!H51, "'")))</f>
-        <v>'.1'</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A132" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H52), Sheet1!H52, IF(Sheet1!H52="Null", "Null", _xlfn.CONCAT("'", Sheet1!H52, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="B132" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I52), Sheet1!I52, IF(Sheet1!I52="Null", "Null", _xlfn.CONCAT("'", Sheet1!I52, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C132" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J52), Sheet1!J52, IF(Sheet1!J52="Null", "Null", _xlfn.CONCAT("'", Sheet1!J52, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="D132" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K52), Sheet1!K52, IF(Sheet1!K52="Null", "Null", _xlfn.CONCAT("'", Sheet1!K52, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F132" t="str">
-        <f>IF(ISNUMBER(Sheet1!H52), Sheet1!H52, IF(Sheet1!H52="Null", "Null", _xlfn.CONCAT("'", Sheet1!H52, "'")))</f>
-        <v>'t'</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A133" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H53), Sheet1!H53, IF(Sheet1!H53="Null", "Null", _xlfn.CONCAT("'", Sheet1!H53, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B133" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I53), Sheet1!I53, IF(Sheet1!I53="Null", "Null", _xlfn.CONCAT("'", Sheet1!I53, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C133" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J53), Sheet1!J53, IF(Sheet1!J53="Null", "Null", _xlfn.CONCAT("'", Sheet1!J53, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D133" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K53), Sheet1!K53, IF(Sheet1!K53="Null", "Null", _xlfn.CONCAT("'", Sheet1!K53, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F133" t="str">
-        <f>IF(ISNUMBER(Sheet1!H53), Sheet1!H53, IF(Sheet1!H53="Null", "Null", _xlfn.CONCAT("'", Sheet1!H53, "'")))</f>
-        <v>Null</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A134" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H54), Sheet1!H54, IF(Sheet1!H54="Null", "Null", _xlfn.CONCAT("'", Sheet1!H54, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="B134" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I54), Sheet1!I54, IF(Sheet1!I54="Null", "Null", _xlfn.CONCAT("'", Sheet1!I54, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="C134" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J54), Sheet1!J54, IF(Sheet1!J54="Null", "Null", _xlfn.CONCAT("'", Sheet1!J54, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D134" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K54), Sheet1!K54, IF(Sheet1!K54="Null", "Null", _xlfn.CONCAT("'", Sheet1!K54, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="F134" t="str">
-        <f>IF(ISNUMBER(Sheet1!H54), Sheet1!H54, IF(Sheet1!H54="Null", "Null", _xlfn.CONCAT("'", Sheet1!H54, "'")))</f>
-        <v>'t'</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A135" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H55), Sheet1!H55, IF(Sheet1!H55="Null", "Null", _xlfn.CONCAT("'", Sheet1!H55, "'"))), ",")</f>
-        <v>'f',</v>
-      </c>
-      <c r="B135" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I55), Sheet1!I55, IF(Sheet1!I55="Null", "Null", _xlfn.CONCAT("'", Sheet1!I55, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="C135" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J55), Sheet1!J55, IF(Sheet1!J55="Null", "Null", _xlfn.CONCAT("'", Sheet1!J55, "'"))), ",")</f>
-        <v>'f',</v>
-      </c>
-      <c r="D135" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K55), Sheet1!K55, IF(Sheet1!K55="Null", "Null", _xlfn.CONCAT("'", Sheet1!K55, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F135" t="str">
-        <f>IF(ISNUMBER(Sheet1!H55), Sheet1!H55, IF(Sheet1!H55="Null", "Null", _xlfn.CONCAT("'", Sheet1!H55, "'")))</f>
-        <v>'f'</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A136" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H56), Sheet1!H56, IF(Sheet1!H56="Null", "Null", _xlfn.CONCAT("'", Sheet1!H56, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="B136" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I56), Sheet1!I56, IF(Sheet1!I56="Null", "Null", _xlfn.CONCAT("'", Sheet1!I56, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="C136" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J56), Sheet1!J56, IF(Sheet1!J56="Null", "Null", _xlfn.CONCAT("'", Sheet1!J56, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="D136" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K56), Sheet1!K56, IF(Sheet1!K56="Null", "Null", _xlfn.CONCAT("'", Sheet1!K56, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="F136">
-        <f>IF(ISNUMBER(Sheet1!H56), Sheet1!H56, IF(Sheet1!H56="Null", "Null", _xlfn.CONCAT("'", Sheet1!H56, "'")))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A137" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H57), Sheet1!H57, IF(Sheet1!H57="Null", "Null", _xlfn.CONCAT("'", Sheet1!H57, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="B137" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I57), Sheet1!I57, IF(Sheet1!I57="Null", "Null", _xlfn.CONCAT("'", Sheet1!I57, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="C137" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J57), Sheet1!J57, IF(Sheet1!J57="Null", "Null", _xlfn.CONCAT("'", Sheet1!J57, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="D137" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K57), Sheet1!K57, IF(Sheet1!K57="Null", "Null", _xlfn.CONCAT("'", Sheet1!K57, "'"))), ",")</f>
-        <v>4,</v>
-      </c>
-      <c r="F137">
-        <f>IF(ISNUMBER(Sheet1!H57), Sheet1!H57, IF(Sheet1!H57="Null", "Null", _xlfn.CONCAT("'", Sheet1!H57, "'")))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A138" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H58), Sheet1!H58, IF(Sheet1!H58="Null", "Null", _xlfn.CONCAT("'", Sheet1!H58, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B138" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I58), Sheet1!I58, IF(Sheet1!I58="Null", "Null", _xlfn.CONCAT("'", Sheet1!I58, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C138" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J58), Sheet1!J58, IF(Sheet1!J58="Null", "Null", _xlfn.CONCAT("'", Sheet1!J58, "'"))), ",")</f>
-        <v>4,</v>
-      </c>
-      <c r="D138" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K58), Sheet1!K58, IF(Sheet1!K58="Null", "Null", _xlfn.CONCAT("'", Sheet1!K58, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F138" t="str">
-        <f>IF(ISNUMBER(Sheet1!H58), Sheet1!H58, IF(Sheet1!H58="Null", "Null", _xlfn.CONCAT("'", Sheet1!H58, "'")))</f>
-        <v>Null</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A139" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H59), Sheet1!H59, IF(Sheet1!H59="Null", "Null", _xlfn.CONCAT("'", Sheet1!H59, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B139" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I59), Sheet1!I59, IF(Sheet1!I59="Null", "Null", _xlfn.CONCAT("'", Sheet1!I59, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C139" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J59), Sheet1!J59, IF(Sheet1!J59="Null", "Null", _xlfn.CONCAT("'", Sheet1!J59, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D139" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K59), Sheet1!K59, IF(Sheet1!K59="Null", "Null", _xlfn.CONCAT("'", Sheet1!K59, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F139" t="str">
-        <f>IF(ISNUMBER(Sheet1!H59), Sheet1!H59, IF(Sheet1!H59="Null", "Null", _xlfn.CONCAT("'", Sheet1!H59, "'")))</f>
-        <v>Null</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A140" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H60), Sheet1!H60, IF(Sheet1!H60="Null", "Null", _xlfn.CONCAT("'", Sheet1!H60, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="B140" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I60), Sheet1!I60, IF(Sheet1!I60="Null", "Null", _xlfn.CONCAT("'", Sheet1!I60, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="C140" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J60), Sheet1!J60, IF(Sheet1!J60="Null", "Null", _xlfn.CONCAT("'", Sheet1!J60, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="D140" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K60), Sheet1!K60, IF(Sheet1!K60="Null", "Null", _xlfn.CONCAT("'", Sheet1!K60, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="F140">
-        <f>IF(ISNUMBER(Sheet1!H60), Sheet1!H60, IF(Sheet1!H60="Null", "Null", _xlfn.CONCAT("'", Sheet1!H60, "'")))</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A141" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H61), Sheet1!H61, IF(Sheet1!H61="Null", "Null", _xlfn.CONCAT("'", Sheet1!H61, "'"))), ",")</f>
-        <v>35,</v>
-      </c>
-      <c r="B141" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I61), Sheet1!I61, IF(Sheet1!I61="Null", "Null", _xlfn.CONCAT("'", Sheet1!I61, "'"))), ",")</f>
-        <v>35,</v>
-      </c>
-      <c r="C141" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J61), Sheet1!J61, IF(Sheet1!J61="Null", "Null", _xlfn.CONCAT("'", Sheet1!J61, "'"))), ",")</f>
-        <v>35,</v>
-      </c>
-      <c r="D141" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K61), Sheet1!K61, IF(Sheet1!K61="Null", "Null", _xlfn.CONCAT("'", Sheet1!K61, "'"))), ",")</f>
-        <v>35,</v>
-      </c>
-      <c r="F141">
-        <f>IF(ISNUMBER(Sheet1!H61), Sheet1!H61, IF(Sheet1!H61="Null", "Null", _xlfn.CONCAT("'", Sheet1!H61, "'")))</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A142" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H62), Sheet1!H62, IF(Sheet1!H62="Null", "Null", _xlfn.CONCAT("'", Sheet1!H62, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B142" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I62), Sheet1!I62, IF(Sheet1!I62="Null", "Null", _xlfn.CONCAT("'", Sheet1!I62, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C142" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J62), Sheet1!J62, IF(Sheet1!J62="Null", "Null", _xlfn.CONCAT("'", Sheet1!J62, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D142" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K62), Sheet1!K62, IF(Sheet1!K62="Null", "Null", _xlfn.CONCAT("'", Sheet1!K62, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F142" t="str">
-        <f>IF(ISNUMBER(Sheet1!H62), Sheet1!H62, IF(Sheet1!H62="Null", "Null", _xlfn.CONCAT("'", Sheet1!H62, "'")))</f>
-        <v>Null</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A143" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H63), Sheet1!H63, IF(Sheet1!H63="Null", "Null", _xlfn.CONCAT("'", Sheet1!H63, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="B143" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I63), Sheet1!I63, IF(Sheet1!I63="Null", "Null", _xlfn.CONCAT("'", Sheet1!I63, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="C143" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J63), Sheet1!J63, IF(Sheet1!J63="Null", "Null", _xlfn.CONCAT("'", Sheet1!J63, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="D143" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K63), Sheet1!K63, IF(Sheet1!K63="Null", "Null", _xlfn.CONCAT("'", Sheet1!K63, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="F143">
-        <f>IF(ISNUMBER(Sheet1!H63), Sheet1!H63, IF(Sheet1!H63="Null", "Null", _xlfn.CONCAT("'", Sheet1!H63, "'")))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A144" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H64), Sheet1!H64, IF(Sheet1!H64="Null", "Null", _xlfn.CONCAT("'", Sheet1!H64, "'"))), ",")</f>
-        <v>'09211600-7',</v>
-      </c>
-      <c r="B144" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I64), Sheet1!I64, IF(Sheet1!I64="Null", "Null", _xlfn.CONCAT("'", Sheet1!I64, "'"))), ",")</f>
-        <v>'09221000-4',</v>
-      </c>
-      <c r="C144" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J64), Sheet1!J64, IF(Sheet1!J64="Null", "Null", _xlfn.CONCAT("'", Sheet1!J64, "'"))), ",")</f>
-        <v>'09221400-8',</v>
-      </c>
-      <c r="D144" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K64), Sheet1!K64, IF(Sheet1!K64="Null", "Null", _xlfn.CONCAT("'", Sheet1!K64, "'"))), ",")</f>
-        <v>'09230000-0',</v>
-      </c>
-      <c r="F144" t="str">
-        <f>IF(ISNUMBER(Sheet1!H64), Sheet1!H64, IF(Sheet1!H64="Null", "Null", _xlfn.CONCAT("'", Sheet1!H64, "'")))</f>
-        <v>'09211600-7'</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A145" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H65), Sheet1!H65, IF(Sheet1!H65="Null", "Null", _xlfn.CONCAT("'", Sheet1!H65, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="B145" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I65), Sheet1!I65, IF(Sheet1!I65="Null", "Null", _xlfn.CONCAT("'", Sheet1!I65, "'"))), ",")</f>
-        <v>4,</v>
-      </c>
-      <c r="C145" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J65), Sheet1!J65, IF(Sheet1!J65="Null", "Null", _xlfn.CONCAT("'", Sheet1!J65, "'"))), ",")</f>
-        <v>4,</v>
-      </c>
-      <c r="D145" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K65), Sheet1!K65, IF(Sheet1!K65="Null", "Null", _xlfn.CONCAT("'", Sheet1!K65, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="F145">
-        <f>IF(ISNUMBER(Sheet1!H65), Sheet1!H65, IF(Sheet1!H65="Null", "Null", _xlfn.CONCAT("'", Sheet1!H65, "'")))</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A146" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H66), Sheet1!H66, IF(Sheet1!H66="Null", "Null", _xlfn.CONCAT("'", Sheet1!H66, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B146" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I66), Sheet1!I66, IF(Sheet1!I66="Null", "Null", _xlfn.CONCAT("'", Sheet1!I66, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="C146" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J66), Sheet1!J66, IF(Sheet1!J66="Null", "Null", _xlfn.CONCAT("'", Sheet1!J66, "'"))), ",")</f>
-        <v>4,</v>
-      </c>
-      <c r="D146" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K66), Sheet1!K66, IF(Sheet1!K66="Null", "Null", _xlfn.CONCAT("'", Sheet1!K66, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F146" t="str">
-        <f>IF(ISNUMBER(Sheet1!H66), Sheet1!H66, IF(Sheet1!H66="Null", "Null", _xlfn.CONCAT("'", Sheet1!H66, "'")))</f>
-        <v>Null</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A147" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H67), Sheet1!H67, IF(Sheet1!H67="Null", "Null", _xlfn.CONCAT("'", Sheet1!H67, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="B147" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I67), Sheet1!I67, IF(Sheet1!I67="Null", "Null", _xlfn.CONCAT("'", Sheet1!I67, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C147" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J67), Sheet1!J67, IF(Sheet1!J67="Null", "Null", _xlfn.CONCAT("'", Sheet1!J67, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="D147" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K67), Sheet1!K67, IF(Sheet1!K67="Null", "Null", _xlfn.CONCAT("'", Sheet1!K67, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F147" t="str">
-        <f>IF(ISNUMBER(Sheet1!H67), Sheet1!H67, IF(Sheet1!H67="Null", "Null", _xlfn.CONCAT("'", Sheet1!H67, "'")))</f>
-        <v>'t'</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A148" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H68), Sheet1!H68, IF(Sheet1!H68="Null", "Null", _xlfn.CONCAT("'", Sheet1!H68, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="B148" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I68), Sheet1!I68, IF(Sheet1!I68="Null", "Null", _xlfn.CONCAT("'", Sheet1!I68, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C148" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J68), Sheet1!J68, IF(Sheet1!J68="Null", "Null", _xlfn.CONCAT("'", Sheet1!J68, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="D148" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K68), Sheet1!K68, IF(Sheet1!K68="Null", "Null", _xlfn.CONCAT("'", Sheet1!K68, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F148">
-        <f>IF(ISNUMBER(Sheet1!H68), Sheet1!H68, IF(Sheet1!H68="Null", "Null", _xlfn.CONCAT("'", Sheet1!H68, "'")))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A149" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H69), Sheet1!H69, IF(Sheet1!H69="Null", "Null", _xlfn.CONCAT("'", Sheet1!H69, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="B149" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I69), Sheet1!I69, IF(Sheet1!I69="Null", "Null", _xlfn.CONCAT("'", Sheet1!I69, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C149" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J69), Sheet1!J69, IF(Sheet1!J69="Null", "Null", _xlfn.CONCAT("'", Sheet1!J69, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="D149" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K69), Sheet1!K69, IF(Sheet1!K69="Null", "Null", _xlfn.CONCAT("'", Sheet1!K69, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="F149">
-        <f>IF(ISNUMBER(Sheet1!H69), Sheet1!H69, IF(Sheet1!H69="Null", "Null", _xlfn.CONCAT("'", Sheet1!H69, "'")))</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A150" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H70), Sheet1!H70, IF(Sheet1!H70="Null", "Null", _xlfn.CONCAT("'", Sheet1!H70, "'"))), ",")</f>
-        <v>14,</v>
-      </c>
-      <c r="B150" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I70), Sheet1!I70, IF(Sheet1!I70="Null", "Null", _xlfn.CONCAT("'", Sheet1!I70, "'"))), ",")</f>
-        <v>14,</v>
-      </c>
-      <c r="C150" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J70), Sheet1!J70, IF(Sheet1!J70="Null", "Null", _xlfn.CONCAT("'", Sheet1!J70, "'"))), ",")</f>
-        <v>14,</v>
-      </c>
-      <c r="D150" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K70), Sheet1!K70, IF(Sheet1!K70="Null", "Null", _xlfn.CONCAT("'", Sheet1!K70, "'"))), ",")</f>
-        <v>14,</v>
-      </c>
-      <c r="F150">
-        <f>IF(ISNUMBER(Sheet1!H70), Sheet1!H70, IF(Sheet1!H70="Null", "Null", _xlfn.CONCAT("'", Sheet1!H70, "'")))</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A151" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H71), Sheet1!H71, IF(Sheet1!H71="Null", "Null", _xlfn.CONCAT("'", Sheet1!H71, "'"))), ",")</f>
-        <v>'SYSTEMM',</v>
-      </c>
-      <c r="B151" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I71), Sheet1!I71, IF(Sheet1!I71="Null", "Null", _xlfn.CONCAT("'", Sheet1!I71, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C151" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J71), Sheet1!J71, IF(Sheet1!J71="Null", "Null", _xlfn.CONCAT("'", Sheet1!J71, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D151" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K71), Sheet1!K71, IF(Sheet1!K71="Null", "Null", _xlfn.CONCAT("'", Sheet1!K71, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F151" t="str">
-        <f>IF(ISNUMBER(Sheet1!H71), Sheet1!H71, IF(Sheet1!H71="Null", "Null", _xlfn.CONCAT("'", Sheet1!H71, "'")))</f>
-        <v>'SYSTEMM'</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A152" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H72), Sheet1!H72, IF(Sheet1!H72="Null", "Null", _xlfn.CONCAT("'", Sheet1!H72, "'"))), ",")</f>
-        <v>'55G',</v>
-      </c>
-      <c r="B152" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I72), Sheet1!I72, IF(Sheet1!I72="Null", "Null", _xlfn.CONCAT("'", Sheet1!I72, "'"))), ",")</f>
-        <v>'55G',</v>
-      </c>
-      <c r="C152" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J72), Sheet1!J72, IF(Sheet1!J72="Null", "Null", _xlfn.CONCAT("'", Sheet1!J72, "'"))), ",")</f>
-        <v>'55G',</v>
-      </c>
-      <c r="D152" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K72), Sheet1!K72, IF(Sheet1!K72="Null", "Null", _xlfn.CONCAT("'", Sheet1!K72, "'"))), ",")</f>
-        <v>'55G',</v>
-      </c>
-      <c r="F152" t="str">
-        <f>IF(ISNUMBER(Sheet1!H72), Sheet1!H72, IF(Sheet1!H72="Null", "Null", _xlfn.CONCAT("'", Sheet1!H72, "'")))</f>
-        <v>'55G'</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A153" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H73), Sheet1!H73, IF(Sheet1!H73="Null", "Null", _xlfn.CONCAT("'", Sheet1!H73, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="B153" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I73), Sheet1!I73, IF(Sheet1!I73="Null", "Null", _xlfn.CONCAT("'", Sheet1!I73, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C153" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J73), Sheet1!J73, IF(Sheet1!J73="Null", "Null", _xlfn.CONCAT("'", Sheet1!J73, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="D153" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K73), Sheet1!K73, IF(Sheet1!K73="Null", "Null", _xlfn.CONCAT("'", Sheet1!K73, "'"))), ",")</f>
-        <v>'f',</v>
-      </c>
-      <c r="F153" t="str">
-        <f>IF(ISNUMBER(Sheet1!H73), Sheet1!H73, IF(Sheet1!H73="Null", "Null", _xlfn.CONCAT("'", Sheet1!H73, "'")))</f>
-        <v>'t'</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A154" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H74), Sheet1!H74, IF(Sheet1!H74="Null", "Null", _xlfn.CONCAT("'", Sheet1!H74, "'"))), ",")</f>
-        <v>'NEXTHIGHER',</v>
-      </c>
-      <c r="B154" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I74), Sheet1!I74, IF(Sheet1!I74="Null", "Null", _xlfn.CONCAT("'", Sheet1!I74, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C154" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J74), Sheet1!J74, IF(Sheet1!J74="Null", "Null", _xlfn.CONCAT("'", Sheet1!J74, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D154" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K74), Sheet1!K74, IF(Sheet1!K74="Null", "Null", _xlfn.CONCAT("'", Sheet1!K74, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F154" t="str">
-        <f>IF(ISNUMBER(Sheet1!H74), Sheet1!H74, IF(Sheet1!H74="Null", "Null", _xlfn.CONCAT("'", Sheet1!H74, "'")))</f>
-        <v>'NEXTHIGHER'</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A155" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H75), Sheet1!H75, IF(Sheet1!H75="Null", "Null", _xlfn.CONCAT("'", Sheet1!H75, "'"))), ",")</f>
-        <v>'NESCHUB',</v>
-      </c>
-      <c r="B155" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I75), Sheet1!I75, IF(Sheet1!I75="Null", "Null", _xlfn.CONCAT("'", Sheet1!I75, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C155" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J75), Sheet1!J75, IF(Sheet1!J75="Null", "Null", _xlfn.CONCAT("'", Sheet1!J75, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D155" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K75), Sheet1!K75, IF(Sheet1!K75="Null", "Null", _xlfn.CONCAT("'", Sheet1!K75, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F155" t="str">
-        <f>IF(ISNUMBER(Sheet1!H75), Sheet1!H75, IF(Sheet1!H75="Null", "Null", _xlfn.CONCAT("'", Sheet1!H75, "'")))</f>
-        <v>'NESCHUB'</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A156" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H76), Sheet1!H76, IF(Sheet1!H76="Null", "Null", _xlfn.CONCAT("'", Sheet1!H76, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="B156" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I76), Sheet1!I76, IF(Sheet1!I76="Null", "Null", _xlfn.CONCAT("'", Sheet1!I76, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C156" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J76), Sheet1!J76, IF(Sheet1!J76="Null", "Null", _xlfn.CONCAT("'", Sheet1!J76, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="D156" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K76), Sheet1!K76, IF(Sheet1!K76="Null", "Null", _xlfn.CONCAT("'", Sheet1!K76, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F156" t="str">
-        <f>IF(ISNUMBER(Sheet1!H76), Sheet1!H76, IF(Sheet1!H76="Null", "Null", _xlfn.CONCAT("'", Sheet1!H76, "'")))</f>
-        <v>'t'</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A157" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H77), Sheet1!H77, IF(Sheet1!H77="Null", "Null", _xlfn.CONCAT("'", Sheet1!H77, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="B157" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I77), Sheet1!I77, IF(Sheet1!I77="Null", "Null", _xlfn.CONCAT("'", Sheet1!I77, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C157" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J77), Sheet1!J77, IF(Sheet1!J77="Null", "Null", _xlfn.CONCAT("'", Sheet1!J77, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D157" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K77), Sheet1!K77, IF(Sheet1!K77="Null", "Null", _xlfn.CONCAT("'", Sheet1!K77, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F157" t="str">
-        <f>IF(ISNUMBER(Sheet1!H77), Sheet1!H77, IF(Sheet1!H77="Null", "Null", _xlfn.CONCAT("'", Sheet1!H77, "'")))</f>
-        <v>'t'</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A158" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H78), Sheet1!H78, IF(Sheet1!H78="Null", "Null", _xlfn.CONCAT("'", Sheet1!H78, "'"))), ",")</f>
-        <v>'t',</v>
-      </c>
-      <c r="B158" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I78), Sheet1!I78, IF(Sheet1!I78="Null", "Null", _xlfn.CONCAT("'", Sheet1!I78, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C158" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J78), Sheet1!J78, IF(Sheet1!J78="Null", "Null", _xlfn.CONCAT("'", Sheet1!J78, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D158" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K78), Sheet1!K78, IF(Sheet1!K78="Null", "Null", _xlfn.CONCAT("'", Sheet1!K78, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="F158" t="str">
-        <f>IF(ISNUMBER(Sheet1!H78), Sheet1!H78, IF(Sheet1!H78="Null", "Null", _xlfn.CONCAT("'", Sheet1!H78, "'")))</f>
-        <v>'t'</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A159" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H79), Sheet1!H79, IF(Sheet1!H79="Null", "Null", _xlfn.CONCAT("'", Sheet1!H79, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="B159" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I79), Sheet1!I79, IF(Sheet1!I79="Null", "Null", _xlfn.CONCAT("'", Sheet1!I79, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="C159" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J79), Sheet1!J79, IF(Sheet1!J79="Null", "Null", _xlfn.CONCAT("'", Sheet1!J79, "'"))), ",")</f>
-        <v>1,</v>
-      </c>
-      <c r="D159" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K79), Sheet1!K79, IF(Sheet1!K79="Null", "Null", _xlfn.CONCAT("'", Sheet1!K79, "'"))), ",")</f>
-        <v>4,</v>
-      </c>
-      <c r="F159">
-        <f>IF(ISNUMBER(Sheet1!H79), Sheet1!H79, IF(Sheet1!H79="Null", "Null", _xlfn.CONCAT("'", Sheet1!H79, "'")))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A160" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H80), Sheet1!H80, IF(Sheet1!H80="Null", "Null", _xlfn.CONCAT("'", Sheet1!H80, "'"))), ",")</f>
-        <v>3,</v>
-      </c>
-      <c r="B160" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I80), Sheet1!I80, IF(Sheet1!I80="Null", "Null", _xlfn.CONCAT("'", Sheet1!I80, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="C160" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J80), Sheet1!J80, IF(Sheet1!J80="Null", "Null", _xlfn.CONCAT("'", Sheet1!J80, "'"))), ",")</f>
-        <v>4,</v>
-      </c>
-      <c r="D160" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K80), Sheet1!K80, IF(Sheet1!K80="Null", "Null", _xlfn.CONCAT("'", Sheet1!K80, "'"))), ",")</f>
-        <v>2,</v>
-      </c>
-      <c r="F160">
-        <f>IF(ISNUMBER(Sheet1!H80), Sheet1!H80, IF(Sheet1!H80="Null", "Null", _xlfn.CONCAT("'", Sheet1!H80, "'")))</f>
-        <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Added the field 'orderbuchpflicht'.
</commit_message>
<xml_diff>
--- a/b11_1/fields/insert.xlsx
+++ b/b11_1/fields/insert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yann/Prog/Python/LBA/b11_1/fields/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA054F5B-81EA-7940-90B9-DB15437D4E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4886AB-7594-2C48-BDA8-48DB02BBDCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="5000" windowWidth="46780" windowHeight="18000" activeTab="1" xr2:uid="{41FF1C03-8D98-44C8-8EDC-6562CA448D86}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="276">
   <si>
     <t>Positions-Nr.</t>
   </si>
@@ -876,6 +876,12 @@
   </si>
   <si>
     <t>);</t>
+  </si>
+  <si>
+    <t>Orderbuchpflicht</t>
+  </si>
+  <si>
+    <t>orderbuchpflicht</t>
   </si>
 </sst>
 </file>
@@ -1256,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1F6E88-797B-42CA-9EC0-C2555AB4031B}">
-  <dimension ref="A1:K80"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24:K24"/>
+    <sheetView topLeftCell="A53" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="L76" sqref="L76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3489,40 +3495,35 @@
     </row>
     <row r="76" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>274</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C76" t="s">
-        <v>117</v>
-      </c>
-      <c r="E76" t="s">
-        <v>117</v>
+        <v>275</v>
       </c>
       <c r="H76" t="s">
         <v>268</v>
       </c>
-      <c r="I76" s="2" t="s">
-        <v>271</v>
-      </c>
+      <c r="I76" s="2"/>
       <c r="J76" t="s">
         <v>268</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C77" t="s">
         <v>117</v>
       </c>
+      <c r="E77" t="s">
+        <v>117</v>
+      </c>
       <c r="H77" t="s">
         <v>268</v>
       </c>
@@ -3530,7 +3531,7 @@
         <v>271</v>
       </c>
       <c r="J77" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>271</v>
@@ -3538,10 +3539,10 @@
     </row>
     <row r="78" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C78" t="s">
         <v>117</v>
@@ -3559,69 +3560,92 @@
         <v>271</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
-        <v>76</v>
+    <row r="79" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>75</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G79" s="5"/>
-      <c r="H79" s="2">
-        <v>2</v>
-      </c>
-      <c r="I79" s="2">
-        <v>3</v>
-      </c>
-      <c r="J79" s="2">
-        <v>1</v>
-      </c>
-      <c r="K79" s="2">
-        <v>4</v>
+        <v>237</v>
+      </c>
+      <c r="C79" t="s">
+        <v>117</v>
+      </c>
+      <c r="H79" t="s">
+        <v>268</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="J79" t="s">
+        <v>271</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="G80" s="5"/>
       <c r="H80" s="2">
+        <v>2</v>
+      </c>
+      <c r="I80" s="2">
         <v>3</v>
       </c>
-      <c r="I80" s="2">
+      <c r="J80" s="2">
+        <v>1</v>
+      </c>
+      <c r="K80" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G81" s="5"/>
+      <c r="H81" s="2">
+        <v>3</v>
+      </c>
+      <c r="I81" s="2">
         <v>2</v>
       </c>
-      <c r="J80" s="2">
+      <c r="J81" s="2">
         <v>4</v>
       </c>
-      <c r="K80" s="2">
+      <c r="K81" s="2">
         <v>2</v>
       </c>
     </row>
@@ -3633,11 +3657,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB86915-FE40-8640-8F00-428279462302}">
-  <dimension ref="A1:D161"/>
+  <dimension ref="A1:D163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4993,1540 +5015,1576 @@
     <row r="76" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A76" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B76, ",")</f>
-        <v>verteilung_apm_kerda,</v>
+        <v>orderbuchpflicht,</v>
       </c>
       <c r="B76" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B76, ",")</f>
-        <v>verteilung_apm_kerda,</v>
+        <v>orderbuchpflicht,</v>
       </c>
       <c r="C76" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B76, ",")</f>
-        <v>verteilung_apm_kerda,</v>
+        <v>orderbuchpflicht,</v>
       </c>
       <c r="D76" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B76, ",")</f>
-        <v>verteilung_apm_kerda,</v>
+        <v>orderbuchpflicht,</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A77" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B77, ",")</f>
-        <v>verteilung_svsaa,</v>
+        <v>verteilung_apm_kerda,</v>
       </c>
       <c r="B77" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B77, ",")</f>
-        <v>verteilung_svsaa,</v>
+        <v>verteilung_apm_kerda,</v>
       </c>
       <c r="C77" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B77, ",")</f>
-        <v>verteilung_svsaa,</v>
+        <v>verteilung_apm_kerda,</v>
       </c>
       <c r="D77" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B77, ",")</f>
-        <v>verteilung_svsaa,</v>
+        <v>verteilung_apm_kerda,</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A78" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B78, ",")</f>
-        <v>verteilung_cheops,</v>
+        <v>verteilung_svsaa,</v>
       </c>
       <c r="B78" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B78, ",")</f>
-        <v>verteilung_cheops,</v>
+        <v>verteilung_svsaa,</v>
       </c>
       <c r="C78" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B78, ",")</f>
-        <v>verteilung_cheops,</v>
+        <v>verteilung_svsaa,</v>
       </c>
       <c r="D78" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B78, ",")</f>
-        <v>verteilung_cheops,</v>
+        <v>verteilung_svsaa,</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A79" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B79, ",")</f>
-        <v>zuteilung_id,</v>
+        <v>verteilung_cheops,</v>
       </c>
       <c r="B79" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B79, ",")</f>
-        <v>zuteilung_id,</v>
+        <v>verteilung_cheops,</v>
       </c>
       <c r="C79" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B79, ",")</f>
-        <v>zuteilung_id,</v>
+        <v>verteilung_cheops,</v>
       </c>
       <c r="D79" t="str">
         <f>_xlfn.CONCAT(Sheet1!$B79, ",")</f>
-        <v>zuteilung_id,</v>
+        <v>verteilung_cheops,</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A80" t="str">
-        <f>Sheet1!$B80</f>
+        <f>_xlfn.CONCAT(Sheet1!$B80, ",")</f>
+        <v>zuteilung_id,</v>
+      </c>
+      <c r="B80" t="str">
+        <f>_xlfn.CONCAT(Sheet1!$B80, ",")</f>
+        <v>zuteilung_id,</v>
+      </c>
+      <c r="C80" t="str">
+        <f>_xlfn.CONCAT(Sheet1!$B80, ",")</f>
+        <v>zuteilung_id,</v>
+      </c>
+      <c r="D80" t="str">
+        <f>_xlfn.CONCAT(Sheet1!$B80, ",")</f>
+        <v>zuteilung_id,</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A81" t="str">
+        <f>Sheet1!$B81</f>
         <v>auspraegung_id</v>
       </c>
-      <c r="B80" t="str">
-        <f>Sheet1!$B80</f>
+      <c r="B81" t="str">
+        <f>Sheet1!$B81</f>
         <v>auspraegung_id</v>
       </c>
-      <c r="C80" t="str">
-        <f>Sheet1!$B80</f>
+      <c r="C81" t="str">
+        <f>Sheet1!$B81</f>
         <v>auspraegung_id</v>
       </c>
-      <c r="D80" t="str">
-        <f>Sheet1!$B80</f>
+      <c r="D81" t="str">
+        <f>Sheet1!$B81</f>
         <v>auspraegung_id</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A81" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
         <v>267</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>267</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>267</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D82" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A82" t="str">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A83" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H2), Sheet1!H2, IF(OR(Sheet1!H2="Null", Sheet1!H2=""), "Null", _xlfn.CONCAT("'", Sheet1!H2, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="B82" t="str">
+      <c r="B83" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I2), Sheet1!I2, IF(OR(Sheet1!I2="Null", Sheet1!I2=""), "Null", _xlfn.CONCAT("'", Sheet1!I2, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="C82" t="str">
+      <c r="C83" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J2), Sheet1!J2, IF(OR(Sheet1!J2="Null", Sheet1!J2=""), "Null", _xlfn.CONCAT("'", Sheet1!J2, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="D82" t="str">
+      <c r="D83" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K2), Sheet1!K2, IF(OR(Sheet1!K2="Null", Sheet1!K2=""), "Null", _xlfn.CONCAT("'", Sheet1!K2, "'"))), ",")</f>
         <v>'t',</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A83" t="str">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A84" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H3), Sheet1!H3, IF(OR(Sheet1!H3="Null", Sheet1!H3=""), "Null", _xlfn.CONCAT("'", Sheet1!H3, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="B83" t="str">
+      <c r="B84" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I3), Sheet1!I3, IF(OR(Sheet1!I3="Null", Sheet1!I3=""), "Null", _xlfn.CONCAT("'", Sheet1!I3, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="C83" t="str">
+      <c r="C84" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J3), Sheet1!J3, IF(OR(Sheet1!J3="Null", Sheet1!J3=""), "Null", _xlfn.CONCAT("'", Sheet1!J3, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="D83" t="str">
+      <c r="D84" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K3), Sheet1!K3, IF(OR(Sheet1!K3="Null", Sheet1!K3=""), "Null", _xlfn.CONCAT("'", Sheet1!K3, "'"))), ",")</f>
         <v>4,</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A84" t="str">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A85" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H4), Sheet1!H4, IF(OR(Sheet1!H4="Null", Sheet1!H4=""), "Null", _xlfn.CONCAT("'", Sheet1!H4, "'"))), ",")</f>
         <v>'Kurztext DE XYZ',</v>
       </c>
-      <c r="B84" t="str">
+      <c r="B85" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I4), Sheet1!I4, IF(OR(Sheet1!I4="Null", Sheet1!I4=""), "Null", _xlfn.CONCAT("'", Sheet1!I4, "'"))), ",")</f>
         <v>'Kurztext DE 2',</v>
       </c>
-      <c r="C84" t="str">
+      <c r="C85" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J4), Sheet1!J4, IF(OR(Sheet1!J4="Null", Sheet1!J4=""), "Null", _xlfn.CONCAT("'", Sheet1!J4, "'"))), ",")</f>
         <v>'Kurztext DE 3',</v>
       </c>
-      <c r="D84" t="str">
+      <c r="D85" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K4), Sheet1!K4, IF(OR(Sheet1!K4="Null", Sheet1!K4=""), "Null", _xlfn.CONCAT("'", Sheet1!K4, "'"))), ",")</f>
         <v>'asdfasdfasdfasdf',</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A85" t="str">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A86" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H5), Sheet1!H5, IF(OR(Sheet1!H5="Null", Sheet1!H5=""), "Null", _xlfn.CONCAT("'", Sheet1!H5, "'"))), ",")</f>
         <v>'Kurztext FR',</v>
       </c>
-      <c r="B85" t="str">
+      <c r="B86" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I5), Sheet1!I5, IF(OR(Sheet1!I5="Null", Sheet1!I5=""), "Null", _xlfn.CONCAT("'", Sheet1!I5, "'"))), ",")</f>
         <v>'asdfasF',</v>
       </c>
-      <c r="C85" t="str">
+      <c r="C86" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J5), Sheet1!J5, IF(OR(Sheet1!J5="Null", Sheet1!J5=""), "Null", _xlfn.CONCAT("'", Sheet1!J5, "'"))), ",")</f>
         <v>'rrhqhqF',</v>
       </c>
-      <c r="D85" t="str">
+      <c r="D86" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K5), Sheet1!K5, IF(OR(Sheet1!K5="Null", Sheet1!K5=""), "Null", _xlfn.CONCAT("'", Sheet1!K5, "'"))), ",")</f>
         <v>'1tqgqdbq',</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A86" t="str">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A87" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H6), Sheet1!H6, IF(OR(Sheet1!H6="Null", Sheet1!H6=""), "Null", _xlfn.CONCAT("'", Sheet1!H6, "'"))), ",")</f>
         <v>'Kurztext EN',</v>
       </c>
-      <c r="B86" t="str">
+      <c r="B87" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I6), Sheet1!I6, IF(OR(Sheet1!I6="Null", Sheet1!I6=""), "Null", _xlfn.CONCAT("'", Sheet1!I6, "'"))), ",")</f>
         <v>'asdfasE',</v>
       </c>
-      <c r="C86" t="str">
+      <c r="C87" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J6), Sheet1!J6, IF(OR(Sheet1!J6="Null", Sheet1!J6=""), "Null", _xlfn.CONCAT("'", Sheet1!J6, "'"))), ",")</f>
         <v>'rrhqhqE',</v>
       </c>
-      <c r="D86" t="str">
+      <c r="D87" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K6), Sheet1!K6, IF(OR(Sheet1!K6="Null", Sheet1!K6=""), "Null", _xlfn.CONCAT("'", Sheet1!K6, "'"))), ",")</f>
         <v>'asahasr5t',</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A87" t="str">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A88" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H7), Sheet1!H7, IF(OR(Sheet1!H7="Null", Sheet1!H7=""), "Null", _xlfn.CONCAT("'", Sheet1!H7, "'"))), ",")</f>
         <v>'Grunddatentext DE - 1. Zeile',</v>
       </c>
-      <c r="B87" t="str">
+      <c r="B88" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I7), Sheet1!I7, IF(OR(Sheet1!I7="Null", Sheet1!I7=""), "Null", _xlfn.CONCAT("'", Sheet1!I7, "'"))), ",")</f>
         <v>'Grunddatentext DE - 1. Zeile 2',</v>
       </c>
-      <c r="C87" t="str">
+      <c r="C88" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J7), Sheet1!J7, IF(OR(Sheet1!J7="Null", Sheet1!J7=""), "Null", _xlfn.CONCAT("'", Sheet1!J7, "'"))), ",")</f>
         <v>'Grunddatentext DE - 1. Zeile 3',</v>
       </c>
-      <c r="D87" t="str">
+      <c r="D88" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K7), Sheet1!K7, IF(OR(Sheet1!K7="Null", Sheet1!K7=""), "Null", _xlfn.CONCAT("'", Sheet1!K7, "'"))), ",")</f>
         <v>'Grunddatentext DE - 1. Zeile 4',</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A88" t="str">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A89" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H8), Sheet1!H8, IF(OR(Sheet1!H8="Null", Sheet1!H8=""), "Null", _xlfn.CONCAT("'", Sheet1!H8, "'"))), ",")</f>
         <v>'Grunddatentext DE - 2. Zeile',</v>
       </c>
-      <c r="B88" t="str">
+      <c r="B89" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I8), Sheet1!I8, IF(OR(Sheet1!I8="Null", Sheet1!I8=""), "Null", _xlfn.CONCAT("'", Sheet1!I8, "'"))), ",")</f>
         <v>'Grunddatentext DE - 2. Zeile 2',</v>
       </c>
-      <c r="C88" t="str">
+      <c r="C89" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J8), Sheet1!J8, IF(OR(Sheet1!J8="Null", Sheet1!J8=""), "Null", _xlfn.CONCAT("'", Sheet1!J8, "'"))), ",")</f>
         <v>'Grunddatentext DE - 2. Zeile 3',</v>
       </c>
-      <c r="D88" t="str">
+      <c r="D89" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K8), Sheet1!K8, IF(OR(Sheet1!K8="Null", Sheet1!K8=""), "Null", _xlfn.CONCAT("'", Sheet1!K8, "'"))), ",")</f>
         <v>'Grunddatentext DE - 2. Zeile 4',</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A89" t="str">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A90" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H9), Sheet1!H9, IF(OR(Sheet1!H9="Null", Sheet1!H9=""), "Null", _xlfn.CONCAT("'", Sheet1!H9, "'"))), ",")</f>
         <v>'Grunddatentext FR - 1. Zeile',</v>
       </c>
-      <c r="B89" t="str">
+      <c r="B90" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I9), Sheet1!I9, IF(OR(Sheet1!I9="Null", Sheet1!I9=""), "Null", _xlfn.CONCAT("'", Sheet1!I9, "'"))), ",")</f>
         <v>'Grunddatentext FR - 1. Zeile 2',</v>
       </c>
-      <c r="C89" t="str">
+      <c r="C90" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J9), Sheet1!J9, IF(OR(Sheet1!J9="Null", Sheet1!J9=""), "Null", _xlfn.CONCAT("'", Sheet1!J9, "'"))), ",")</f>
         <v>'Grunddatentext FR - 1. Zeile 3',</v>
       </c>
-      <c r="D89" t="str">
+      <c r="D90" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K9), Sheet1!K9, IF(OR(Sheet1!K9="Null", Sheet1!K9=""), "Null", _xlfn.CONCAT("'", Sheet1!K9, "'"))), ",")</f>
         <v>'Grunddatentext FR - 1. Zeile 4',</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A90" t="str">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A91" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H10), Sheet1!H10, IF(OR(Sheet1!H10="Null", Sheet1!H10=""), "Null", _xlfn.CONCAT("'", Sheet1!H10, "'"))), ",")</f>
         <v>'Grunddatentext FR - 2. Zeile',</v>
       </c>
-      <c r="B90" t="str">
+      <c r="B91" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I10), Sheet1!I10, IF(OR(Sheet1!I10="Null", Sheet1!I10=""), "Null", _xlfn.CONCAT("'", Sheet1!I10, "'"))), ",")</f>
         <v>'Grunddatentext FR - 2. Zeile 2',</v>
       </c>
-      <c r="C90" t="str">
+      <c r="C91" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J10), Sheet1!J10, IF(OR(Sheet1!J10="Null", Sheet1!J10=""), "Null", _xlfn.CONCAT("'", Sheet1!J10, "'"))), ",")</f>
         <v>'Grunddatentext FR - 2. Zeile 3',</v>
       </c>
-      <c r="D90" t="str">
+      <c r="D91" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K10), Sheet1!K10, IF(OR(Sheet1!K10="Null", Sheet1!K10=""), "Null", _xlfn.CONCAT("'", Sheet1!K10, "'"))), ",")</f>
         <v>'Grunddatentext FR - 2. Zeile 4',</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A91" t="str">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A92" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H11), Sheet1!H11, IF(OR(Sheet1!H11="Null", Sheet1!H11=""), "Null", _xlfn.CONCAT("'", Sheet1!H11, "'"))), ",")</f>
         <v>'Grunddatentext EN - 1. Zeile',</v>
       </c>
-      <c r="B91" t="str">
+      <c r="B92" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I11), Sheet1!I11, IF(OR(Sheet1!I11="Null", Sheet1!I11=""), "Null", _xlfn.CONCAT("'", Sheet1!I11, "'"))), ",")</f>
         <v>'Grunddatentext EN - 1. Zeile 2',</v>
       </c>
-      <c r="C91" t="str">
+      <c r="C92" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J11), Sheet1!J11, IF(OR(Sheet1!J11="Null", Sheet1!J11=""), "Null", _xlfn.CONCAT("'", Sheet1!J11, "'"))), ",")</f>
         <v>'Grunddatentext EN - 1. Zeile 3',</v>
       </c>
-      <c r="D91" t="str">
+      <c r="D92" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K11), Sheet1!K11, IF(OR(Sheet1!K11="Null", Sheet1!K11=""), "Null", _xlfn.CONCAT("'", Sheet1!K11, "'"))), ",")</f>
         <v>'Grunddatentext EN - 1. Zeile 4',</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A92" t="str">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A93" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H12), Sheet1!H12, IF(OR(Sheet1!H12="Null", Sheet1!H12=""), "Null", _xlfn.CONCAT("'", Sheet1!H12, "'"))), ",")</f>
         <v>'Grunddatentext EN - 2. Zeile',</v>
       </c>
-      <c r="B92" t="str">
+      <c r="B93" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I12), Sheet1!I12, IF(OR(Sheet1!I12="Null", Sheet1!I12=""), "Null", _xlfn.CONCAT("'", Sheet1!I12, "'"))), ",")</f>
         <v>'Grunddatentext EN - 2. Zeile 2',</v>
       </c>
-      <c r="C92" t="str">
+      <c r="C93" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J12), Sheet1!J12, IF(OR(Sheet1!J12="Null", Sheet1!J12=""), "Null", _xlfn.CONCAT("'", Sheet1!J12, "'"))), ",")</f>
         <v>'Grunddatentext EN - 2. Zeile 3',</v>
       </c>
-      <c r="D92" t="str">
+      <c r="D93" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K12), Sheet1!K12, IF(OR(Sheet1!K12="Null", Sheet1!K12=""), "Null", _xlfn.CONCAT("'", Sheet1!K12, "'"))), ",")</f>
         <v>'Grunddatentext EN - 2. Zeile 4',</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A93" t="str">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A94" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H13), Sheet1!H13, IF(OR(Sheet1!H13="Null", Sheet1!H13=""), "Null", _xlfn.CONCAT("'", Sheet1!H13, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="B93" t="str">
+      <c r="B94" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I13), Sheet1!I13, IF(OR(Sheet1!I13="Null", Sheet1!I13=""), "Null", _xlfn.CONCAT("'", Sheet1!I13, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="C93" t="str">
+      <c r="C94" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J13), Sheet1!J13, IF(OR(Sheet1!J13="Null", Sheet1!J13=""), "Null", _xlfn.CONCAT("'", Sheet1!J13, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="D93" t="str">
+      <c r="D94" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K13), Sheet1!K13, IF(OR(Sheet1!K13="Null", Sheet1!K13=""), "Null", _xlfn.CONCAT("'", Sheet1!K13, "'"))), ",")</f>
         <v>4,</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A94" t="str">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A95" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H14), Sheet1!H14, IF(OR(Sheet1!H14="Null", Sheet1!H14=""), "Null", _xlfn.CONCAT("'", Sheet1!H14, "'"))), ",")</f>
         <v>12,</v>
       </c>
-      <c r="B94" t="str">
+      <c r="B95" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I14), Sheet1!I14, IF(OR(Sheet1!I14="Null", Sheet1!I14=""), "Null", _xlfn.CONCAT("'", Sheet1!I14, "'"))), ",")</f>
         <v>22,</v>
       </c>
-      <c r="C94" t="str">
+      <c r="C95" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J14), Sheet1!J14, IF(OR(Sheet1!J14="Null", Sheet1!J14=""), "Null", _xlfn.CONCAT("'", Sheet1!J14, "'"))), ",")</f>
         <v>32,</v>
       </c>
-      <c r="D94" t="str">
+      <c r="D95" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K14), Sheet1!K14, IF(OR(Sheet1!K14="Null", Sheet1!K14=""), "Null", _xlfn.CONCAT("'", Sheet1!K14, "'"))), ",")</f>
         <v>42,</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A95" t="str">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A96" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H15), Sheet1!H15, IF(OR(Sheet1!H15="Null", Sheet1!H15=""), "Null", _xlfn.CONCAT("'", Sheet1!H15, "'"))), ",")</f>
         <v>23,</v>
       </c>
-      <c r="B95" t="str">
+      <c r="B96" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I15), Sheet1!I15, IF(OR(Sheet1!I15="Null", Sheet1!I15=""), "Null", _xlfn.CONCAT("'", Sheet1!I15, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C95" t="str">
+      <c r="C96" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J15), Sheet1!J15, IF(OR(Sheet1!J15="Null", Sheet1!J15=""), "Null", _xlfn.CONCAT("'", Sheet1!J15, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="D95" t="str">
+      <c r="D96" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K15), Sheet1!K15, IF(OR(Sheet1!K15="Null", Sheet1!K15=""), "Null", _xlfn.CONCAT("'", Sheet1!K15, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A96" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H16), Sheet1!H16, IF(OR(Sheet1!H16="Null", Sheet1!H16=""), "Null", _xlfn.CONCAT("'", Sheet1!H16, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B96" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I16), Sheet1!I16, IF(OR(Sheet1!I16="Null", Sheet1!I16=""), "Null", _xlfn.CONCAT("'", Sheet1!I16, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C96" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J16), Sheet1!J16, IF(OR(Sheet1!J16="Null", Sheet1!J16=""), "Null", _xlfn.CONCAT("'", Sheet1!J16, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D96" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K16), Sheet1!K16, IF(OR(Sheet1!K16="Null", Sheet1!K16=""), "Null", _xlfn.CONCAT("'", Sheet1!K16, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A97" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H17), Sheet1!H17, IF(OR(Sheet1!H17="Null", Sheet1!H17=""), "Null", _xlfn.CONCAT("'", Sheet1!H17, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H16), Sheet1!H16, IF(OR(Sheet1!H16="Null", Sheet1!H16=""), "Null", _xlfn.CONCAT("'", Sheet1!H16, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="B97" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I17), Sheet1!I17, IF(OR(Sheet1!I17="Null", Sheet1!I17=""), "Null", _xlfn.CONCAT("'", Sheet1!I17, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I16), Sheet1!I16, IF(OR(Sheet1!I16="Null", Sheet1!I16=""), "Null", _xlfn.CONCAT("'", Sheet1!I16, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="C97" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J17), Sheet1!J17, IF(OR(Sheet1!J17="Null", Sheet1!J17=""), "Null", _xlfn.CONCAT("'", Sheet1!J17, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J16), Sheet1!J16, IF(OR(Sheet1!J16="Null", Sheet1!J16=""), "Null", _xlfn.CONCAT("'", Sheet1!J16, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="D97" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K17), Sheet1!K17, IF(OR(Sheet1!K17="Null", Sheet1!K17=""), "Null", _xlfn.CONCAT("'", Sheet1!K17, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K16), Sheet1!K16, IF(OR(Sheet1!K16="Null", Sheet1!K16=""), "Null", _xlfn.CONCAT("'", Sheet1!K16, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A98" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H18), Sheet1!H18, IF(OR(Sheet1!H18="Null", Sheet1!H18=""), "Null", _xlfn.CONCAT("'", Sheet1!H18, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H17), Sheet1!H17, IF(OR(Sheet1!H17="Null", Sheet1!H17=""), "Null", _xlfn.CONCAT("'", Sheet1!H17, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="B98" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I18), Sheet1!I18, IF(OR(Sheet1!I18="Null", Sheet1!I18=""), "Null", _xlfn.CONCAT("'", Sheet1!I18, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I17), Sheet1!I17, IF(OR(Sheet1!I17="Null", Sheet1!I17=""), "Null", _xlfn.CONCAT("'", Sheet1!I17, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="C98" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J18), Sheet1!J18, IF(OR(Sheet1!J18="Null", Sheet1!J18=""), "Null", _xlfn.CONCAT("'", Sheet1!J18, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J17), Sheet1!J17, IF(OR(Sheet1!J17="Null", Sheet1!J17=""), "Null", _xlfn.CONCAT("'", Sheet1!J17, "'"))), ",")</f>
         <v>Null,</v>
       </c>
       <c r="D98" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K18), Sheet1!K18, IF(OR(Sheet1!K18="Null", Sheet1!K18=""), "Null", _xlfn.CONCAT("'", Sheet1!K18, "'"))), ",")</f>
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K17), Sheet1!K17, IF(OR(Sheet1!K17="Null", Sheet1!K17=""), "Null", _xlfn.CONCAT("'", Sheet1!K17, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A99" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H18), Sheet1!H18, IF(OR(Sheet1!H18="Null", Sheet1!H18=""), "Null", _xlfn.CONCAT("'", Sheet1!H18, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B99" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I18), Sheet1!I18, IF(OR(Sheet1!I18="Null", Sheet1!I18=""), "Null", _xlfn.CONCAT("'", Sheet1!I18, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C99" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J18), Sheet1!J18, IF(OR(Sheet1!J18="Null", Sheet1!J18=""), "Null", _xlfn.CONCAT("'", Sheet1!J18, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D99" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K18), Sheet1!K18, IF(OR(Sheet1!K18="Null", Sheet1!K18=""), "Null", _xlfn.CONCAT("'", Sheet1!K18, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A100" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H19), Sheet1!H19, IF(OR(Sheet1!H19="Null", Sheet1!H19=""), "Null", _xlfn.CONCAT("'", Sheet1!H19, "'"))), ",")</f>
         <v>'yann011111111111111',</v>
       </c>
-      <c r="B99" t="str">
+      <c r="B100" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I19), Sheet1!I19, IF(OR(Sheet1!I19="Null", Sheet1!I19=""), "Null", _xlfn.CONCAT("'", Sheet1!I19, "'"))), ",")</f>
         <v>'yann022222222222222',</v>
       </c>
-      <c r="C99" t="str">
+      <c r="C100" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J19), Sheet1!J19, IF(OR(Sheet1!J19="Null", Sheet1!J19=""), "Null", _xlfn.CONCAT("'", Sheet1!J19, "'"))), ",")</f>
         <v>'yann033333333333333',</v>
       </c>
-      <c r="D99" t="str">
+      <c r="D100" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K19), Sheet1!K19, IF(OR(Sheet1!K19="Null", Sheet1!K19=""), "Null", _xlfn.CONCAT("'", Sheet1!K19, "'"))), ",")</f>
         <v>'yann044444444444444',</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A100" t="str">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A101" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H20), Sheet1!H20, IF(OR(Sheet1!H20="Null", Sheet1!H20=""), "Null", _xlfn.CONCAT("'", Sheet1!H20, "'"))), ",")</f>
         <v>'aa',</v>
       </c>
-      <c r="B100" t="str">
+      <c r="B101" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I20), Sheet1!I20, IF(OR(Sheet1!I20="Null", Sheet1!I20=""), "Null", _xlfn.CONCAT("'", Sheet1!I20, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C100" t="str">
+      <c r="C101" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J20), Sheet1!J20, IF(OR(Sheet1!J20="Null", Sheet1!J20=""), "Null", _xlfn.CONCAT("'", Sheet1!J20, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="D100" t="str">
+      <c r="D101" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K20), Sheet1!K20, IF(OR(Sheet1!K20="Null", Sheet1!K20=""), "Null", _xlfn.CONCAT("'", Sheet1!K20, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A101" t="str">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A102" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H21), Sheet1!H21, IF(OR(Sheet1!H21="Null", Sheet1!H21=""), "Null", _xlfn.CONCAT("'", Sheet1!H21, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="B101" t="str">
+      <c r="B102" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I21), Sheet1!I21, IF(OR(Sheet1!I21="Null", Sheet1!I21=""), "Null", _xlfn.CONCAT("'", Sheet1!I21, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="C101" t="str">
+      <c r="C102" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J21), Sheet1!J21, IF(OR(Sheet1!J21="Null", Sheet1!J21=""), "Null", _xlfn.CONCAT("'", Sheet1!J21, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="D101" t="str">
+      <c r="D102" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K21), Sheet1!K21, IF(OR(Sheet1!K21="Null", Sheet1!K21=""), "Null", _xlfn.CONCAT("'", Sheet1!K21, "'"))), ",")</f>
         <v>2,</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A102" t="str">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A103" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H22), Sheet1!H22, IF(OR(Sheet1!H22="Null", Sheet1!H22=""), "Null", _xlfn.CONCAT("'", Sheet1!H22, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="B102" t="str">
+      <c r="B103" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I22), Sheet1!I22, IF(OR(Sheet1!I22="Null", Sheet1!I22=""), "Null", _xlfn.CONCAT("'", Sheet1!I22, "'"))), ",")</f>
         <v>'f',</v>
       </c>
-      <c r="C102" t="str">
+      <c r="C103" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J22), Sheet1!J22, IF(OR(Sheet1!J22="Null", Sheet1!J22=""), "Null", _xlfn.CONCAT("'", Sheet1!J22, "'"))), ",")</f>
         <v>'f',</v>
       </c>
-      <c r="D102" t="str">
+      <c r="D103" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K22), Sheet1!K22, IF(OR(Sheet1!K22="Null", Sheet1!K22=""), "Null", _xlfn.CONCAT("'", Sheet1!K22, "'"))), ",")</f>
         <v>'f',</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A103" t="str">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A104" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H23), Sheet1!H23, IF(OR(Sheet1!H23="Null", Sheet1!H23=""), "Null", _xlfn.CONCAT("'", Sheet1!H23, "'"))), ",")</f>
         <v>'f',</v>
       </c>
-      <c r="B103" t="str">
+      <c r="B104" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I23), Sheet1!I23, IF(OR(Sheet1!I23="Null", Sheet1!I23=""), "Null", _xlfn.CONCAT("'", Sheet1!I23, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="C103" t="str">
+      <c r="C104" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J23), Sheet1!J23, IF(OR(Sheet1!J23="Null", Sheet1!J23=""), "Null", _xlfn.CONCAT("'", Sheet1!J23, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="D103" t="str">
+      <c r="D104" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K23), Sheet1!K23, IF(OR(Sheet1!K23="Null", Sheet1!K23=""), "Null", _xlfn.CONCAT("'", Sheet1!K23, "'"))), ",")</f>
         <v>'t',</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A104" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H24), Sheet1!H24, IF(OR(Sheet1!H24="Null", Sheet1!H24=""), "Null", _xlfn.CONCAT("'", Sheet1!H24, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B104" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I24), Sheet1!I24, IF(OR(Sheet1!I24="Null", Sheet1!I24=""), "Null", _xlfn.CONCAT("'", Sheet1!I24, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C104" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J24), Sheet1!J24, IF(OR(Sheet1!J24="Null", Sheet1!J24=""), "Null", _xlfn.CONCAT("'", Sheet1!J24, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D104" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K24), Sheet1!K24, IF(OR(Sheet1!K24="Null", Sheet1!K24=""), "Null", _xlfn.CONCAT("'", Sheet1!K24, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-    </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A105" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H24), Sheet1!H24, IF(OR(Sheet1!H24="Null", Sheet1!H24=""), "Null", _xlfn.CONCAT("'", Sheet1!H24, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B105" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I24), Sheet1!I24, IF(OR(Sheet1!I24="Null", Sheet1!I24=""), "Null", _xlfn.CONCAT("'", Sheet1!I24, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C105" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J24), Sheet1!J24, IF(OR(Sheet1!J24="Null", Sheet1!J24=""), "Null", _xlfn.CONCAT("'", Sheet1!J24, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D105" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K24), Sheet1!K24, IF(OR(Sheet1!K24="Null", Sheet1!K24=""), "Null", _xlfn.CONCAT("'", Sheet1!K24, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A106" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H25), Sheet1!H25, IF(OR(Sheet1!H25="Null", Sheet1!H25=""), "Null", _xlfn.CONCAT("'", Sheet1!H25, "'"))), ",")</f>
         <v>11,</v>
       </c>
-      <c r="B105" t="str">
+      <c r="B106" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I25), Sheet1!I25, IF(OR(Sheet1!I25="Null", Sheet1!I25=""), "Null", _xlfn.CONCAT("'", Sheet1!I25, "'"))), ",")</f>
         <v>22,</v>
       </c>
-      <c r="C105" t="str">
+      <c r="C106" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J25), Sheet1!J25, IF(OR(Sheet1!J25="Null", Sheet1!J25=""), "Null", _xlfn.CONCAT("'", Sheet1!J25, "'"))), ",")</f>
         <v>33,</v>
       </c>
-      <c r="D105" t="str">
+      <c r="D106" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K25), Sheet1!K25, IF(OR(Sheet1!K25="Null", Sheet1!K25=""), "Null", _xlfn.CONCAT("'", Sheet1!K25, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A106" t="str">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A107" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H26), Sheet1!H26, IF(OR(Sheet1!H26="Null", Sheet1!H26=""), "Null", _xlfn.CONCAT("'", Sheet1!H26, "'"))), ",")</f>
         <v>111,</v>
       </c>
-      <c r="B106" t="str">
+      <c r="B107" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I26), Sheet1!I26, IF(OR(Sheet1!I26="Null", Sheet1!I26=""), "Null", _xlfn.CONCAT("'", Sheet1!I26, "'"))), ",")</f>
         <v>222,</v>
       </c>
-      <c r="C106" t="str">
+      <c r="C107" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J26), Sheet1!J26, IF(OR(Sheet1!J26="Null", Sheet1!J26=""), "Null", _xlfn.CONCAT("'", Sheet1!J26, "'"))), ",")</f>
         <v>333,</v>
       </c>
-      <c r="D106" t="str">
+      <c r="D107" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K26), Sheet1!K26, IF(OR(Sheet1!K26="Null", Sheet1!K26=""), "Null", _xlfn.CONCAT("'", Sheet1!K26, "'"))), ",")</f>
         <v>444,</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A107" t="str">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A108" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H27), Sheet1!H27, IF(OR(Sheet1!H27="Null", Sheet1!H27=""), "Null", _xlfn.CONCAT("'", Sheet1!H27, "'"))), ",")</f>
         <v>55,</v>
       </c>
-      <c r="B107" t="str">
+      <c r="B108" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I27), Sheet1!I27, IF(OR(Sheet1!I27="Null", Sheet1!I27=""), "Null", _xlfn.CONCAT("'", Sheet1!I27, "'"))), ",")</f>
         <v>66,</v>
       </c>
-      <c r="C107" t="str">
+      <c r="C108" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J27), Sheet1!J27, IF(OR(Sheet1!J27="Null", Sheet1!J27=""), "Null", _xlfn.CONCAT("'", Sheet1!J27, "'"))), ",")</f>
         <v>77,</v>
       </c>
-      <c r="D107" t="str">
+      <c r="D108" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K27), Sheet1!K27, IF(OR(Sheet1!K27="Null", Sheet1!K27=""), "Null", _xlfn.CONCAT("'", Sheet1!K27, "'"))), ",")</f>
         <v>88,</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A108" t="str">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A109" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H28), Sheet1!H28, IF(OR(Sheet1!H28="Null", Sheet1!H28=""), "Null", _xlfn.CONCAT("'", Sheet1!H28, "'"))), ",")</f>
         <v>44,</v>
       </c>
-      <c r="B108" t="str">
+      <c r="B109" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I28), Sheet1!I28, IF(OR(Sheet1!I28="Null", Sheet1!I28=""), "Null", _xlfn.CONCAT("'", Sheet1!I28, "'"))), ",")</f>
         <v>987,</v>
       </c>
-      <c r="C108" t="str">
+      <c r="C109" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J28), Sheet1!J28, IF(OR(Sheet1!J28="Null", Sheet1!J28=""), "Null", _xlfn.CONCAT("'", Sheet1!J28, "'"))), ",")</f>
         <v>12,</v>
       </c>
-      <c r="D108" t="str">
+      <c r="D109" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K28), Sheet1!K28, IF(OR(Sheet1!K28="Null", Sheet1!K28=""), "Null", _xlfn.CONCAT("'", Sheet1!K28, "'"))), ",")</f>
         <v>15,</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A109" t="str">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A110" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H29), Sheet1!H29, IF(OR(Sheet1!H29="Null", Sheet1!H29=""), "Null", _xlfn.CONCAT("'", Sheet1!H29, "'"))), ",")</f>
         <v>33,</v>
       </c>
-      <c r="B109" t="str">
+      <c r="B110" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I29), Sheet1!I29, IF(OR(Sheet1!I29="Null", Sheet1!I29=""), "Null", _xlfn.CONCAT("'", Sheet1!I29, "'"))), ",")</f>
         <v>232,</v>
       </c>
-      <c r="C109" t="str">
+      <c r="C110" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J29), Sheet1!J29, IF(OR(Sheet1!J29="Null", Sheet1!J29=""), "Null", _xlfn.CONCAT("'", Sheet1!J29, "'"))), ",")</f>
         <v>253,</v>
       </c>
-      <c r="D109" t="str">
+      <c r="D110" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K29), Sheet1!K29, IF(OR(Sheet1!K29="Null", Sheet1!K29=""), "Null", _xlfn.CONCAT("'", Sheet1!K29, "'"))), ",")</f>
         <v>75,</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A110" t="str">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A111" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H30), Sheet1!H30, IF(OR(Sheet1!H30="Null", Sheet1!H30=""), "Null", _xlfn.CONCAT("'", Sheet1!H30, "'"))), ",")</f>
         <v>22,</v>
       </c>
-      <c r="B110" t="str">
+      <c r="B111" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I30), Sheet1!I30, IF(OR(Sheet1!I30="Null", Sheet1!I30=""), "Null", _xlfn.CONCAT("'", Sheet1!I30, "'"))), ",")</f>
         <v>253,</v>
       </c>
-      <c r="C110" t="str">
+      <c r="C111" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J30), Sheet1!J30, IF(OR(Sheet1!J30="Null", Sheet1!J30=""), "Null", _xlfn.CONCAT("'", Sheet1!J30, "'"))), ",")</f>
         <v>1000,</v>
       </c>
-      <c r="D110" t="str">
+      <c r="D111" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K30), Sheet1!K30, IF(OR(Sheet1!K30="Null", Sheet1!K30=""), "Null", _xlfn.CONCAT("'", Sheet1!K30, "'"))), ",")</f>
         <v>65,</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A111" t="str">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A112" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H31), Sheet1!H31, IF(OR(Sheet1!H31="Null", Sheet1!H31=""), "Null", _xlfn.CONCAT("'", Sheet1!H31, "'"))), ",")</f>
         <v>50,</v>
       </c>
-      <c r="B111" t="str">
+      <c r="B112" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I31), Sheet1!I31, IF(OR(Sheet1!I31="Null", Sheet1!I31=""), "Null", _xlfn.CONCAT("'", Sheet1!I31, "'"))), ",")</f>
         <v>23,</v>
       </c>
-      <c r="C111" t="str">
+      <c r="C112" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J31), Sheet1!J31, IF(OR(Sheet1!J31="Null", Sheet1!J31=""), "Null", _xlfn.CONCAT("'", Sheet1!J31, "'"))), ",")</f>
         <v>465,</v>
       </c>
-      <c r="D111" t="str">
+      <c r="D112" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K31), Sheet1!K31, IF(OR(Sheet1!K31="Null", Sheet1!K31=""), "Null", _xlfn.CONCAT("'", Sheet1!K31, "'"))), ",")</f>
         <v>50,</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A112" t="str">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A113" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H32), Sheet1!H32, IF(OR(Sheet1!H32="Null", Sheet1!H32=""), "Null", _xlfn.CONCAT("'", Sheet1!H32, "'"))), ",")</f>
         <v>100,</v>
       </c>
-      <c r="B112" t="str">
+      <c r="B113" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I32), Sheet1!I32, IF(OR(Sheet1!I32="Null", Sheet1!I32=""), "Null", _xlfn.CONCAT("'", Sheet1!I32, "'"))), ",")</f>
         <v>55,</v>
       </c>
-      <c r="C112" t="str">
+      <c r="C113" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J32), Sheet1!J32, IF(OR(Sheet1!J32="Null", Sheet1!J32=""), "Null", _xlfn.CONCAT("'", Sheet1!J32, "'"))), ",")</f>
         <v>313,</v>
       </c>
-      <c r="D112" t="str">
+      <c r="D113" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K32), Sheet1!K32, IF(OR(Sheet1!K32="Null", Sheet1!K32=""), "Null", _xlfn.CONCAT("'", Sheet1!K32, "'"))), ",")</f>
         <v>987,</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A113" t="str">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A114" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H33), Sheet1!H33, IF(OR(Sheet1!H33="Null", Sheet1!H33=""), "Null", _xlfn.CONCAT("'", Sheet1!H33, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="B113" t="str">
+      <c r="B114" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I33), Sheet1!I33, IF(OR(Sheet1!I33="Null", Sheet1!I33=""), "Null", _xlfn.CONCAT("'", Sheet1!I33, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C113" t="str">
+      <c r="C114" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J33), Sheet1!J33, IF(OR(Sheet1!J33="Null", Sheet1!J33=""), "Null", _xlfn.CONCAT("'", Sheet1!J33, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="D113" t="str">
+      <c r="D114" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K33), Sheet1!K33, IF(OR(Sheet1!K33="Null", Sheet1!K33=""), "Null", _xlfn.CONCAT("'", Sheet1!K33, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A114" t="str">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A115" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H34), Sheet1!H34, IF(OR(Sheet1!H34="Null", Sheet1!H34=""), "Null", _xlfn.CONCAT("'", Sheet1!H34, "'"))), ",")</f>
         <v>'D9182',</v>
       </c>
-      <c r="B114" t="str">
+      <c r="B115" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I34), Sheet1!I34, IF(OR(Sheet1!I34="Null", Sheet1!I34=""), "Null", _xlfn.CONCAT("'", Sheet1!I34, "'"))), ",")</f>
         <v>'KCX07',</v>
       </c>
-      <c r="C114" t="str">
+      <c r="C115" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J34), Sheet1!J34, IF(OR(Sheet1!J34="Null", Sheet1!J34=""), "Null", _xlfn.CONCAT("'", Sheet1!J34, "'"))), ",")</f>
         <v>'DD901',</v>
       </c>
-      <c r="D114" t="str">
+      <c r="D115" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K34), Sheet1!K34, IF(OR(Sheet1!K34="Null", Sheet1!K34=""), "Null", _xlfn.CONCAT("'", Sheet1!K34, "'"))), ",")</f>
         <v>'1NQ67',</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A115" t="str">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A116" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H35), Sheet1!H35, IF(OR(Sheet1!H35="Null", Sheet1!H35=""), "Null", _xlfn.CONCAT("'", Sheet1!H35, "'"))), ",")</f>
         <v>'MOWAG',</v>
       </c>
-      <c r="B115" t="str">
+      <c r="B116" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I35), Sheet1!I35, IF(OR(Sheet1!I35="Null", Sheet1!I35=""), "Null", _xlfn.CONCAT("'", Sheet1!I35, "'"))), ",")</f>
         <v>'asdfas',</v>
       </c>
-      <c r="C115" t="str">
+      <c r="C116" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J35), Sheet1!J35, IF(OR(Sheet1!J35="Null", Sheet1!J35=""), "Null", _xlfn.CONCAT("'", Sheet1!J35, "'"))), ",")</f>
         <v>'Apple',</v>
       </c>
-      <c r="D115" t="str">
+      <c r="D116" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K35), Sheet1!K35, IF(OR(Sheet1!K35="Null", Sheet1!K35=""), "Null", _xlfn.CONCAT("'", Sheet1!K35, "'"))), ",")</f>
         <v>'Samsung',</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A116" t="str">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A117" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H36), Sheet1!H36, IF(OR(Sheet1!H36="Null", Sheet1!H36=""), "Null", _xlfn.CONCAT("'", Sheet1!H36, "'"))), ",")</f>
         <v>'Bernstrasse 1',</v>
       </c>
-      <c r="B116" t="str">
+      <c r="B117" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I36), Sheet1!I36, IF(OR(Sheet1!I36="Null", Sheet1!I36=""), "Null", _xlfn.CONCAT("'", Sheet1!I36, "'"))), ",")</f>
         <v>'Rte du Lac 12',</v>
       </c>
-      <c r="C116" t="str">
+      <c r="C117" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J36), Sheet1!J36, IF(OR(Sheet1!J36="Null", Sheet1!J36=""), "Null", _xlfn.CONCAT("'", Sheet1!J36, "'"))), ",")</f>
         <v>'One Apple Park Way',</v>
       </c>
-      <c r="D116" t="str">
+      <c r="D117" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K36), Sheet1!K36, IF(OR(Sheet1!K36="Null", Sheet1!K36=""), "Null", _xlfn.CONCAT("'", Sheet1!K36, "'"))), ",")</f>
         <v>'Against Apple Way',</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A117" t="str">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A118" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H37), Sheet1!H37, IF(OR(Sheet1!H37="Null", Sheet1!H37=""), "Null", _xlfn.CONCAT("'", Sheet1!H37, "'"))), ",")</f>
         <v>2000,</v>
       </c>
-      <c r="B117" t="str">
+      <c r="B118" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I37), Sheet1!I37, IF(OR(Sheet1!I37="Null", Sheet1!I37=""), "Null", _xlfn.CONCAT("'", Sheet1!I37, "'"))), ",")</f>
         <v>1215,</v>
       </c>
-      <c r="C117" t="str">
+      <c r="C118" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J37), Sheet1!J37, IF(OR(Sheet1!J37="Null", Sheet1!J37=""), "Null", _xlfn.CONCAT("'", Sheet1!J37, "'"))), ",")</f>
         <v>95014,</v>
       </c>
-      <c r="D117" t="str">
+      <c r="D118" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K37), Sheet1!K37, IF(OR(Sheet1!K37="Null", Sheet1!K37=""), "Null", _xlfn.CONCAT("'", Sheet1!K37, "'"))), ",")</f>
         <v>1,</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A118" t="str">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A119" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H38), Sheet1!H38, IF(OR(Sheet1!H38="Null", Sheet1!H38=""), "Null", _xlfn.CONCAT("'", Sheet1!H38, "'"))), ",")</f>
         <v>'Neuchâtel',</v>
       </c>
-      <c r="B118" t="str">
+      <c r="B119" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I38), Sheet1!I38, IF(OR(Sheet1!I38="Null", Sheet1!I38=""), "Null", _xlfn.CONCAT("'", Sheet1!I38, "'"))), ",")</f>
         <v>'Genère',</v>
       </c>
-      <c r="C118" t="str">
+      <c r="C119" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J38), Sheet1!J38, IF(OR(Sheet1!J38="Null", Sheet1!J38=""), "Null", _xlfn.CONCAT("'", Sheet1!J38, "'"))), ",")</f>
         <v>'Cupertino',</v>
       </c>
-      <c r="D118" t="str">
+      <c r="D119" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K38), Sheet1!K38, IF(OR(Sheet1!K38="Null", Sheet1!K38=""), "Null", _xlfn.CONCAT("'", Sheet1!K38, "'"))), ",")</f>
         <v>'Seoul',</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A119" t="str">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A120" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H39), Sheet1!H39, IF(OR(Sheet1!H39="Null", Sheet1!H39=""), "Null", _xlfn.CONCAT("'", Sheet1!H39, "'"))), ",")</f>
         <v>'1.1',</v>
       </c>
-      <c r="B119" t="str">
+      <c r="B120" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I39), Sheet1!I39, IF(OR(Sheet1!I39="Null", Sheet1!I39=""), "Null", _xlfn.CONCAT("'", Sheet1!I39, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C119" t="str">
+      <c r="C120" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J39), Sheet1!J39, IF(OR(Sheet1!J39="Null", Sheet1!J39=""), "Null", _xlfn.CONCAT("'", Sheet1!J39, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="D119" t="str">
+      <c r="D120" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K39), Sheet1!K39, IF(OR(Sheet1!K39="Null", Sheet1!K39=""), "Null", _xlfn.CONCAT("'", Sheet1!K39, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A120" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H40), Sheet1!H40, IF(OR(Sheet1!H40="Null", Sheet1!H40=""), "Null", _xlfn.CONCAT("'", Sheet1!H40, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B120" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I40), Sheet1!I40, IF(OR(Sheet1!I40="Null", Sheet1!I40=""), "Null", _xlfn.CONCAT("'", Sheet1!I40, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C120" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J40), Sheet1!J40, IF(OR(Sheet1!J40="Null", Sheet1!J40=""), "Null", _xlfn.CONCAT("'", Sheet1!J40, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D120" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K40), Sheet1!K40, IF(OR(Sheet1!K40="Null", Sheet1!K40=""), "Null", _xlfn.CONCAT("'", Sheet1!K40, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A121" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H40), Sheet1!H40, IF(OR(Sheet1!H40="Null", Sheet1!H40=""), "Null", _xlfn.CONCAT("'", Sheet1!H40, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B121" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I40), Sheet1!I40, IF(OR(Sheet1!I40="Null", Sheet1!I40=""), "Null", _xlfn.CONCAT("'", Sheet1!I40, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C121" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J40), Sheet1!J40, IF(OR(Sheet1!J40="Null", Sheet1!J40=""), "Null", _xlfn.CONCAT("'", Sheet1!J40, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D121" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K40), Sheet1!K40, IF(OR(Sheet1!K40="Null", Sheet1!K40=""), "Null", _xlfn.CONCAT("'", Sheet1!K40, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A122" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H41), Sheet1!H41, IF(OR(Sheet1!H41="Null", Sheet1!H41=""), "Null", _xlfn.CONCAT("'", Sheet1!H41, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="B121" t="str">
+      <c r="B122" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I41), Sheet1!I41, IF(OR(Sheet1!I41="Null", Sheet1!I41=""), "Null", _xlfn.CONCAT("'", Sheet1!I41, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="C121" t="str">
+      <c r="C122" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J41), Sheet1!J41, IF(OR(Sheet1!J41="Null", Sheet1!J41=""), "Null", _xlfn.CONCAT("'", Sheet1!J41, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="D121" t="str">
+      <c r="D122" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K41), Sheet1!K41, IF(OR(Sheet1!K41="Null", Sheet1!K41=""), "Null", _xlfn.CONCAT("'", Sheet1!K41, "'"))), ",")</f>
         <v>1,</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A122" t="str">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A123" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H42), Sheet1!H42, IF(OR(Sheet1!H42="Null", Sheet1!H42=""), "Null", _xlfn.CONCAT("'", Sheet1!H42, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="B122" t="str">
+      <c r="B123" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I42), Sheet1!I42, IF(OR(Sheet1!I42="Null", Sheet1!I42=""), "Null", _xlfn.CONCAT("'", Sheet1!I42, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="C122" t="str">
+      <c r="C123" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J42), Sheet1!J42, IF(OR(Sheet1!J42="Null", Sheet1!J42=""), "Null", _xlfn.CONCAT("'", Sheet1!J42, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="D122" t="str">
+      <c r="D123" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K42), Sheet1!K42, IF(OR(Sheet1!K42="Null", Sheet1!K42=""), "Null", _xlfn.CONCAT("'", Sheet1!K42, "'"))), ",")</f>
         <v>3,</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A123" t="str">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A124" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H43), Sheet1!H43, IF(OR(Sheet1!H43="Null", Sheet1!H43=""), "Null", _xlfn.CONCAT("'", Sheet1!H43, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="B123" t="str">
+      <c r="B124" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I43), Sheet1!I43, IF(OR(Sheet1!I43="Null", Sheet1!I43=""), "Null", _xlfn.CONCAT("'", Sheet1!I43, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="C123" t="str">
+      <c r="C124" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J43), Sheet1!J43, IF(OR(Sheet1!J43="Null", Sheet1!J43=""), "Null", _xlfn.CONCAT("'", Sheet1!J43, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="D123" t="str">
+      <c r="D124" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K43), Sheet1!K43, IF(OR(Sheet1!K43="Null", Sheet1!K43=""), "Null", _xlfn.CONCAT("'", Sheet1!K43, "'"))), ",")</f>
         <v>2,</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A124" t="str">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A125" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H44), Sheet1!H44, IF(OR(Sheet1!H44="Null", Sheet1!H44=""), "Null", _xlfn.CONCAT("'", Sheet1!H44, "'"))), ",")</f>
         <v>'0022',</v>
       </c>
-      <c r="B124" t="str">
+      <c r="B125" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I44), Sheet1!I44, IF(OR(Sheet1!I44="Null", Sheet1!I44=""), "Null", _xlfn.CONCAT("'", Sheet1!I44, "'"))), ",")</f>
         <v>'0045',</v>
       </c>
-      <c r="C124" t="str">
+      <c r="C125" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J44), Sheet1!J44, IF(OR(Sheet1!J44="Null", Sheet1!J44=""), "Null", _xlfn.CONCAT("'", Sheet1!J44, "'"))), ",")</f>
         <v>'0001',</v>
       </c>
-      <c r="D124" t="str">
+      <c r="D125" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K44), Sheet1!K44, IF(OR(Sheet1!K44="Null", Sheet1!K44=""), "Null", _xlfn.CONCAT("'", Sheet1!K44, "'"))), ",")</f>
         <v>'0496',</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A125" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H45), Sheet1!H45, IF(OR(Sheet1!H45="Null", Sheet1!H45=""), "Null", _xlfn.CONCAT("'", Sheet1!H45, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B125" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I45), Sheet1!I45, IF(OR(Sheet1!I45="Null", Sheet1!I45=""), "Null", _xlfn.CONCAT("'", Sheet1!I45, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C125" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J45), Sheet1!J45, IF(OR(Sheet1!J45="Null", Sheet1!J45=""), "Null", _xlfn.CONCAT("'", Sheet1!J45, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D125" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K45), Sheet1!K45, IF(OR(Sheet1!K45="Null", Sheet1!K45=""), "Null", _xlfn.CONCAT("'", Sheet1!K45, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-    </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A126" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H45), Sheet1!H45, IF(OR(Sheet1!H45="Null", Sheet1!H45=""), "Null", _xlfn.CONCAT("'", Sheet1!H45, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B126" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I45), Sheet1!I45, IF(OR(Sheet1!I45="Null", Sheet1!I45=""), "Null", _xlfn.CONCAT("'", Sheet1!I45, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C126" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J45), Sheet1!J45, IF(OR(Sheet1!J45="Null", Sheet1!J45=""), "Null", _xlfn.CONCAT("'", Sheet1!J45, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D126" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K45), Sheet1!K45, IF(OR(Sheet1!K45="Null", Sheet1!K45=""), "Null", _xlfn.CONCAT("'", Sheet1!K45, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A127" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H46), Sheet1!H46, IF(OR(Sheet1!H46="Null", Sheet1!H46=""), "Null", _xlfn.CONCAT("'", Sheet1!H46, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="B126" t="str">
+      <c r="B127" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I46), Sheet1!I46, IF(OR(Sheet1!I46="Null", Sheet1!I46=""), "Null", _xlfn.CONCAT("'", Sheet1!I46, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="C126" t="str">
+      <c r="C127" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J46), Sheet1!J46, IF(OR(Sheet1!J46="Null", Sheet1!J46=""), "Null", _xlfn.CONCAT("'", Sheet1!J46, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="D126" t="str">
+      <c r="D127" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K46), Sheet1!K46, IF(OR(Sheet1!K46="Null", Sheet1!K46=""), "Null", _xlfn.CONCAT("'", Sheet1!K46, "'"))), ",")</f>
         <v>1,</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A127" t="str">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A128" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H47), Sheet1!H47, IF(OR(Sheet1!H47="Null", Sheet1!H47=""), "Null", _xlfn.CONCAT("'", Sheet1!H47, "'"))), ",")</f>
         <v>'1000051294',</v>
       </c>
-      <c r="B127" t="str">
+      <c r="B128" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I47), Sheet1!I47, IF(OR(Sheet1!I47="Null", Sheet1!I47=""), "Null", _xlfn.CONCAT("'", Sheet1!I47, "'"))), ",")</f>
         <v>'1000058908',</v>
       </c>
-      <c r="C127" t="str">
+      <c r="C128" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J47), Sheet1!J47, IF(OR(Sheet1!J47="Null", Sheet1!J47=""), "Null", _xlfn.CONCAT("'", Sheet1!J47, "'"))), ",")</f>
         <v>'1000057308',</v>
       </c>
-      <c r="D127" t="str">
+      <c r="D128" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K47), Sheet1!K47, IF(OR(Sheet1!K47="Null", Sheet1!K47=""), "Null", _xlfn.CONCAT("'", Sheet1!K47, "'"))), ",")</f>
         <v>'1000053644',</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A128" t="str">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A129" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H48), Sheet1!H48, IF(OR(Sheet1!H48="Null", Sheet1!H48=""), "Null", _xlfn.CONCAT("'", Sheet1!H48, "'"))), ",")</f>
         <v>'ZX0000040',</v>
       </c>
-      <c r="B128" t="str">
+      <c r="B129" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I48), Sheet1!I48, IF(OR(Sheet1!I48="Null", Sheet1!I48=""), "Null", _xlfn.CONCAT("'", Sheet1!I48, "'"))), ",")</f>
         <v>'ZX0000040',</v>
       </c>
-      <c r="C128" t="str">
+      <c r="C129" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J48), Sheet1!J48, IF(OR(Sheet1!J48="Null", Sheet1!J48=""), "Null", _xlfn.CONCAT("'", Sheet1!J48, "'"))), ",")</f>
         <v>'ZX0000040',</v>
       </c>
-      <c r="D128" t="str">
+      <c r="D129" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K48), Sheet1!K48, IF(OR(Sheet1!K48="Null", Sheet1!K48=""), "Null", _xlfn.CONCAT("'", Sheet1!K48, "'"))), ",")</f>
         <v>'ZX0000040',</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A129" t="str">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A130" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H49), Sheet1!H49, IF(OR(Sheet1!H49="Null", Sheet1!H49=""), "Null", _xlfn.CONCAT("'", Sheet1!H49, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="B129" t="str">
+      <c r="B130" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I49), Sheet1!I49, IF(OR(Sheet1!I49="Null", Sheet1!I49=""), "Null", _xlfn.CONCAT("'", Sheet1!I49, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="C129" t="str">
+      <c r="C130" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J49), Sheet1!J49, IF(OR(Sheet1!J49="Null", Sheet1!J49=""), "Null", _xlfn.CONCAT("'", Sheet1!J49, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="D129" t="str">
+      <c r="D130" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K49), Sheet1!K49, IF(OR(Sheet1!K49="Null", Sheet1!K49=""), "Null", _xlfn.CONCAT("'", Sheet1!K49, "'"))), ",")</f>
         <v>1,</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A130" t="str">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A131" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H50), Sheet1!H50, IF(OR(Sheet1!H50="Null", Sheet1!H50=""), "Null", _xlfn.CONCAT("'", Sheet1!H50, "'"))), ",")</f>
         <v>'abcde',</v>
       </c>
-      <c r="B130" t="str">
+      <c r="B131" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I50), Sheet1!I50, IF(OR(Sheet1!I50="Null", Sheet1!I50=""), "Null", _xlfn.CONCAT("'", Sheet1!I50, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C130" t="str">
+      <c r="C131" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J50), Sheet1!J50, IF(OR(Sheet1!J50="Null", Sheet1!J50=""), "Null", _xlfn.CONCAT("'", Sheet1!J50, "'"))), ",")</f>
         <v>54321,</v>
       </c>
-      <c r="D130" t="str">
+      <c r="D131" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K50), Sheet1!K50, IF(OR(Sheet1!K50="Null", Sheet1!K50=""), "Null", _xlfn.CONCAT("'", Sheet1!K50, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A131" t="str">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A132" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H51), Sheet1!H51, IF(OR(Sheet1!H51="Null", Sheet1!H51=""), "Null", _xlfn.CONCAT("'", Sheet1!H51, "'"))), ",")</f>
         <v>'.1',</v>
       </c>
-      <c r="B131" t="str">
+      <c r="B132" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I51), Sheet1!I51, IF(OR(Sheet1!I51="Null", Sheet1!I51=""), "Null", _xlfn.CONCAT("'", Sheet1!I51, "'"))), ",")</f>
         <v>'0000',</v>
       </c>
-      <c r="C131" t="str">
+      <c r="C132" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J51), Sheet1!J51, IF(OR(Sheet1!J51="Null", Sheet1!J51=""), "Null", _xlfn.CONCAT("'", Sheet1!J51, "'"))), ",")</f>
         <v>1.01,</v>
       </c>
-      <c r="D131" t="str">
+      <c r="D132" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K51), Sheet1!K51, IF(OR(Sheet1!K51="Null", Sheet1!K51=""), "Null", _xlfn.CONCAT("'", Sheet1!K51, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A132" t="str">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A133" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H52), Sheet1!H52, IF(OR(Sheet1!H52="Null", Sheet1!H52=""), "Null", _xlfn.CONCAT("'", Sheet1!H52, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="B132" t="str">
+      <c r="B133" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I52), Sheet1!I52, IF(OR(Sheet1!I52="Null", Sheet1!I52=""), "Null", _xlfn.CONCAT("'", Sheet1!I52, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C132" t="str">
+      <c r="C133" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J52), Sheet1!J52, IF(OR(Sheet1!J52="Null", Sheet1!J52=""), "Null", _xlfn.CONCAT("'", Sheet1!J52, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="D132" t="str">
+      <c r="D133" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K52), Sheet1!K52, IF(OR(Sheet1!K52="Null", Sheet1!K52=""), "Null", _xlfn.CONCAT("'", Sheet1!K52, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A133" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H53), Sheet1!H53, IF(OR(Sheet1!H53="Null", Sheet1!H53=""), "Null", _xlfn.CONCAT("'", Sheet1!H53, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B133" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I53), Sheet1!I53, IF(OR(Sheet1!I53="Null", Sheet1!I53=""), "Null", _xlfn.CONCAT("'", Sheet1!I53, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C133" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J53), Sheet1!J53, IF(OR(Sheet1!J53="Null", Sheet1!J53=""), "Null", _xlfn.CONCAT("'", Sheet1!J53, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D133" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K53), Sheet1!K53, IF(OR(Sheet1!K53="Null", Sheet1!K53=""), "Null", _xlfn.CONCAT("'", Sheet1!K53, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A134" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H53), Sheet1!H53, IF(OR(Sheet1!H53="Null", Sheet1!H53=""), "Null", _xlfn.CONCAT("'", Sheet1!H53, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B134" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I53), Sheet1!I53, IF(OR(Sheet1!I53="Null", Sheet1!I53=""), "Null", _xlfn.CONCAT("'", Sheet1!I53, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C134" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J53), Sheet1!J53, IF(OR(Sheet1!J53="Null", Sheet1!J53=""), "Null", _xlfn.CONCAT("'", Sheet1!J53, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D134" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K53), Sheet1!K53, IF(OR(Sheet1!K53="Null", Sheet1!K53=""), "Null", _xlfn.CONCAT("'", Sheet1!K53, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A135" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H54), Sheet1!H54, IF(OR(Sheet1!H54="Null", Sheet1!H54=""), "Null", _xlfn.CONCAT("'", Sheet1!H54, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="B134" t="str">
+      <c r="B135" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I54), Sheet1!I54, IF(OR(Sheet1!I54="Null", Sheet1!I54=""), "Null", _xlfn.CONCAT("'", Sheet1!I54, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="C134" t="str">
+      <c r="C135" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J54), Sheet1!J54, IF(OR(Sheet1!J54="Null", Sheet1!J54=""), "Null", _xlfn.CONCAT("'", Sheet1!J54, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="D134" t="str">
+      <c r="D135" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K54), Sheet1!K54, IF(OR(Sheet1!K54="Null", Sheet1!K54=""), "Null", _xlfn.CONCAT("'", Sheet1!K54, "'"))), ",")</f>
         <v>'t',</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A135" t="str">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A136" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H55), Sheet1!H55, IF(OR(Sheet1!H55="Null", Sheet1!H55=""), "Null", _xlfn.CONCAT("'", Sheet1!H55, "'"))), ",")</f>
         <v>'f',</v>
       </c>
-      <c r="B135" t="str">
+      <c r="B136" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I55), Sheet1!I55, IF(OR(Sheet1!I55="Null", Sheet1!I55=""), "Null", _xlfn.CONCAT("'", Sheet1!I55, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="C135" t="str">
+      <c r="C136" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J55), Sheet1!J55, IF(OR(Sheet1!J55="Null", Sheet1!J55=""), "Null", _xlfn.CONCAT("'", Sheet1!J55, "'"))), ",")</f>
         <v>'f',</v>
       </c>
-      <c r="D135" t="str">
+      <c r="D136" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K55), Sheet1!K55, IF(OR(Sheet1!K55="Null", Sheet1!K55=""), "Null", _xlfn.CONCAT("'", Sheet1!K55, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A136" t="str">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A137" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H56), Sheet1!H56, IF(OR(Sheet1!H56="Null", Sheet1!H56=""), "Null", _xlfn.CONCAT("'", Sheet1!H56, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="B136" t="str">
+      <c r="B137" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I56), Sheet1!I56, IF(OR(Sheet1!I56="Null", Sheet1!I56=""), "Null", _xlfn.CONCAT("'", Sheet1!I56, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="C136" t="str">
+      <c r="C137" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J56), Sheet1!J56, IF(OR(Sheet1!J56="Null", Sheet1!J56=""), "Null", _xlfn.CONCAT("'", Sheet1!J56, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="D136" t="str">
+      <c r="D137" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K56), Sheet1!K56, IF(OR(Sheet1!K56="Null", Sheet1!K56=""), "Null", _xlfn.CONCAT("'", Sheet1!K56, "'"))), ",")</f>
         <v>1,</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A137" t="str">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A138" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H57), Sheet1!H57, IF(OR(Sheet1!H57="Null", Sheet1!H57=""), "Null", _xlfn.CONCAT("'", Sheet1!H57, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="B137" t="str">
+      <c r="B138" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I57), Sheet1!I57, IF(OR(Sheet1!I57="Null", Sheet1!I57=""), "Null", _xlfn.CONCAT("'", Sheet1!I57, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="C137" t="str">
+      <c r="C138" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J57), Sheet1!J57, IF(OR(Sheet1!J57="Null", Sheet1!J57=""), "Null", _xlfn.CONCAT("'", Sheet1!J57, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="D137" t="str">
+      <c r="D138" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K57), Sheet1!K57, IF(OR(Sheet1!K57="Null", Sheet1!K57=""), "Null", _xlfn.CONCAT("'", Sheet1!K57, "'"))), ",")</f>
         <v>4,</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A138" t="str">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A139" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H58), Sheet1!H58, IF(OR(Sheet1!H58="Null", Sheet1!H58=""), "Null", _xlfn.CONCAT("'", Sheet1!H58, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="B138" t="str">
+      <c r="B139" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I58), Sheet1!I58, IF(OR(Sheet1!I58="Null", Sheet1!I58=""), "Null", _xlfn.CONCAT("'", Sheet1!I58, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C138" t="str">
+      <c r="C139" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J58), Sheet1!J58, IF(OR(Sheet1!J58="Null", Sheet1!J58=""), "Null", _xlfn.CONCAT("'", Sheet1!J58, "'"))), ",")</f>
         <v>4,</v>
       </c>
-      <c r="D138" t="str">
+      <c r="D139" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K58), Sheet1!K58, IF(OR(Sheet1!K58="Null", Sheet1!K58=""), "Null", _xlfn.CONCAT("'", Sheet1!K58, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A139" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H59), Sheet1!H59, IF(OR(Sheet1!H59="Null", Sheet1!H59=""), "Null", _xlfn.CONCAT("'", Sheet1!H59, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B139" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I59), Sheet1!I59, IF(OR(Sheet1!I59="Null", Sheet1!I59=""), "Null", _xlfn.CONCAT("'", Sheet1!I59, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C139" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J59), Sheet1!J59, IF(OR(Sheet1!J59="Null", Sheet1!J59=""), "Null", _xlfn.CONCAT("'", Sheet1!J59, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D139" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K59), Sheet1!K59, IF(OR(Sheet1!K59="Null", Sheet1!K59=""), "Null", _xlfn.CONCAT("'", Sheet1!K59, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A140" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H59), Sheet1!H59, IF(OR(Sheet1!H59="Null", Sheet1!H59=""), "Null", _xlfn.CONCAT("'", Sheet1!H59, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B140" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I59), Sheet1!I59, IF(OR(Sheet1!I59="Null", Sheet1!I59=""), "Null", _xlfn.CONCAT("'", Sheet1!I59, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C140" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J59), Sheet1!J59, IF(OR(Sheet1!J59="Null", Sheet1!J59=""), "Null", _xlfn.CONCAT("'", Sheet1!J59, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D140" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K59), Sheet1!K59, IF(OR(Sheet1!K59="Null", Sheet1!K59=""), "Null", _xlfn.CONCAT("'", Sheet1!K59, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A141" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H60), Sheet1!H60, IF(OR(Sheet1!H60="Null", Sheet1!H60=""), "Null", _xlfn.CONCAT("'", Sheet1!H60, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="B140" t="str">
+      <c r="B141" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I60), Sheet1!I60, IF(OR(Sheet1!I60="Null", Sheet1!I60=""), "Null", _xlfn.CONCAT("'", Sheet1!I60, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="C140" t="str">
+      <c r="C141" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J60), Sheet1!J60, IF(OR(Sheet1!J60="Null", Sheet1!J60=""), "Null", _xlfn.CONCAT("'", Sheet1!J60, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="D140" t="str">
+      <c r="D141" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K60), Sheet1!K60, IF(OR(Sheet1!K60="Null", Sheet1!K60=""), "Null", _xlfn.CONCAT("'", Sheet1!K60, "'"))), ",")</f>
         <v>3,</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A141" t="str">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A142" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H61), Sheet1!H61, IF(OR(Sheet1!H61="Null", Sheet1!H61=""), "Null", _xlfn.CONCAT("'", Sheet1!H61, "'"))), ",")</f>
         <v>35,</v>
       </c>
-      <c r="B141" t="str">
+      <c r="B142" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I61), Sheet1!I61, IF(OR(Sheet1!I61="Null", Sheet1!I61=""), "Null", _xlfn.CONCAT("'", Sheet1!I61, "'"))), ",")</f>
         <v>35,</v>
       </c>
-      <c r="C141" t="str">
+      <c r="C142" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J61), Sheet1!J61, IF(OR(Sheet1!J61="Null", Sheet1!J61=""), "Null", _xlfn.CONCAT("'", Sheet1!J61, "'"))), ",")</f>
         <v>35,</v>
       </c>
-      <c r="D141" t="str">
+      <c r="D142" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K61), Sheet1!K61, IF(OR(Sheet1!K61="Null", Sheet1!K61=""), "Null", _xlfn.CONCAT("'", Sheet1!K61, "'"))), ",")</f>
         <v>35,</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A142" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H62), Sheet1!H62, IF(OR(Sheet1!H62="Null", Sheet1!H62=""), "Null", _xlfn.CONCAT("'", Sheet1!H62, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="B142" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I62), Sheet1!I62, IF(OR(Sheet1!I62="Null", Sheet1!I62=""), "Null", _xlfn.CONCAT("'", Sheet1!I62, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="C142" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J62), Sheet1!J62, IF(OR(Sheet1!J62="Null", Sheet1!J62=""), "Null", _xlfn.CONCAT("'", Sheet1!J62, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D142" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K62), Sheet1!K62, IF(OR(Sheet1!K62="Null", Sheet1!K62=""), "Null", _xlfn.CONCAT("'", Sheet1!K62, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-    </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A143" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H62), Sheet1!H62, IF(OR(Sheet1!H62="Null", Sheet1!H62=""), "Null", _xlfn.CONCAT("'", Sheet1!H62, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="B143" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I62), Sheet1!I62, IF(OR(Sheet1!I62="Null", Sheet1!I62=""), "Null", _xlfn.CONCAT("'", Sheet1!I62, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C143" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J62), Sheet1!J62, IF(OR(Sheet1!J62="Null", Sheet1!J62=""), "Null", _xlfn.CONCAT("'", Sheet1!J62, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D143" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K62), Sheet1!K62, IF(OR(Sheet1!K62="Null", Sheet1!K62=""), "Null", _xlfn.CONCAT("'", Sheet1!K62, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A144" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H63), Sheet1!H63, IF(OR(Sheet1!H63="Null", Sheet1!H63=""), "Null", _xlfn.CONCAT("'", Sheet1!H63, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="B143" t="str">
+      <c r="B144" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I63), Sheet1!I63, IF(OR(Sheet1!I63="Null", Sheet1!I63=""), "Null", _xlfn.CONCAT("'", Sheet1!I63, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="C143" t="str">
+      <c r="C144" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J63), Sheet1!J63, IF(OR(Sheet1!J63="Null", Sheet1!J63=""), "Null", _xlfn.CONCAT("'", Sheet1!J63, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="D143" t="str">
+      <c r="D144" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K63), Sheet1!K63, IF(OR(Sheet1!K63="Null", Sheet1!K63=""), "Null", _xlfn.CONCAT("'", Sheet1!K63, "'"))), ",")</f>
         <v>1,</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A144" t="str">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A145" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H64), Sheet1!H64, IF(OR(Sheet1!H64="Null", Sheet1!H64=""), "Null", _xlfn.CONCAT("'", Sheet1!H64, "'"))), ",")</f>
         <v>'09211600-7',</v>
       </c>
-      <c r="B144" t="str">
+      <c r="B145" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I64), Sheet1!I64, IF(OR(Sheet1!I64="Null", Sheet1!I64=""), "Null", _xlfn.CONCAT("'", Sheet1!I64, "'"))), ",")</f>
         <v>'09221000-4',</v>
       </c>
-      <c r="C144" t="str">
+      <c r="C145" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J64), Sheet1!J64, IF(OR(Sheet1!J64="Null", Sheet1!J64=""), "Null", _xlfn.CONCAT("'", Sheet1!J64, "'"))), ",")</f>
         <v>'09221400-8',</v>
       </c>
-      <c r="D144" t="str">
+      <c r="D145" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K64), Sheet1!K64, IF(OR(Sheet1!K64="Null", Sheet1!K64=""), "Null", _xlfn.CONCAT("'", Sheet1!K64, "'"))), ",")</f>
         <v>'09230000-0',</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A145" t="str">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A146" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H65), Sheet1!H65, IF(OR(Sheet1!H65="Null", Sheet1!H65=""), "Null", _xlfn.CONCAT("'", Sheet1!H65, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="B145" t="str">
+      <c r="B146" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I65), Sheet1!I65, IF(OR(Sheet1!I65="Null", Sheet1!I65=""), "Null", _xlfn.CONCAT("'", Sheet1!I65, "'"))), ",")</f>
         <v>4,</v>
       </c>
-      <c r="C145" t="str">
+      <c r="C146" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J65), Sheet1!J65, IF(OR(Sheet1!J65="Null", Sheet1!J65=""), "Null", _xlfn.CONCAT("'", Sheet1!J65, "'"))), ",")</f>
         <v>4,</v>
       </c>
-      <c r="D145" t="str">
+      <c r="D146" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K65), Sheet1!K65, IF(OR(Sheet1!K65="Null", Sheet1!K65=""), "Null", _xlfn.CONCAT("'", Sheet1!K65, "'"))), ",")</f>
         <v>3,</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A146" t="str">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A147" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H66), Sheet1!H66, IF(OR(Sheet1!H66="Null", Sheet1!H66=""), "Null", _xlfn.CONCAT("'", Sheet1!H66, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="B146" t="str">
+      <c r="B147" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I66), Sheet1!I66, IF(OR(Sheet1!I66="Null", Sheet1!I66=""), "Null", _xlfn.CONCAT("'", Sheet1!I66, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="C146" t="str">
+      <c r="C147" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J66), Sheet1!J66, IF(OR(Sheet1!J66="Null", Sheet1!J66=""), "Null", _xlfn.CONCAT("'", Sheet1!J66, "'"))), ",")</f>
         <v>4,</v>
       </c>
-      <c r="D146" t="str">
+      <c r="D147" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K66), Sheet1!K66, IF(OR(Sheet1!K66="Null", Sheet1!K66=""), "Null", _xlfn.CONCAT("'", Sheet1!K66, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A147" t="str">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A148" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H67), Sheet1!H67, IF(OR(Sheet1!H67="Null", Sheet1!H67=""), "Null", _xlfn.CONCAT("'", Sheet1!H67, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="B147" t="str">
+      <c r="B148" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I67), Sheet1!I67, IF(OR(Sheet1!I67="Null", Sheet1!I67=""), "Null", _xlfn.CONCAT("'", Sheet1!I67, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C147" t="str">
+      <c r="C148" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J67), Sheet1!J67, IF(OR(Sheet1!J67="Null", Sheet1!J67=""), "Null", _xlfn.CONCAT("'", Sheet1!J67, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="D147" t="str">
+      <c r="D148" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K67), Sheet1!K67, IF(OR(Sheet1!K67="Null", Sheet1!K67=""), "Null", _xlfn.CONCAT("'", Sheet1!K67, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A148" t="str">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A149" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H68), Sheet1!H68, IF(OR(Sheet1!H68="Null", Sheet1!H68=""), "Null", _xlfn.CONCAT("'", Sheet1!H68, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="B148" t="str">
+      <c r="B149" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I68), Sheet1!I68, IF(OR(Sheet1!I68="Null", Sheet1!I68=""), "Null", _xlfn.CONCAT("'", Sheet1!I68, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C148" t="str">
+      <c r="C149" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J68), Sheet1!J68, IF(OR(Sheet1!J68="Null", Sheet1!J68=""), "Null", _xlfn.CONCAT("'", Sheet1!J68, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="D148" t="str">
+      <c r="D149" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K68), Sheet1!K68, IF(OR(Sheet1!K68="Null", Sheet1!K68=""), "Null", _xlfn.CONCAT("'", Sheet1!K68, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A149" t="str">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A150" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H69), Sheet1!H69, IF(OR(Sheet1!H69="Null", Sheet1!H69=""), "Null", _xlfn.CONCAT("'", Sheet1!H69, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="B149" t="str">
+      <c r="B150" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I69), Sheet1!I69, IF(OR(Sheet1!I69="Null", Sheet1!I69=""), "Null", _xlfn.CONCAT("'", Sheet1!I69, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C149" t="str">
+      <c r="C150" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J69), Sheet1!J69, IF(OR(Sheet1!J69="Null", Sheet1!J69=""), "Null", _xlfn.CONCAT("'", Sheet1!J69, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="D149" t="str">
+      <c r="D150" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K69), Sheet1!K69, IF(OR(Sheet1!K69="Null", Sheet1!K69=""), "Null", _xlfn.CONCAT("'", Sheet1!K69, "'"))), ",")</f>
         <v>1,</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A150" t="str">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A151" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H70), Sheet1!H70, IF(OR(Sheet1!H70="Null", Sheet1!H70=""), "Null", _xlfn.CONCAT("'", Sheet1!H70, "'"))), ",")</f>
         <v>14,</v>
       </c>
-      <c r="B150" t="str">
+      <c r="B151" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I70), Sheet1!I70, IF(OR(Sheet1!I70="Null", Sheet1!I70=""), "Null", _xlfn.CONCAT("'", Sheet1!I70, "'"))), ",")</f>
         <v>14,</v>
       </c>
-      <c r="C150" t="str">
+      <c r="C151" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J70), Sheet1!J70, IF(OR(Sheet1!J70="Null", Sheet1!J70=""), "Null", _xlfn.CONCAT("'", Sheet1!J70, "'"))), ",")</f>
         <v>14,</v>
       </c>
-      <c r="D150" t="str">
+      <c r="D151" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K70), Sheet1!K70, IF(OR(Sheet1!K70="Null", Sheet1!K70=""), "Null", _xlfn.CONCAT("'", Sheet1!K70, "'"))), ",")</f>
         <v>14,</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A151" t="str">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A152" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H71), Sheet1!H71, IF(OR(Sheet1!H71="Null", Sheet1!H71=""), "Null", _xlfn.CONCAT("'", Sheet1!H71, "'"))), ",")</f>
         <v>'SYSTEMM',</v>
       </c>
-      <c r="B151" t="str">
+      <c r="B152" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I71), Sheet1!I71, IF(OR(Sheet1!I71="Null", Sheet1!I71=""), "Null", _xlfn.CONCAT("'", Sheet1!I71, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C151" t="str">
+      <c r="C152" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J71), Sheet1!J71, IF(OR(Sheet1!J71="Null", Sheet1!J71=""), "Null", _xlfn.CONCAT("'", Sheet1!J71, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="D151" t="str">
+      <c r="D152" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K71), Sheet1!K71, IF(OR(Sheet1!K71="Null", Sheet1!K71=""), "Null", _xlfn.CONCAT("'", Sheet1!K71, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A152" t="str">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A153" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H72), Sheet1!H72, IF(OR(Sheet1!H72="Null", Sheet1!H72=""), "Null", _xlfn.CONCAT("'", Sheet1!H72, "'"))), ",")</f>
         <v>'55G',</v>
       </c>
-      <c r="B152" t="str">
+      <c r="B153" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I72), Sheet1!I72, IF(OR(Sheet1!I72="Null", Sheet1!I72=""), "Null", _xlfn.CONCAT("'", Sheet1!I72, "'"))), ",")</f>
         <v>'55G',</v>
       </c>
-      <c r="C152" t="str">
+      <c r="C153" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J72), Sheet1!J72, IF(OR(Sheet1!J72="Null", Sheet1!J72=""), "Null", _xlfn.CONCAT("'", Sheet1!J72, "'"))), ",")</f>
         <v>'55G',</v>
       </c>
-      <c r="D152" t="str">
+      <c r="D153" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K72), Sheet1!K72, IF(OR(Sheet1!K72="Null", Sheet1!K72=""), "Null", _xlfn.CONCAT("'", Sheet1!K72, "'"))), ",")</f>
         <v>'55G',</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A153" t="str">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A154" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H73), Sheet1!H73, IF(OR(Sheet1!H73="Null", Sheet1!H73=""), "Null", _xlfn.CONCAT("'", Sheet1!H73, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="B153" t="str">
+      <c r="B154" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I73), Sheet1!I73, IF(OR(Sheet1!I73="Null", Sheet1!I73=""), "Null", _xlfn.CONCAT("'", Sheet1!I73, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C153" t="str">
+      <c r="C154" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J73), Sheet1!J73, IF(OR(Sheet1!J73="Null", Sheet1!J73=""), "Null", _xlfn.CONCAT("'", Sheet1!J73, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="D153" t="str">
+      <c r="D154" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K73), Sheet1!K73, IF(OR(Sheet1!K73="Null", Sheet1!K73=""), "Null", _xlfn.CONCAT("'", Sheet1!K73, "'"))), ",")</f>
         <v>'f',</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A154" t="str">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A155" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H74), Sheet1!H74, IF(OR(Sheet1!H74="Null", Sheet1!H74=""), "Null", _xlfn.CONCAT("'", Sheet1!H74, "'"))), ",")</f>
         <v>'NEXTHIGHER',</v>
       </c>
-      <c r="B154" t="str">
+      <c r="B155" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I74), Sheet1!I74, IF(OR(Sheet1!I74="Null", Sheet1!I74=""), "Null", _xlfn.CONCAT("'", Sheet1!I74, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C154" t="str">
+      <c r="C155" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J74), Sheet1!J74, IF(OR(Sheet1!J74="Null", Sheet1!J74=""), "Null", _xlfn.CONCAT("'", Sheet1!J74, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="D154" t="str">
+      <c r="D155" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K74), Sheet1!K74, IF(OR(Sheet1!K74="Null", Sheet1!K74=""), "Null", _xlfn.CONCAT("'", Sheet1!K74, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A155" t="str">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A156" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H75), Sheet1!H75, IF(OR(Sheet1!H75="Null", Sheet1!H75=""), "Null", _xlfn.CONCAT("'", Sheet1!H75, "'"))), ",")</f>
         <v>'NESCHUB',</v>
       </c>
-      <c r="B155" t="str">
+      <c r="B156" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I75), Sheet1!I75, IF(OR(Sheet1!I75="Null", Sheet1!I75=""), "Null", _xlfn.CONCAT("'", Sheet1!I75, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C155" t="str">
+      <c r="C156" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J75), Sheet1!J75, IF(OR(Sheet1!J75="Null", Sheet1!J75=""), "Null", _xlfn.CONCAT("'", Sheet1!J75, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="D155" t="str">
+      <c r="D156" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K75), Sheet1!K75, IF(OR(Sheet1!K75="Null", Sheet1!K75=""), "Null", _xlfn.CONCAT("'", Sheet1!K75, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A156" t="str">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A157" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H76), Sheet1!H76, IF(OR(Sheet1!H76="Null", Sheet1!H76=""), "Null", _xlfn.CONCAT("'", Sheet1!H76, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="B156" t="str">
+      <c r="B157" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I76), Sheet1!I76, IF(OR(Sheet1!I76="Null", Sheet1!I76=""), "Null", _xlfn.CONCAT("'", Sheet1!I76, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C156" t="str">
+      <c r="C157" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J76), Sheet1!J76, IF(OR(Sheet1!J76="Null", Sheet1!J76=""), "Null", _xlfn.CONCAT("'", Sheet1!J76, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="D156" t="str">
+      <c r="D157" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K76), Sheet1!K76, IF(OR(Sheet1!K76="Null", Sheet1!K76=""), "Null", _xlfn.CONCAT("'", Sheet1!K76, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A157" t="str">
+        <v>'t',</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A158" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H77), Sheet1!H77, IF(OR(Sheet1!H77="Null", Sheet1!H77=""), "Null", _xlfn.CONCAT("'", Sheet1!H77, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="B157" t="str">
+      <c r="B158" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I77), Sheet1!I77, IF(OR(Sheet1!I77="Null", Sheet1!I77=""), "Null", _xlfn.CONCAT("'", Sheet1!I77, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C157" t="str">
+      <c r="C158" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J77), Sheet1!J77, IF(OR(Sheet1!J77="Null", Sheet1!J77=""), "Null", _xlfn.CONCAT("'", Sheet1!J77, "'"))), ",")</f>
-        <v>Null,</v>
-      </c>
-      <c r="D157" t="str">
+        <v>'t',</v>
+      </c>
+      <c r="D158" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K77), Sheet1!K77, IF(OR(Sheet1!K77="Null", Sheet1!K77=""), "Null", _xlfn.CONCAT("'", Sheet1!K77, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A158" t="str">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A159" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H78), Sheet1!H78, IF(OR(Sheet1!H78="Null", Sheet1!H78=""), "Null", _xlfn.CONCAT("'", Sheet1!H78, "'"))), ",")</f>
         <v>'t',</v>
       </c>
-      <c r="B158" t="str">
+      <c r="B159" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I78), Sheet1!I78, IF(OR(Sheet1!I78="Null", Sheet1!I78=""), "Null", _xlfn.CONCAT("'", Sheet1!I78, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="C158" t="str">
+      <c r="C159" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J78), Sheet1!J78, IF(OR(Sheet1!J78="Null", Sheet1!J78=""), "Null", _xlfn.CONCAT("'", Sheet1!J78, "'"))), ",")</f>
         <v>Null,</v>
       </c>
-      <c r="D158" t="str">
+      <c r="D159" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K78), Sheet1!K78, IF(OR(Sheet1!K78="Null", Sheet1!K78=""), "Null", _xlfn.CONCAT("'", Sheet1!K78, "'"))), ",")</f>
         <v>Null,</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A159" t="str">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A160" t="str">
         <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H79), Sheet1!H79, IF(OR(Sheet1!H79="Null", Sheet1!H79=""), "Null", _xlfn.CONCAT("'", Sheet1!H79, "'"))), ",")</f>
+        <v>'t',</v>
+      </c>
+      <c r="B160" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I79), Sheet1!I79, IF(OR(Sheet1!I79="Null", Sheet1!I79=""), "Null", _xlfn.CONCAT("'", Sheet1!I79, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="C160" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J79), Sheet1!J79, IF(OR(Sheet1!J79="Null", Sheet1!J79=""), "Null", _xlfn.CONCAT("'", Sheet1!J79, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+      <c r="D160" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K79), Sheet1!K79, IF(OR(Sheet1!K79="Null", Sheet1!K79=""), "Null", _xlfn.CONCAT("'", Sheet1!K79, "'"))), ",")</f>
+        <v>Null,</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A161" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!H80), Sheet1!H80, IF(OR(Sheet1!H80="Null", Sheet1!H80=""), "Null", _xlfn.CONCAT("'", Sheet1!H80, "'"))), ",")</f>
         <v>2,</v>
       </c>
-      <c r="B159" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I79), Sheet1!I79, IF(OR(Sheet1!I79="Null", Sheet1!I79=""), "Null", _xlfn.CONCAT("'", Sheet1!I79, "'"))), ",")</f>
+      <c r="B161" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!I80), Sheet1!I80, IF(OR(Sheet1!I80="Null", Sheet1!I80=""), "Null", _xlfn.CONCAT("'", Sheet1!I80, "'"))), ",")</f>
         <v>3,</v>
       </c>
-      <c r="C159" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J79), Sheet1!J79, IF(OR(Sheet1!J79="Null", Sheet1!J79=""), "Null", _xlfn.CONCAT("'", Sheet1!J79, "'"))), ",")</f>
+      <c r="C161" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!J80), Sheet1!J80, IF(OR(Sheet1!J80="Null", Sheet1!J80=""), "Null", _xlfn.CONCAT("'", Sheet1!J80, "'"))), ",")</f>
         <v>1,</v>
       </c>
-      <c r="D159" t="str">
-        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K79), Sheet1!K79, IF(OR(Sheet1!K79="Null", Sheet1!K79=""), "Null", _xlfn.CONCAT("'", Sheet1!K79, "'"))), ",")</f>
+      <c r="D161" t="str">
+        <f>_xlfn.CONCAT(IF(ISNUMBER(Sheet1!K80), Sheet1!K80, IF(OR(Sheet1!K80="Null", Sheet1!K80=""), "Null", _xlfn.CONCAT("'", Sheet1!K80, "'"))), ",")</f>
         <v>4,</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A160">
-        <f>IF(ISNUMBER(Sheet1!H80),Sheet1!H80,IF(OR(Sheet1!H80="Null",Sheet1!H80=""),"Null",_xlfn.CONCAT("'",Sheet1!H80,"'")))</f>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A162">
+        <f>IF(ISNUMBER(Sheet1!H81), Sheet1!H81, IF(OR(Sheet1!H81="Null", Sheet1!H81=""), "Null", _xlfn.CONCAT("'", Sheet1!H81, "'")))</f>
         <v>3</v>
       </c>
-      <c r="B160">
-        <f>IF(ISNUMBER(Sheet1!I80),Sheet1!I80,IF(OR(Sheet1!I80="Null",Sheet1!I80=""),"Null",_xlfn.CONCAT("'",Sheet1!I80,"'")))</f>
+      <c r="B162">
+        <f>IF(ISNUMBER(Sheet1!I81), Sheet1!I81, IF(OR(Sheet1!I81="Null", Sheet1!I81=""), "Null", _xlfn.CONCAT("'", Sheet1!I81, "'")))</f>
         <v>2</v>
       </c>
-      <c r="C160">
-        <f>IF(ISNUMBER(Sheet1!J80),Sheet1!J80,IF(OR(Sheet1!J80="Null",Sheet1!J80=""),"Null",_xlfn.CONCAT("'",Sheet1!J80,"'")))</f>
+      <c r="C162">
+        <f>IF(ISNUMBER(Sheet1!J81), Sheet1!J81, IF(OR(Sheet1!J81="Null", Sheet1!J81=""), "Null", _xlfn.CONCAT("'", Sheet1!J81, "'")))</f>
         <v>4</v>
       </c>
-      <c r="D160">
-        <f>IF(ISNUMBER(Sheet1!K80),Sheet1!K80,IF(OR(Sheet1!K80="Null",Sheet1!K80=""),"Null",_xlfn.CONCAT("'",Sheet1!K80,"'")))</f>
+      <c r="D162">
+        <f>IF(ISNUMBER(Sheet1!K81), Sheet1!K81, IF(OR(Sheet1!K81="Null", Sheet1!K81=""), "Null", _xlfn.CONCAT("'", Sheet1!K81, "'")))</f>
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A161" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A163" t="s">
         <v>273</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B163" t="s">
         <v>273</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C163" t="s">
         <v>273</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D163" t="s">
         <v>273</v>
       </c>
     </row>

</xml_diff>